<commit_message>
#27: Added speaker HW and amplifiers to gantt chart
</commit_message>
<xml_diff>
--- a/docs/Gantt Chart.xlsx
+++ b/docs/Gantt Chart.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06AE785D-D242-40A3-AEB5-9BA2A24FA1D9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE1547AC-1989-4AFF-9B79-822DAF8B08E6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="79">
   <si>
     <t>PROGRESS</t>
   </si>
@@ -194,9 +194,6 @@
     <t>Hardware Prototyping</t>
   </si>
   <si>
-    <t>PDR &amp; Presentation</t>
-  </si>
-  <si>
     <t>Sensor Fusion - Algorithm comparisons, define expected output</t>
   </si>
   <si>
@@ -206,16 +203,10 @@
     <t>Joint Movement Sensors - Stretch material selection, circuit design</t>
   </si>
   <si>
-    <t>Li-ion Battery Charger - Circuit design, LTSpice simulation</t>
-  </si>
-  <si>
     <t>Wireless Communication - Bluetooth device selection</t>
   </si>
   <si>
     <t>Gyroscope, accelerometer, magnetometer selection</t>
-  </si>
-  <si>
-    <t>Data Plotter Script - Python script that receives messages from the device and plots finger/orientation data</t>
   </si>
   <si>
     <t>TASK NUM</t>
@@ -227,52 +218,16 @@
     <t>Order Prototyping Components - Staggering orders so parts can be tested early next week</t>
   </si>
   <si>
-    <t>2.3.1</t>
-  </si>
-  <si>
-    <t>2.3.2</t>
-  </si>
-  <si>
-    <t>2.4.1</t>
-  </si>
-  <si>
-    <t>2.4.2</t>
-  </si>
-  <si>
-    <t>Gyroscope, Accelerometer, Magnetometer</t>
-  </si>
-  <si>
-    <t>2.3.3</t>
-  </si>
-  <si>
     <t>Wireless Communication</t>
   </si>
   <si>
     <t xml:space="preserve">        Build "stretch" sensors and measure min/max resistances</t>
   </si>
   <si>
-    <t xml:space="preserve">        Build voltage divider / mux circuits for each joint sensor</t>
-  </si>
-  <si>
     <t xml:space="preserve">        SW to read data from each joint's sensor</t>
   </si>
   <si>
-    <t xml:space="preserve">        I2C or SPI connections to each IC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        SW to read X,Y,Z data from each sensor</t>
-  </si>
-  <si>
     <t xml:space="preserve">        Hardware connections between C2000 and Bluetooth module</t>
-  </si>
-  <si>
-    <t>3.1.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        Define message protocol</t>
-  </si>
-  <si>
-    <t>3.1.2</t>
   </si>
   <si>
     <t>Polish &amp; Demo</t>
@@ -284,58 +239,13 @@
     <t>Status LCD wiring and software to write characters out</t>
   </si>
   <si>
-    <t>3.3.1</t>
-  </si>
-  <si>
-    <t>Sensor Fusion</t>
-  </si>
-  <si>
-    <t>3.3.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        CPU time measurement to determine if dual core is necessary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        Algorithm implementation (and algorithm comparison if necessary)</t>
-  </si>
-  <si>
-    <t>3.3.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        Dual-core setup + interprocess communication (if necessary)</t>
-  </si>
-  <si>
     <t>Main C code development combining all inputs and outputs</t>
   </si>
   <si>
     <t xml:space="preserve">Li-ion Battery Charge Guage - HW/SW  for Voltage Estimation vs Coloumb Counting experiment </t>
   </si>
   <si>
-    <t>2.5.1</t>
-  </si>
-  <si>
-    <t>2.5.2</t>
-  </si>
-  <si>
-    <t>First PCB assembly</t>
-  </si>
-  <si>
-    <t>Finger Spread Sensors</t>
-  </si>
-  <si>
-    <t>Hand Movement Software - Modify Bluetooth message protocol, add accelerometer plot to Live Data Plotter</t>
-  </si>
-  <si>
-    <t>Virtual Hand Demo (or video game) - Unity 3D / C# scripting development</t>
-  </si>
-  <si>
-    <t>Load Sharing circuit modification to Battery Charger, add charging status to LCD, and GPIOs to detect charging</t>
-  </si>
-  <si>
     <t>Li-ion Battery Charger - Breadboard the battery charger and indicate charging mode on LEDs (CC, CV, OFF)</t>
-  </si>
-  <si>
-    <t>Extra time for improving core requirements or completing stretch goals</t>
   </si>
   <si>
     <t>TBD</t>
@@ -347,31 +257,64 @@
     <t>Writing final report</t>
   </si>
   <si>
-    <t>Second PCB assembly</t>
-  </si>
-  <si>
-    <t>Second PCB Design - Fix hardware issues from PCB 1, reduce PCB size, add stretch goal HW if time permits</t>
-  </si>
-  <si>
     <t xml:space="preserve">        Software to transfer data bytes between C2000 and desktop with low latency</t>
-  </si>
-  <si>
-    <t>2.7.1</t>
   </si>
   <si>
     <t xml:space="preserve">First PCB Design </t>
   </si>
   <si>
-    <t xml:space="preserve">        Schematic creation (SMD components, TMS320 breakout, JTAG headers)</t>
-  </si>
-  <si>
-    <t>2.7.2</t>
-  </si>
-  <si>
     <t xml:space="preserve">        Part placement &amp; order from JLCPCB</t>
   </si>
   <si>
-    <t xml:space="preserve">        Device SW to encode, decode, and transfer data according to the protocol + connect/disconnect to script</t>
+    <t>Presentation</t>
+  </si>
+  <si>
+    <t>First PCB assembly &amp; Debugging</t>
+  </si>
+  <si>
+    <t>Video Game development in Unity</t>
+  </si>
+  <si>
+    <t>Second PCB assembly &amp; Debugging</t>
+  </si>
+  <si>
+    <t>Li-ion Battery Charger - Circuit design</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Build voltage divider / mux circuits for each joint sensor (proto with potentiometers)</t>
+  </si>
+  <si>
+    <t>Gyroscope, Accelerometer, Magnetometer - I2C connections + basic SW to read X, Y, Z.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Schematic creation (Some thru-hole components, TMS320 breakout, JTAG headers)</t>
+  </si>
+  <si>
+    <t>Wireless Communication - Define msg protocol + write SW to encode/decode/transfer data + connect/disconnect</t>
+  </si>
+  <si>
+    <t>Madgwick sensor fusion implementation in C# script</t>
+  </si>
+  <si>
+    <t>Second PCB Design - Fix hardware issues from PCB 1, reduce PCB size, all SMD, add stretch goals if time permits</t>
+  </si>
+  <si>
+    <t>Extra time if tasks took longer than expected. Otherwise, stretch goal SW development goes here.</t>
+  </si>
+  <si>
+    <t>Hand Movement Software - Modify Bluetooth message protocol, add accelerometer data, make simple demo</t>
+  </si>
+  <si>
+    <t>Finger spread detection sensors</t>
+  </si>
+  <si>
+    <t>Speaker hardware</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        4 frequency triangle wave generator - Voltage ladder w/ MOSFETs + 555 w/ RC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Voltage amplifier + AB Amplifier</t>
   </si>
 </sst>
 </file>
@@ -522,7 +465,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -610,6 +553,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -765,7 +714,7 @@
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -937,6 +886,69 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="8" applyBorder="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="13" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="13" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="13" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="2" xfId="12" applyFill="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="14" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="14" borderId="2" xfId="10" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="12" applyFont="1" applyFill="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="12" applyFont="1" applyFill="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="12" applyFont="1" applyFill="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="2" xfId="12" applyFont="1" applyFill="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="2" xfId="12" applyFont="1" applyFill="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="2" xfId="12" applyFont="1" applyFill="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyProtection="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="3" xfId="9">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="166" fontId="0" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -946,73 +958,7 @@
     <xf numFmtId="166" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="3" xfId="9">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="13" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="13" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="13" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="2" xfId="12" applyFill="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="14" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="14" borderId="2" xfId="10" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="12" applyFont="1" applyFill="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="12" applyFont="1" applyFill="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="12" applyFont="1" applyFill="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="12" applyFont="1" applyFill="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="2" xfId="12" applyFont="1" applyFill="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="2" xfId="12" applyFont="1" applyFill="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="2" xfId="12" applyFont="1" applyFill="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="2" xfId="12" applyFont="1" applyFill="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyProtection="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Comma" xfId="4" builtinId="3" customBuiltin="1"/>
@@ -1029,427 +975,7 @@
     <cellStyle name="Title" xfId="5" builtinId="15" customBuiltin="1"/>
     <cellStyle name="zHiddenText" xfId="3" xr:uid="{26E66EE6-E33F-4D77-BAE4-0FB4F5BBF673}"/>
   </cellStyles>
-  <dxfs count="96">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
+  <dxfs count="54">
     <dxf>
       <fill>
         <patternFill>
@@ -1996,15 +1522,15 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="ToDoList" pivot="0" count="9" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="95"/>
-      <tableStyleElement type="headerRow" dxfId="94"/>
-      <tableStyleElement type="totalRow" dxfId="93"/>
-      <tableStyleElement type="firstColumn" dxfId="92"/>
-      <tableStyleElement type="lastColumn" dxfId="91"/>
-      <tableStyleElement type="firstRowStripe" dxfId="90"/>
-      <tableStyleElement type="secondRowStripe" dxfId="89"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="88"/>
-      <tableStyleElement type="secondColumnStripe" dxfId="87"/>
+      <tableStyleElement type="wholeTable" dxfId="53"/>
+      <tableStyleElement type="headerRow" dxfId="52"/>
+      <tableStyleElement type="totalRow" dxfId="51"/>
+      <tableStyleElement type="firstColumn" dxfId="50"/>
+      <tableStyleElement type="lastColumn" dxfId="49"/>
+      <tableStyleElement type="firstRowStripe" dxfId="48"/>
+      <tableStyleElement type="secondRowStripe" dxfId="47"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="46"/>
+      <tableStyleElement type="secondColumnStripe" dxfId="45"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -2419,11 +1945,11 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:DB54"/>
+  <dimension ref="A1:DB48"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="70" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="DD48" sqref="DD48"/>
+      <selection pane="bottomLeft" activeCell="BV13" sqref="BV13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2460,7 +1986,7 @@
         <v>20</v>
       </c>
       <c r="C2" s="50"/>
-      <c r="I2" s="83" t="s">
+      <c r="I2" s="76" t="s">
         <v>13</v>
       </c>
     </row>
@@ -2472,11 +1998,11 @@
         <v>36</v>
       </c>
       <c r="D3" s="60"/>
-      <c r="E3" s="64">
+      <c r="E3" s="81">
         <f ca="1">TODAY()</f>
-        <v>44219</v>
-      </c>
-      <c r="F3" s="64"/>
+        <v>44225</v>
+      </c>
+      <c r="F3" s="81"/>
     </row>
     <row r="4" spans="1:106" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="48" t="s">
@@ -2485,159 +2011,159 @@
       <c r="B4" s="48"/>
       <c r="D4" s="60"/>
       <c r="E4" s="5">
-        <v>1</v>
-      </c>
-      <c r="I4" s="61">
+        <v>0</v>
+      </c>
+      <c r="I4" s="82">
         <f ca="1">I5</f>
         <v>44214</v>
       </c>
-      <c r="J4" s="62"/>
-      <c r="K4" s="62"/>
-      <c r="L4" s="62"/>
-      <c r="M4" s="62"/>
-      <c r="N4" s="62"/>
-      <c r="O4" s="63"/>
-      <c r="P4" s="61">
+      <c r="J4" s="83"/>
+      <c r="K4" s="83"/>
+      <c r="L4" s="83"/>
+      <c r="M4" s="83"/>
+      <c r="N4" s="83"/>
+      <c r="O4" s="84"/>
+      <c r="P4" s="82">
         <f ca="1">P5</f>
         <v>44221</v>
       </c>
-      <c r="Q4" s="62"/>
-      <c r="R4" s="62"/>
-      <c r="S4" s="62"/>
-      <c r="T4" s="62"/>
-      <c r="U4" s="62"/>
-      <c r="V4" s="63"/>
-      <c r="W4" s="61">
+      <c r="Q4" s="83"/>
+      <c r="R4" s="83"/>
+      <c r="S4" s="83"/>
+      <c r="T4" s="83"/>
+      <c r="U4" s="83"/>
+      <c r="V4" s="84"/>
+      <c r="W4" s="82">
         <f ca="1">W5</f>
         <v>44228</v>
       </c>
-      <c r="X4" s="62"/>
-      <c r="Y4" s="62"/>
-      <c r="Z4" s="62"/>
-      <c r="AA4" s="62"/>
-      <c r="AB4" s="62"/>
-      <c r="AC4" s="63"/>
-      <c r="AD4" s="61">
+      <c r="X4" s="83"/>
+      <c r="Y4" s="83"/>
+      <c r="Z4" s="83"/>
+      <c r="AA4" s="83"/>
+      <c r="AB4" s="83"/>
+      <c r="AC4" s="84"/>
+      <c r="AD4" s="82">
         <f ca="1">AD5</f>
         <v>44235</v>
       </c>
-      <c r="AE4" s="62"/>
-      <c r="AF4" s="62"/>
-      <c r="AG4" s="62"/>
-      <c r="AH4" s="62"/>
-      <c r="AI4" s="62"/>
-      <c r="AJ4" s="63"/>
-      <c r="AK4" s="61">
+      <c r="AE4" s="83"/>
+      <c r="AF4" s="83"/>
+      <c r="AG4" s="83"/>
+      <c r="AH4" s="83"/>
+      <c r="AI4" s="83"/>
+      <c r="AJ4" s="84"/>
+      <c r="AK4" s="82">
         <f ca="1">AK5</f>
         <v>44242</v>
       </c>
-      <c r="AL4" s="62"/>
-      <c r="AM4" s="62"/>
-      <c r="AN4" s="62"/>
-      <c r="AO4" s="62"/>
-      <c r="AP4" s="62"/>
-      <c r="AQ4" s="63"/>
-      <c r="AR4" s="61">
+      <c r="AL4" s="83"/>
+      <c r="AM4" s="83"/>
+      <c r="AN4" s="83"/>
+      <c r="AO4" s="83"/>
+      <c r="AP4" s="83"/>
+      <c r="AQ4" s="84"/>
+      <c r="AR4" s="82">
         <f ca="1">AR5</f>
         <v>44249</v>
       </c>
-      <c r="AS4" s="62"/>
-      <c r="AT4" s="62"/>
-      <c r="AU4" s="62"/>
-      <c r="AV4" s="62"/>
-      <c r="AW4" s="62"/>
-      <c r="AX4" s="63"/>
-      <c r="AY4" s="61">
+      <c r="AS4" s="83"/>
+      <c r="AT4" s="83"/>
+      <c r="AU4" s="83"/>
+      <c r="AV4" s="83"/>
+      <c r="AW4" s="83"/>
+      <c r="AX4" s="84"/>
+      <c r="AY4" s="82">
         <f ca="1">AY5</f>
         <v>44256</v>
       </c>
-      <c r="AZ4" s="62"/>
-      <c r="BA4" s="62"/>
-      <c r="BB4" s="62"/>
-      <c r="BC4" s="62"/>
-      <c r="BD4" s="62"/>
-      <c r="BE4" s="63"/>
-      <c r="BF4" s="61">
+      <c r="AZ4" s="83"/>
+      <c r="BA4" s="83"/>
+      <c r="BB4" s="83"/>
+      <c r="BC4" s="83"/>
+      <c r="BD4" s="83"/>
+      <c r="BE4" s="84"/>
+      <c r="BF4" s="82">
         <f ca="1">BF5</f>
         <v>44263</v>
       </c>
-      <c r="BG4" s="62"/>
-      <c r="BH4" s="62"/>
-      <c r="BI4" s="62"/>
-      <c r="BJ4" s="62"/>
-      <c r="BK4" s="62"/>
-      <c r="BL4" s="63"/>
-      <c r="BM4" s="61">
+      <c r="BG4" s="83"/>
+      <c r="BH4" s="83"/>
+      <c r="BI4" s="83"/>
+      <c r="BJ4" s="83"/>
+      <c r="BK4" s="83"/>
+      <c r="BL4" s="84"/>
+      <c r="BM4" s="82">
         <f ca="1">BM5</f>
         <v>44270</v>
       </c>
-      <c r="BN4" s="62"/>
-      <c r="BO4" s="62"/>
-      <c r="BP4" s="62"/>
-      <c r="BQ4" s="62"/>
-      <c r="BR4" s="62"/>
-      <c r="BS4" s="63"/>
-      <c r="BT4" s="61">
+      <c r="BN4" s="83"/>
+      <c r="BO4" s="83"/>
+      <c r="BP4" s="83"/>
+      <c r="BQ4" s="83"/>
+      <c r="BR4" s="83"/>
+      <c r="BS4" s="84"/>
+      <c r="BT4" s="82">
         <f ca="1">BT5</f>
         <v>44277</v>
       </c>
-      <c r="BU4" s="62"/>
-      <c r="BV4" s="62"/>
-      <c r="BW4" s="62"/>
-      <c r="BX4" s="62"/>
-      <c r="BY4" s="62"/>
-      <c r="BZ4" s="63"/>
-      <c r="CA4" s="61">
+      <c r="BU4" s="83"/>
+      <c r="BV4" s="83"/>
+      <c r="BW4" s="83"/>
+      <c r="BX4" s="83"/>
+      <c r="BY4" s="83"/>
+      <c r="BZ4" s="84"/>
+      <c r="CA4" s="82">
         <f ca="1">CA5</f>
         <v>44284</v>
       </c>
-      <c r="CB4" s="62"/>
-      <c r="CC4" s="62"/>
-      <c r="CD4" s="62"/>
-      <c r="CE4" s="62"/>
-      <c r="CF4" s="62"/>
-      <c r="CG4" s="63"/>
-      <c r="CH4" s="61">
+      <c r="CB4" s="83"/>
+      <c r="CC4" s="83"/>
+      <c r="CD4" s="83"/>
+      <c r="CE4" s="83"/>
+      <c r="CF4" s="83"/>
+      <c r="CG4" s="84"/>
+      <c r="CH4" s="82">
         <f ca="1">CH5</f>
         <v>44291</v>
       </c>
-      <c r="CI4" s="62"/>
-      <c r="CJ4" s="62"/>
-      <c r="CK4" s="62"/>
-      <c r="CL4" s="62"/>
-      <c r="CM4" s="62"/>
-      <c r="CN4" s="63"/>
-      <c r="CO4" s="61">
+      <c r="CI4" s="83"/>
+      <c r="CJ4" s="83"/>
+      <c r="CK4" s="83"/>
+      <c r="CL4" s="83"/>
+      <c r="CM4" s="83"/>
+      <c r="CN4" s="84"/>
+      <c r="CO4" s="82">
         <f ca="1">CO5</f>
         <v>44298</v>
       </c>
-      <c r="CP4" s="62"/>
-      <c r="CQ4" s="62"/>
-      <c r="CR4" s="62"/>
-      <c r="CS4" s="62"/>
-      <c r="CT4" s="62"/>
-      <c r="CU4" s="63"/>
-      <c r="CV4" s="61">
+      <c r="CP4" s="83"/>
+      <c r="CQ4" s="83"/>
+      <c r="CR4" s="83"/>
+      <c r="CS4" s="83"/>
+      <c r="CT4" s="83"/>
+      <c r="CU4" s="84"/>
+      <c r="CV4" s="82">
         <f ca="1">CV5</f>
         <v>44305</v>
       </c>
-      <c r="CW4" s="62"/>
-      <c r="CX4" s="62"/>
-      <c r="CY4" s="62"/>
-      <c r="CZ4" s="62"/>
-      <c r="DA4" s="62"/>
-      <c r="DB4" s="63"/>
+      <c r="CW4" s="83"/>
+      <c r="CX4" s="83"/>
+      <c r="CY4" s="83"/>
+      <c r="CZ4" s="83"/>
+      <c r="DA4" s="83"/>
+      <c r="DB4" s="84"/>
     </row>
     <row r="5" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="48" t="s">
         <v>28</v>
       </c>
       <c r="B5" s="48"/>
-      <c r="C5" s="65"/>
-      <c r="D5" s="65"/>
-      <c r="E5" s="65"/>
-      <c r="F5" s="65"/>
-      <c r="G5" s="65"/>
+      <c r="C5" s="85"/>
+      <c r="D5" s="85"/>
+      <c r="E5" s="85"/>
+      <c r="F5" s="85"/>
+      <c r="G5" s="85"/>
       <c r="I5" s="9">
         <f ca="1">Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
         <v>44214</v>
@@ -3035,8 +2561,8 @@
       <c r="A6" s="48" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="75" t="s">
-        <v>46</v>
+      <c r="B6" s="69" t="s">
+        <v>43</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>5</v>
@@ -3570,7 +3096,7 @@
       <c r="F8" s="17"/>
       <c r="G8" s="13"/>
       <c r="H8" s="13" t="str">
-        <f t="shared" ref="H8:H54" si="37">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <f t="shared" ref="H8:H48" si="37">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v/>
       </c>
       <c r="I8" s="34"/>
@@ -3578,14 +3104,14 @@
       <c r="K8" s="34"/>
       <c r="L8" s="34"/>
       <c r="M8" s="34"/>
-      <c r="N8" s="73"/>
-      <c r="O8" s="73"/>
-      <c r="P8" s="73"/>
-      <c r="Q8" s="73"/>
-      <c r="R8" s="73"/>
-      <c r="S8" s="34"/>
-      <c r="T8" s="34"/>
-      <c r="U8" s="34"/>
+      <c r="N8" s="68"/>
+      <c r="O8" s="68"/>
+      <c r="P8" s="68"/>
+      <c r="Q8" s="68"/>
+      <c r="R8" s="68"/>
+      <c r="S8" s="68"/>
+      <c r="T8" s="68"/>
+      <c r="U8" s="68"/>
       <c r="V8" s="34"/>
       <c r="W8" s="34"/>
       <c r="X8" s="34"/>
@@ -3676,27 +3202,25 @@
       <c r="A9" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="77">
+      <c r="B9" s="71">
         <v>1.1000000000000001</v>
       </c>
       <c r="C9" s="56" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="D9" s="18">
-        <v>0.25</v>
+        <v>0.75</v>
       </c>
       <c r="E9" s="52">
-        <f ca="1">Project_Start</f>
         <v>44219</v>
       </c>
       <c r="F9" s="52">
-        <f ca="1">E9+1</f>
-        <v>44220</v>
+        <v>44225</v>
       </c>
       <c r="G9" s="13"/>
       <c r="H9" s="13">
-        <f t="shared" ca="1" si="37"/>
-        <v>2</v>
+        <f t="shared" si="37"/>
+        <v>7</v>
       </c>
       <c r="I9" s="34"/>
       <c r="J9" s="34"/>
@@ -3801,26 +3325,26 @@
       <c r="A10" s="48" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="77">
+      <c r="B10" s="71">
         <v>1.2</v>
       </c>
       <c r="C10" s="56" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D10" s="18">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="E10" s="52">
-        <f ca="1">F9</f>
-        <v>44220</v>
+        <f>F9</f>
+        <v>44225</v>
       </c>
       <c r="F10" s="52">
-        <f ca="1">E10+1</f>
-        <v>44221</v>
+        <f>E10+1</f>
+        <v>44226</v>
       </c>
       <c r="G10" s="13"/>
       <c r="H10" s="13">
-        <f t="shared" ca="1" si="37"/>
+        <f t="shared" si="37"/>
         <v>2</v>
       </c>
       <c r="I10" s="34"/>
@@ -3922,25 +3446,28 @@
       <c r="DA10" s="34"/>
       <c r="DB10" s="34"/>
     </row>
-    <row r="11" spans="1:106" s="2" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="48"/>
-      <c r="B11" s="77">
+    <row r="11" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="47"/>
+      <c r="B11" s="71">
         <v>1.3</v>
       </c>
       <c r="C11" s="56" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D11" s="18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11" s="52">
-        <v>44221</v>
+        <v>44222</v>
       </c>
       <c r="F11" s="52">
-        <v>44221</v>
+        <v>44222</v>
       </c>
       <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
+      <c r="H11" s="13">
+        <f t="shared" si="37"/>
+        <v>1</v>
+      </c>
       <c r="I11" s="34"/>
       <c r="J11" s="34"/>
       <c r="K11" s="34"/>
@@ -3953,11 +3480,11 @@
       <c r="R11" s="34"/>
       <c r="S11" s="34"/>
       <c r="T11" s="34"/>
-      <c r="U11" s="35"/>
-      <c r="V11" s="35"/>
+      <c r="U11" s="34"/>
+      <c r="V11" s="34"/>
       <c r="W11" s="34"/>
       <c r="X11" s="34"/>
-      <c r="Y11" s="34"/>
+      <c r="Y11" s="35"/>
       <c r="Z11" s="34"/>
       <c r="AA11" s="34"/>
       <c r="AB11" s="34"/>
@@ -4040,25 +3567,28 @@
       <c r="DA11" s="34"/>
       <c r="DB11" s="34"/>
     </row>
-    <row r="12" spans="1:106" s="2" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="48"/>
-      <c r="B12" s="77">
+    <row r="12" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="47"/>
+      <c r="B12" s="71">
         <v>1.4</v>
       </c>
       <c r="C12" s="56" t="s">
-        <v>44</v>
+        <v>62</v>
       </c>
       <c r="D12" s="18">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="E12" s="52">
-        <v>44222</v>
+        <v>44223</v>
       </c>
       <c r="F12" s="52">
-        <v>44222</v>
+        <v>44223</v>
       </c>
       <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
+      <c r="H12" s="13">
+        <f t="shared" si="37"/>
+        <v>1</v>
+      </c>
       <c r="I12" s="34"/>
       <c r="J12" s="34"/>
       <c r="K12" s="34"/>
@@ -4071,8 +3601,8 @@
       <c r="R12" s="34"/>
       <c r="S12" s="34"/>
       <c r="T12" s="34"/>
-      <c r="U12" s="35"/>
-      <c r="V12" s="35"/>
+      <c r="U12" s="34"/>
+      <c r="V12" s="34"/>
       <c r="W12" s="34"/>
       <c r="X12" s="34"/>
       <c r="Y12" s="34"/>
@@ -4158,28 +3688,25 @@
       <c r="DA12" s="34"/>
       <c r="DB12" s="34"/>
     </row>
-    <row r="13" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="47"/>
-      <c r="B13" s="77">
+    <row r="13" spans="1:106" s="2" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="48"/>
+      <c r="B13" s="71">
         <v>1.5</v>
       </c>
       <c r="C13" s="56" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D13" s="18">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E13" s="52">
-        <v>44222</v>
+        <v>44224</v>
       </c>
       <c r="F13" s="52">
-        <v>44222</v>
+        <v>44224</v>
       </c>
       <c r="G13" s="13"/>
-      <c r="H13" s="13">
-        <f t="shared" si="37"/>
-        <v>1</v>
-      </c>
+      <c r="H13" s="13"/>
       <c r="I13" s="34"/>
       <c r="J13" s="34"/>
       <c r="K13" s="34"/>
@@ -4192,11 +3719,11 @@
       <c r="R13" s="34"/>
       <c r="S13" s="34"/>
       <c r="T13" s="34"/>
-      <c r="U13" s="34"/>
-      <c r="V13" s="34"/>
+      <c r="U13" s="35"/>
+      <c r="V13" s="35"/>
       <c r="W13" s="34"/>
       <c r="X13" s="34"/>
-      <c r="Y13" s="35"/>
+      <c r="Y13" s="34"/>
       <c r="Z13" s="34"/>
       <c r="AA13" s="34"/>
       <c r="AB13" s="34"/>
@@ -4279,22 +3806,22 @@
       <c r="DA13" s="34"/>
       <c r="DB13" s="34"/>
     </row>
-    <row r="14" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="47"/>
-      <c r="B14" s="77">
+    <row r="14" spans="1:106" s="2" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="48"/>
+      <c r="B14" s="71">
         <v>1.6</v>
       </c>
       <c r="C14" s="56" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="D14" s="18">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E14" s="52">
-        <v>44220</v>
+        <v>44226</v>
       </c>
       <c r="F14" s="52">
-        <v>44222</v>
+        <v>44226</v>
       </c>
       <c r="G14" s="13"/>
       <c r="H14" s="13"/>
@@ -4310,11 +3837,11 @@
       <c r="R14" s="34"/>
       <c r="S14" s="34"/>
       <c r="T14" s="34"/>
-      <c r="U14" s="34"/>
-      <c r="V14" s="34"/>
+      <c r="U14" s="35"/>
+      <c r="V14" s="35"/>
       <c r="W14" s="34"/>
       <c r="X14" s="34"/>
-      <c r="Y14" s="35"/>
+      <c r="Y14" s="34"/>
       <c r="Z14" s="34"/>
       <c r="AA14" s="34"/>
       <c r="AB14" s="34"/>
@@ -4399,26 +3926,23 @@
     </row>
     <row r="15" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="47"/>
-      <c r="B15" s="77">
+      <c r="B15" s="71">
         <v>1.7</v>
       </c>
       <c r="C15" s="56" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="D15" s="18">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E15" s="52">
-        <v>44221</v>
+        <v>44220</v>
       </c>
       <c r="F15" s="52">
-        <v>44223</v>
+        <v>44226</v>
       </c>
       <c r="G15" s="13"/>
-      <c r="H15" s="13">
-        <f t="shared" si="37"/>
-        <v>3</v>
-      </c>
+      <c r="H15" s="13"/>
       <c r="I15" s="34"/>
       <c r="J15" s="34"/>
       <c r="K15" s="34"/>
@@ -4435,7 +3959,7 @@
       <c r="V15" s="34"/>
       <c r="W15" s="34"/>
       <c r="X15" s="34"/>
-      <c r="Y15" s="34"/>
+      <c r="Y15" s="35"/>
       <c r="Z15" s="34"/>
       <c r="AA15" s="34"/>
       <c r="AB15" s="34"/>
@@ -4546,40 +4070,40 @@
       <c r="P16" s="34"/>
       <c r="Q16" s="34"/>
       <c r="R16" s="34"/>
-      <c r="S16" s="84"/>
-      <c r="T16" s="84"/>
-      <c r="U16" s="84"/>
-      <c r="V16" s="84"/>
-      <c r="W16" s="84"/>
-      <c r="X16" s="84"/>
-      <c r="Y16" s="84"/>
-      <c r="Z16" s="84"/>
-      <c r="AA16" s="84"/>
-      <c r="AB16" s="84"/>
-      <c r="AC16" s="84"/>
-      <c r="AD16" s="84"/>
-      <c r="AE16" s="84"/>
-      <c r="AF16" s="84"/>
-      <c r="AG16" s="84"/>
-      <c r="AH16" s="84"/>
-      <c r="AI16" s="84"/>
-      <c r="AJ16" s="84"/>
-      <c r="AK16" s="84"/>
-      <c r="AL16" s="84"/>
-      <c r="AM16" s="84"/>
-      <c r="AN16" s="84"/>
-      <c r="AO16" s="84"/>
-      <c r="AP16" s="84"/>
-      <c r="AQ16" s="84"/>
-      <c r="AR16" s="84"/>
-      <c r="AS16" s="84"/>
-      <c r="AT16" s="84"/>
-      <c r="AU16" s="84"/>
-      <c r="AV16" s="84"/>
-      <c r="AW16" s="84"/>
-      <c r="AX16" s="84"/>
-      <c r="AY16" s="84"/>
-      <c r="AZ16" s="84"/>
+      <c r="S16" s="80"/>
+      <c r="T16" s="80"/>
+      <c r="U16" s="80"/>
+      <c r="V16" s="77"/>
+      <c r="W16" s="77"/>
+      <c r="X16" s="77"/>
+      <c r="Y16" s="77"/>
+      <c r="Z16" s="77"/>
+      <c r="AA16" s="77"/>
+      <c r="AB16" s="77"/>
+      <c r="AC16" s="77"/>
+      <c r="AD16" s="77"/>
+      <c r="AE16" s="77"/>
+      <c r="AF16" s="77"/>
+      <c r="AG16" s="77"/>
+      <c r="AH16" s="77"/>
+      <c r="AI16" s="77"/>
+      <c r="AJ16" s="77"/>
+      <c r="AK16" s="77"/>
+      <c r="AL16" s="77"/>
+      <c r="AM16" s="77"/>
+      <c r="AN16" s="77"/>
+      <c r="AO16" s="77"/>
+      <c r="AP16" s="77"/>
+      <c r="AQ16" s="77"/>
+      <c r="AR16" s="77"/>
+      <c r="AS16" s="77"/>
+      <c r="AT16" s="77"/>
+      <c r="AU16" s="77"/>
+      <c r="AV16" s="77"/>
+      <c r="AW16" s="77"/>
+      <c r="AX16" s="77"/>
+      <c r="AY16" s="77"/>
+      <c r="AZ16" s="77"/>
       <c r="BA16" s="34"/>
       <c r="BB16" s="34"/>
       <c r="BC16" s="34"/>
@@ -4637,26 +4161,25 @@
     </row>
     <row r="17" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="47"/>
-      <c r="B17" s="76">
+      <c r="B17" s="70">
         <v>2.1</v>
       </c>
-      <c r="C17" s="57" t="s">
-        <v>84</v>
+      <c r="C17" s="72" t="s">
+        <v>44</v>
       </c>
       <c r="D17" s="23">
         <v>0</v>
       </c>
       <c r="E17" s="53">
-        <v>44224</v>
+        <f>F15+1</f>
+        <v>44227</v>
       </c>
       <c r="F17" s="53">
-        <v>44228</v>
+        <f>E17+4</f>
+        <v>44231</v>
       </c>
       <c r="G17" s="13"/>
-      <c r="H17" s="13">
-        <f t="shared" si="37"/>
-        <v>5</v>
-      </c>
+      <c r="H17" s="13"/>
       <c r="I17" s="34"/>
       <c r="J17" s="34"/>
       <c r="K17" s="34"/>
@@ -4757,27 +4280,29 @@
       <c r="DB17" s="34"/>
     </row>
     <row r="18" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="48"/>
-      <c r="B18" s="76">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="C18" s="78" t="s">
-        <v>76</v>
+      <c r="A18" s="47"/>
+      <c r="B18" s="57" t="str">
+        <f>_xlfn.CONCAT(B17,".1")</f>
+        <v>2.1.1</v>
+      </c>
+      <c r="C18" s="57" t="s">
+        <v>67</v>
       </c>
       <c r="D18" s="23">
         <v>0</v>
       </c>
       <c r="E18" s="53">
-        <v>44229</v>
+        <f>E17</f>
+        <v>44227</v>
       </c>
       <c r="F18" s="53">
-        <f>E18+2</f>
-        <v>44231</v>
+        <f>E18+0</f>
+        <v>44227</v>
       </c>
       <c r="G18" s="13"/>
       <c r="H18" s="13">
         <f t="shared" si="37"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I18" s="34"/>
       <c r="J18" s="34"/>
@@ -4795,7 +4320,7 @@
       <c r="V18" s="34"/>
       <c r="W18" s="34"/>
       <c r="X18" s="34"/>
-      <c r="Y18" s="34"/>
+      <c r="Y18" s="35"/>
       <c r="Z18" s="34"/>
       <c r="AA18" s="34"/>
       <c r="AB18" s="34"/>
@@ -4880,19 +4405,23 @@
     </row>
     <row r="19" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="47"/>
-      <c r="B19" s="76">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="C19" s="78" t="s">
-        <v>47</v>
-      </c>
-      <c r="D19" s="23"/>
+      <c r="B19" s="57" t="str">
+        <f>_xlfn.CONCAT(B17,".2")</f>
+        <v>2.1.2</v>
+      </c>
+      <c r="C19" s="57" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" s="23">
+        <v>0</v>
+      </c>
       <c r="E19" s="53">
-        <v>44232</v>
+        <f>E18</f>
+        <v>44227</v>
       </c>
       <c r="F19" s="53">
-        <f>E19+7</f>
-        <v>44239</v>
+        <f>E19</f>
+        <v>44227</v>
       </c>
       <c r="G19" s="13"/>
       <c r="H19" s="13"/>
@@ -4908,8 +4437,8 @@
       <c r="R19" s="34"/>
       <c r="S19" s="34"/>
       <c r="T19" s="34"/>
-      <c r="U19" s="35"/>
-      <c r="V19" s="35"/>
+      <c r="U19" s="34"/>
+      <c r="V19" s="34"/>
       <c r="W19" s="34"/>
       <c r="X19" s="34"/>
       <c r="Y19" s="34"/>
@@ -4997,19 +4526,23 @@
     </row>
     <row r="20" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="47"/>
-      <c r="B20" s="57" t="s">
-        <v>49</v>
+      <c r="B20" s="57" t="str">
+        <f>_xlfn.CONCAT(B17,".3")</f>
+        <v>2.1.3</v>
       </c>
       <c r="C20" s="57" t="s">
-        <v>56</v>
-      </c>
-      <c r="D20" s="23"/>
+        <v>47</v>
+      </c>
+      <c r="D20" s="23">
+        <v>0</v>
+      </c>
       <c r="E20" s="53">
-        <v>44232</v>
+        <f>F19+1</f>
+        <v>44228</v>
       </c>
       <c r="F20" s="53">
-        <f>E20+3</f>
-        <v>44235</v>
+        <f>F17</f>
+        <v>44231</v>
       </c>
       <c r="G20" s="13"/>
       <c r="H20" s="13">
@@ -5117,25 +4650,25 @@
     </row>
     <row r="21" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="47"/>
-      <c r="B21" s="57" t="s">
-        <v>50</v>
-      </c>
-      <c r="C21" s="57" t="s">
-        <v>57</v>
-      </c>
-      <c r="D21" s="23"/>
+      <c r="B21" s="70">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="C21" s="72" t="s">
+        <v>46</v>
+      </c>
+      <c r="D21" s="23">
+        <v>0</v>
+      </c>
       <c r="E21" s="53">
+        <f>F17+1</f>
+        <v>44232</v>
+      </c>
+      <c r="F21" s="53">
+        <f>E21+4</f>
         <v>44236</v>
       </c>
-      <c r="F21" s="53">
-        <f>E21+1</f>
-        <v>44237</v>
-      </c>
       <c r="G21" s="13"/>
-      <c r="H21" s="13">
-        <f t="shared" si="37"/>
-        <v>2</v>
-      </c>
+      <c r="H21" s="13"/>
       <c r="I21" s="34"/>
       <c r="J21" s="34"/>
       <c r="K21" s="34"/>
@@ -5152,7 +4685,7 @@
       <c r="V21" s="34"/>
       <c r="W21" s="34"/>
       <c r="X21" s="34"/>
-      <c r="Y21" s="35"/>
+      <c r="Y21" s="34"/>
       <c r="Z21" s="34"/>
       <c r="AA21" s="34"/>
       <c r="AB21" s="34"/>
@@ -5237,19 +4770,23 @@
     </row>
     <row r="22" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="47"/>
-      <c r="B22" s="57" t="s">
-        <v>54</v>
+      <c r="B22" s="57" t="str">
+        <f>_xlfn.CONCAT(B21,".1")</f>
+        <v>2.2.1</v>
       </c>
       <c r="C22" s="57" t="s">
-        <v>58</v>
-      </c>
-      <c r="D22" s="23"/>
+        <v>49</v>
+      </c>
+      <c r="D22" s="23">
+        <v>0</v>
+      </c>
       <c r="E22" s="53">
-        <v>44238</v>
+        <f>E21</f>
+        <v>44232</v>
       </c>
       <c r="F22" s="53">
-        <f>E22+1</f>
-        <v>44239</v>
+        <f>E22</f>
+        <v>44232</v>
       </c>
       <c r="G22" s="13"/>
       <c r="H22" s="13"/>
@@ -5269,7 +4806,7 @@
       <c r="V22" s="34"/>
       <c r="W22" s="34"/>
       <c r="X22" s="34"/>
-      <c r="Y22" s="34"/>
+      <c r="Y22" s="35"/>
       <c r="Z22" s="34"/>
       <c r="AA22" s="34"/>
       <c r="AB22" s="34"/>
@@ -5354,19 +4891,23 @@
     </row>
     <row r="23" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="47"/>
-      <c r="B23" s="76">
-        <v>2.4</v>
-      </c>
-      <c r="C23" s="78" t="s">
-        <v>53</v>
-      </c>
-      <c r="D23" s="23"/>
+      <c r="B23" s="57" t="str">
+        <f>_xlfn.CONCAT(B21,".2")</f>
+        <v>2.2.2</v>
+      </c>
+      <c r="C23" s="57" t="s">
+        <v>59</v>
+      </c>
+      <c r="D23" s="23">
+        <v>0</v>
+      </c>
       <c r="E23" s="53">
-        <v>44240</v>
+        <f>F22+1</f>
+        <v>44233</v>
       </c>
       <c r="F23" s="53">
-        <f>E23+4</f>
-        <v>44244</v>
+        <f>E23+3</f>
+        <v>44236</v>
       </c>
       <c r="G23" s="13"/>
       <c r="H23" s="13"/>
@@ -5386,7 +4927,7 @@
       <c r="V23" s="34"/>
       <c r="W23" s="34"/>
       <c r="X23" s="34"/>
-      <c r="Y23" s="34"/>
+      <c r="Y23" s="35"/>
       <c r="Z23" s="34"/>
       <c r="AA23" s="34"/>
       <c r="AB23" s="34"/>
@@ -5471,19 +5012,22 @@
     </row>
     <row r="24" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="47"/>
-      <c r="B24" s="57" t="s">
-        <v>51</v>
+      <c r="B24" s="70">
+        <v>2.2999999999999998</v>
       </c>
       <c r="C24" s="57" t="s">
-        <v>59</v>
-      </c>
-      <c r="D24" s="23"/>
+        <v>76</v>
+      </c>
+      <c r="D24" s="23">
+        <v>0</v>
+      </c>
       <c r="E24" s="53">
-        <v>44240</v>
+        <f>E21+3</f>
+        <v>44235</v>
       </c>
       <c r="F24" s="53">
-        <f>E24</f>
-        <v>44240</v>
+        <f>E24+7</f>
+        <v>44242</v>
       </c>
       <c r="G24" s="13"/>
       <c r="H24" s="13"/>
@@ -5588,19 +5132,23 @@
     </row>
     <row r="25" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="47"/>
-      <c r="B25" s="57" t="s">
-        <v>52</v>
-      </c>
-      <c r="C25" s="74" t="s">
-        <v>60</v>
-      </c>
-      <c r="D25" s="23"/>
+      <c r="B25" s="57" t="str">
+        <f>_xlfn.CONCAT(B24,".1")</f>
+        <v>2.3.1</v>
+      </c>
+      <c r="C25" s="57" t="s">
+        <v>77</v>
+      </c>
+      <c r="D25" s="23">
+        <v>0</v>
+      </c>
       <c r="E25" s="53">
-        <v>44241</v>
+        <f>E24</f>
+        <v>44235</v>
       </c>
       <c r="F25" s="53">
-        <f>E25+3</f>
-        <v>44244</v>
+        <f>E25+1</f>
+        <v>44236</v>
       </c>
       <c r="G25" s="13"/>
       <c r="H25" s="13"/>
@@ -5705,19 +5253,23 @@
     </row>
     <row r="26" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="47"/>
-      <c r="B26" s="76">
-        <v>2.5</v>
-      </c>
-      <c r="C26" s="78" t="s">
-        <v>55</v>
-      </c>
-      <c r="D26" s="23"/>
+      <c r="B26" s="72" t="str">
+        <f>_xlfn.CONCAT(B24,".2")</f>
+        <v>2.3.2</v>
+      </c>
+      <c r="C26" s="57" t="s">
+        <v>78</v>
+      </c>
+      <c r="D26" s="23">
+        <v>0</v>
+      </c>
       <c r="E26" s="53">
-        <v>44245</v>
+        <f>F25+1</f>
+        <v>44237</v>
       </c>
       <c r="F26" s="53">
-        <f>E26+5</f>
-        <v>44250</v>
+        <f>F24</f>
+        <v>44242</v>
       </c>
       <c r="G26" s="13"/>
       <c r="H26" s="13"/>
@@ -5822,20 +5374,22 @@
     </row>
     <row r="27" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="47"/>
-      <c r="B27" s="57" t="s">
-        <v>77</v>
-      </c>
-      <c r="C27" s="57" t="s">
-        <v>61</v>
-      </c>
-      <c r="D27" s="23"/>
+      <c r="B27" s="70">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="C27" s="72" t="s">
+        <v>68</v>
+      </c>
+      <c r="D27" s="23">
+        <v>0</v>
+      </c>
       <c r="E27" s="53">
-        <f>E26</f>
-        <v>44245</v>
+        <f>F21+1</f>
+        <v>44237</v>
       </c>
       <c r="F27" s="53">
-        <f>E27+0</f>
-        <v>44245</v>
+        <f>E27+5</f>
+        <v>44242</v>
       </c>
       <c r="G27" s="13"/>
       <c r="H27" s="13"/>
@@ -5855,7 +5409,7 @@
       <c r="V27" s="34"/>
       <c r="W27" s="34"/>
       <c r="X27" s="34"/>
-      <c r="Y27" s="34"/>
+      <c r="Y27" s="35"/>
       <c r="Z27" s="34"/>
       <c r="AA27" s="34"/>
       <c r="AB27" s="34"/>
@@ -5940,20 +5494,22 @@
     </row>
     <row r="28" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="47"/>
-      <c r="B28" s="57" t="s">
-        <v>78</v>
+      <c r="B28" s="70">
+        <v>2.4</v>
       </c>
       <c r="C28" s="57" t="s">
-        <v>91</v>
-      </c>
-      <c r="D28" s="23"/>
+        <v>52</v>
+      </c>
+      <c r="D28" s="23">
+        <v>0</v>
+      </c>
       <c r="E28" s="53">
         <f>F27+1</f>
-        <v>44246</v>
+        <v>44243</v>
       </c>
       <c r="F28" s="53">
-        <f>E28+4</f>
-        <v>44250</v>
+        <f>E28</f>
+        <v>44243</v>
       </c>
       <c r="G28" s="13"/>
       <c r="H28" s="13"/>
@@ -6058,22 +5614,28 @@
     </row>
     <row r="29" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="47"/>
-      <c r="B29" s="76">
-        <v>2.6</v>
+      <c r="B29" s="70">
+        <v>2.5</v>
       </c>
       <c r="C29" s="57" t="s">
-        <v>67</v>
-      </c>
-      <c r="D29" s="23"/>
+        <v>55</v>
+      </c>
+      <c r="D29" s="23">
+        <v>0</v>
+      </c>
       <c r="E29" s="53">
-        <v>44251</v>
+        <f>F28+1</f>
+        <v>44244</v>
       </c>
       <c r="F29" s="53">
-        <f>E29</f>
-        <v>44251</v>
+        <f>E29+3</f>
+        <v>44247</v>
       </c>
       <c r="G29" s="13"/>
-      <c r="H29" s="13"/>
+      <c r="H29" s="13">
+        <f t="shared" si="37"/>
+        <v>4</v>
+      </c>
       <c r="I29" s="34"/>
       <c r="J29" s="34"/>
       <c r="K29" s="34"/>
@@ -6086,11 +5648,11 @@
       <c r="R29" s="34"/>
       <c r="S29" s="34"/>
       <c r="T29" s="34"/>
-      <c r="U29" s="34"/>
-      <c r="V29" s="34"/>
+      <c r="U29" s="35"/>
+      <c r="V29" s="35"/>
       <c r="W29" s="34"/>
       <c r="X29" s="34"/>
-      <c r="Y29" s="35"/>
+      <c r="Y29" s="34"/>
       <c r="Z29" s="34"/>
       <c r="AA29" s="34"/>
       <c r="AB29" s="34"/>
@@ -6174,24 +5736,28 @@
       <c r="DB29" s="34"/>
     </row>
     <row r="30" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="47"/>
-      <c r="B30" s="76">
-        <v>2.7</v>
-      </c>
-      <c r="C30" s="78" t="s">
-        <v>93</v>
-      </c>
-      <c r="D30" s="23"/>
+      <c r="A30" s="48"/>
+      <c r="B30" s="70">
+        <v>2.6</v>
+      </c>
+      <c r="C30" s="72" t="s">
+        <v>54</v>
+      </c>
+      <c r="D30" s="23">
+        <v>0</v>
+      </c>
       <c r="E30" s="53">
-        <v>44224</v>
+        <f>F29+1</f>
+        <v>44248</v>
       </c>
       <c r="F30" s="53">
-        <v>44255</v>
+        <f>E30+2</f>
+        <v>44250</v>
       </c>
       <c r="G30" s="13"/>
       <c r="H30" s="13">
         <f t="shared" si="37"/>
-        <v>32</v>
+        <v>3</v>
       </c>
       <c r="I30" s="34"/>
       <c r="J30" s="34"/>
@@ -6294,21 +5860,26 @@
     </row>
     <row r="31" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="47"/>
-      <c r="B31" s="78" t="s">
-        <v>92</v>
-      </c>
-      <c r="C31" s="57" t="s">
-        <v>94</v>
-      </c>
-      <c r="D31" s="23"/>
+      <c r="B31" s="70">
+        <v>2.7</v>
+      </c>
+      <c r="C31" s="72" t="s">
+        <v>60</v>
+      </c>
+      <c r="D31" s="23">
+        <v>0</v>
+      </c>
       <c r="E31" s="53">
-        <v>44224</v>
+        <v>44227</v>
       </c>
       <c r="F31" s="53">
-        <v>44251</v>
+        <v>44255</v>
       </c>
       <c r="G31" s="13"/>
-      <c r="H31" s="13"/>
+      <c r="H31" s="13">
+        <f t="shared" si="37"/>
+        <v>29</v>
+      </c>
       <c r="I31" s="34"/>
       <c r="J31" s="34"/>
       <c r="K31" s="34"/>
@@ -6325,7 +5896,7 @@
       <c r="V31" s="34"/>
       <c r="W31" s="34"/>
       <c r="X31" s="34"/>
-      <c r="Y31" s="35"/>
+      <c r="Y31" s="34"/>
       <c r="Z31" s="34"/>
       <c r="AA31" s="34"/>
       <c r="AB31" s="34"/>
@@ -6410,18 +5981,22 @@
     </row>
     <row r="32" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="47"/>
-      <c r="B32" s="78" t="s">
-        <v>95</v>
-      </c>
-      <c r="C32" s="78" t="s">
-        <v>96</v>
-      </c>
-      <c r="D32" s="23"/>
+      <c r="B32" s="72" t="str">
+        <f>_xlfn.CONCAT(B31,".1")</f>
+        <v>2.7.1</v>
+      </c>
+      <c r="C32" s="57" t="s">
+        <v>69</v>
+      </c>
+      <c r="D32" s="23">
+        <v>0</v>
+      </c>
       <c r="E32" s="53">
+        <v>44227</v>
+      </c>
+      <c r="F32" s="53">
+        <f>F30+2</f>
         <v>44252</v>
-      </c>
-      <c r="F32" s="53">
-        <v>44255</v>
       </c>
       <c r="G32" s="13"/>
       <c r="H32" s="13"/>
@@ -6441,7 +6016,7 @@
       <c r="V32" s="34"/>
       <c r="W32" s="34"/>
       <c r="X32" s="34"/>
-      <c r="Y32" s="34"/>
+      <c r="Y32" s="35"/>
       <c r="Z32" s="34"/>
       <c r="AA32" s="34"/>
       <c r="AB32" s="34"/>
@@ -6525,23 +6100,26 @@
       <c r="DB32" s="34"/>
     </row>
     <row r="33" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="47" t="s">
-        <v>21</v>
-      </c>
-      <c r="B33" s="24">
-        <v>3</v>
-      </c>
-      <c r="C33" s="24" t="s">
-        <v>66</v>
-      </c>
-      <c r="D33" s="25"/>
-      <c r="E33" s="26"/>
-      <c r="F33" s="27"/>
+      <c r="A33" s="47"/>
+      <c r="B33" s="72" t="str">
+        <f>_xlfn.CONCAT(B31,".2")</f>
+        <v>2.7.2</v>
+      </c>
+      <c r="C33" s="72" t="s">
+        <v>61</v>
+      </c>
+      <c r="D33" s="23">
+        <v>0</v>
+      </c>
+      <c r="E33" s="53">
+        <f>F32+1</f>
+        <v>44253</v>
+      </c>
+      <c r="F33" s="53">
+        <v>44255</v>
+      </c>
       <c r="G33" s="13"/>
-      <c r="H33" s="13" t="str">
-        <f t="shared" si="37"/>
-        <v/>
-      </c>
+      <c r="H33" s="13"/>
       <c r="I33" s="34"/>
       <c r="J33" s="34"/>
       <c r="K33" s="34"/>
@@ -6584,37 +6162,37 @@
       <c r="AV33" s="34"/>
       <c r="AW33" s="34"/>
       <c r="AX33" s="34"/>
-      <c r="AY33" s="85"/>
-      <c r="AZ33" s="85"/>
-      <c r="BA33" s="85"/>
-      <c r="BB33" s="85"/>
-      <c r="BC33" s="85"/>
-      <c r="BD33" s="85"/>
-      <c r="BE33" s="85"/>
-      <c r="BF33" s="85"/>
-      <c r="BG33" s="85"/>
-      <c r="BH33" s="85"/>
-      <c r="BI33" s="85"/>
-      <c r="BJ33" s="85"/>
-      <c r="BK33" s="85"/>
-      <c r="BL33" s="85"/>
-      <c r="BM33" s="85"/>
-      <c r="BN33" s="85"/>
-      <c r="BO33" s="85"/>
-      <c r="BP33" s="85"/>
-      <c r="BQ33" s="85"/>
-      <c r="BR33" s="85"/>
-      <c r="BS33" s="85"/>
-      <c r="BT33" s="85"/>
-      <c r="BU33" s="85"/>
-      <c r="BV33" s="85"/>
-      <c r="BW33" s="85"/>
-      <c r="BX33" s="85"/>
-      <c r="BY33" s="85"/>
-      <c r="BZ33" s="85"/>
-      <c r="CA33" s="85"/>
-      <c r="CB33" s="85"/>
-      <c r="CC33" s="85"/>
+      <c r="AY33" s="34"/>
+      <c r="AZ33" s="34"/>
+      <c r="BA33" s="34"/>
+      <c r="BB33" s="34"/>
+      <c r="BC33" s="34"/>
+      <c r="BD33" s="34"/>
+      <c r="BE33" s="34"/>
+      <c r="BF33" s="34"/>
+      <c r="BG33" s="34"/>
+      <c r="BH33" s="34"/>
+      <c r="BI33" s="34"/>
+      <c r="BJ33" s="34"/>
+      <c r="BK33" s="34"/>
+      <c r="BL33" s="34"/>
+      <c r="BM33" s="34"/>
+      <c r="BN33" s="34"/>
+      <c r="BO33" s="34"/>
+      <c r="BP33" s="34"/>
+      <c r="BQ33" s="34"/>
+      <c r="BR33" s="34"/>
+      <c r="BS33" s="34"/>
+      <c r="BT33" s="34"/>
+      <c r="BU33" s="34"/>
+      <c r="BV33" s="34"/>
+      <c r="BW33" s="34"/>
+      <c r="BX33" s="34"/>
+      <c r="BY33" s="34"/>
+      <c r="BZ33" s="34"/>
+      <c r="CA33" s="34"/>
+      <c r="CB33" s="34"/>
+      <c r="CC33" s="34"/>
       <c r="CD33" s="34"/>
       <c r="CE33" s="34"/>
       <c r="CF33" s="34"/>
@@ -6641,23 +6219,24 @@
       <c r="DA33" s="34"/>
       <c r="DB33" s="34"/>
     </row>
-    <row r="34" spans="1:106" s="2" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="48"/>
-      <c r="B34" s="79">
-        <v>3.1</v>
-      </c>
-      <c r="C34" s="58" t="s">
-        <v>55</v>
-      </c>
-      <c r="D34" s="28"/>
-      <c r="E34" s="54">
-        <v>44256</v>
-      </c>
-      <c r="F34" s="54">
-        <v>44263</v>
-      </c>
+    <row r="34" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="B34" s="24">
+        <v>3</v>
+      </c>
+      <c r="C34" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="D34" s="25"/>
+      <c r="E34" s="26"/>
+      <c r="F34" s="27"/>
       <c r="G34" s="13"/>
-      <c r="H34" s="13"/>
+      <c r="H34" s="13" t="str">
+        <f t="shared" si="37"/>
+        <v/>
+      </c>
       <c r="I34" s="34"/>
       <c r="J34" s="34"/>
       <c r="K34" s="34"/>
@@ -6670,8 +6249,8 @@
       <c r="R34" s="34"/>
       <c r="S34" s="34"/>
       <c r="T34" s="34"/>
-      <c r="U34" s="35"/>
-      <c r="V34" s="35"/>
+      <c r="U34" s="34"/>
+      <c r="V34" s="34"/>
       <c r="W34" s="34"/>
       <c r="X34" s="34"/>
       <c r="Y34" s="34"/>
@@ -6700,37 +6279,37 @@
       <c r="AV34" s="34"/>
       <c r="AW34" s="34"/>
       <c r="AX34" s="34"/>
-      <c r="AY34" s="34"/>
-      <c r="AZ34" s="34"/>
-      <c r="BA34" s="34"/>
-      <c r="BB34" s="34"/>
-      <c r="BC34" s="34"/>
-      <c r="BD34" s="34"/>
-      <c r="BE34" s="34"/>
-      <c r="BF34" s="34"/>
-      <c r="BG34" s="34"/>
-      <c r="BH34" s="34"/>
-      <c r="BI34" s="34"/>
-      <c r="BJ34" s="34"/>
-      <c r="BK34" s="34"/>
-      <c r="BL34" s="34"/>
-      <c r="BM34" s="34"/>
-      <c r="BN34" s="34"/>
-      <c r="BO34" s="34"/>
-      <c r="BP34" s="34"/>
-      <c r="BQ34" s="34"/>
-      <c r="BR34" s="34"/>
-      <c r="BS34" s="34"/>
-      <c r="BT34" s="34"/>
-      <c r="BU34" s="34"/>
-      <c r="BV34" s="34"/>
-      <c r="BW34" s="34"/>
-      <c r="BX34" s="34"/>
-      <c r="BY34" s="34"/>
-      <c r="BZ34" s="34"/>
-      <c r="CA34" s="34"/>
-      <c r="CB34" s="34"/>
-      <c r="CC34" s="34"/>
+      <c r="AY34" s="78"/>
+      <c r="AZ34" s="78"/>
+      <c r="BA34" s="78"/>
+      <c r="BB34" s="78"/>
+      <c r="BC34" s="78"/>
+      <c r="BD34" s="78"/>
+      <c r="BE34" s="78"/>
+      <c r="BF34" s="78"/>
+      <c r="BG34" s="78"/>
+      <c r="BH34" s="78"/>
+      <c r="BI34" s="78"/>
+      <c r="BJ34" s="78"/>
+      <c r="BK34" s="78"/>
+      <c r="BL34" s="78"/>
+      <c r="BM34" s="78"/>
+      <c r="BN34" s="78"/>
+      <c r="BO34" s="78"/>
+      <c r="BP34" s="78"/>
+      <c r="BQ34" s="78"/>
+      <c r="BR34" s="78"/>
+      <c r="BS34" s="78"/>
+      <c r="BT34" s="78"/>
+      <c r="BU34" s="78"/>
+      <c r="BV34" s="78"/>
+      <c r="BW34" s="78"/>
+      <c r="BX34" s="78"/>
+      <c r="BY34" s="78"/>
+      <c r="BZ34" s="78"/>
+      <c r="CA34" s="78"/>
+      <c r="CB34" s="78"/>
+      <c r="CC34" s="78"/>
       <c r="CD34" s="34"/>
       <c r="CE34" s="34"/>
       <c r="CF34" s="34"/>
@@ -6759,18 +6338,21 @@
     </row>
     <row r="35" spans="1:106" s="2" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="48"/>
-      <c r="B35" s="58" t="s">
-        <v>62</v>
+      <c r="B35" s="73">
+        <v>3.1</v>
       </c>
       <c r="C35" s="58" t="s">
-        <v>63</v>
-      </c>
-      <c r="D35" s="28"/>
+        <v>70</v>
+      </c>
+      <c r="D35" s="28">
+        <v>0</v>
+      </c>
       <c r="E35" s="54">
         <v>44256</v>
       </c>
       <c r="F35" s="54">
-        <v>44256</v>
+        <f>E35+3</f>
+        <v>44259</v>
       </c>
       <c r="G35" s="13"/>
       <c r="H35" s="13"/>
@@ -6873,20 +6455,24 @@
       <c r="DA35" s="34"/>
       <c r="DB35" s="34"/>
     </row>
-    <row r="36" spans="1:106" s="2" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="48"/>
-      <c r="B36" s="58" t="s">
-        <v>64</v>
+    <row r="36" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="47"/>
+      <c r="B36" s="73">
+        <v>3.2</v>
       </c>
       <c r="C36" s="58" t="s">
-        <v>97</v>
-      </c>
-      <c r="D36" s="28"/>
+        <v>53</v>
+      </c>
+      <c r="D36" s="28">
+        <v>0</v>
+      </c>
       <c r="E36" s="54">
-        <v>44257</v>
+        <f>F35+1</f>
+        <v>44260</v>
       </c>
       <c r="F36" s="54">
-        <v>44263</v>
+        <f>E36+4</f>
+        <v>44264</v>
       </c>
       <c r="G36" s="13"/>
       <c r="H36" s="13"/>
@@ -6902,8 +6488,8 @@
       <c r="R36" s="34"/>
       <c r="S36" s="34"/>
       <c r="T36" s="34"/>
-      <c r="U36" s="35"/>
-      <c r="V36" s="35"/>
+      <c r="U36" s="34"/>
+      <c r="V36" s="34"/>
       <c r="W36" s="34"/>
       <c r="X36" s="34"/>
       <c r="Y36" s="34"/>
@@ -6991,23 +6577,27 @@
     </row>
     <row r="37" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="47"/>
-      <c r="B37" s="79">
-        <v>3.2</v>
+      <c r="B37" s="73">
+        <v>3.3</v>
       </c>
       <c r="C37" s="58" t="s">
-        <v>45</v>
-      </c>
-      <c r="D37" s="28"/>
+        <v>64</v>
+      </c>
+      <c r="D37" s="28">
+        <v>0</v>
+      </c>
       <c r="E37" s="54">
-        <v>44256</v>
+        <f>F36+1</f>
+        <v>44265</v>
       </c>
       <c r="F37" s="54">
-        <v>44263</v>
+        <f>E37+10</f>
+        <v>44275</v>
       </c>
       <c r="G37" s="13"/>
       <c r="H37" s="13">
         <f t="shared" si="37"/>
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="I37" s="34"/>
       <c r="J37" s="34"/>
@@ -7110,26 +6700,27 @@
     </row>
     <row r="38" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="47"/>
-      <c r="B38" s="79">
-        <v>3.3</v>
+      <c r="B38" s="73">
+        <v>3.4</v>
       </c>
       <c r="C38" s="58" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D38" s="28">
         <v>0</v>
       </c>
       <c r="E38" s="54">
-        <v>44264</v>
+        <f>F37+1</f>
+        <v>44276</v>
       </c>
       <c r="F38" s="54">
-        <f>E38+11</f>
-        <v>44275</v>
+        <f>E38+10</f>
+        <v>44286</v>
       </c>
       <c r="G38" s="13"/>
       <c r="H38" s="13">
         <f t="shared" si="37"/>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I38" s="34"/>
       <c r="J38" s="34"/>
@@ -7232,18 +6823,22 @@
     </row>
     <row r="39" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="47"/>
-      <c r="B39" s="80" t="s">
-        <v>68</v>
+      <c r="B39" s="73">
+        <v>3.5</v>
       </c>
       <c r="C39" s="58" t="s">
-        <v>72</v>
-      </c>
-      <c r="D39" s="28"/>
+        <v>63</v>
+      </c>
+      <c r="D39" s="28">
+        <v>0</v>
+      </c>
       <c r="E39" s="54">
-        <v>44264</v>
+        <f>F33+14</f>
+        <v>44269</v>
       </c>
       <c r="F39" s="54">
-        <v>44269</v>
+        <f>E39+5</f>
+        <v>44274</v>
       </c>
       <c r="G39" s="13"/>
       <c r="H39" s="13"/>
@@ -7348,21 +6943,28 @@
     </row>
     <row r="40" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="47"/>
-      <c r="B40" s="80" t="s">
-        <v>70</v>
+      <c r="B40" s="73">
+        <v>3.6</v>
       </c>
       <c r="C40" s="58" t="s">
-        <v>71</v>
-      </c>
-      <c r="D40" s="28"/>
+        <v>72</v>
+      </c>
+      <c r="D40" s="28">
+        <v>0</v>
+      </c>
       <c r="E40" s="54">
-        <v>44270</v>
+        <f>F39+1</f>
+        <v>44275</v>
       </c>
       <c r="F40" s="54">
-        <v>44270</v>
+        <f>E40+4</f>
+        <v>44279</v>
       </c>
       <c r="G40" s="13"/>
-      <c r="H40" s="13"/>
+      <c r="H40" s="13">
+        <f t="shared" si="37"/>
+        <v>5</v>
+      </c>
       <c r="I40" s="34"/>
       <c r="J40" s="34"/>
       <c r="K40" s="34"/>
@@ -7463,22 +7065,23 @@
       <c r="DB40" s="34"/>
     </row>
     <row r="41" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="47"/>
-      <c r="B41" s="80" t="s">
-        <v>73</v>
-      </c>
-      <c r="C41" s="58" t="s">
-        <v>74</v>
-      </c>
-      <c r="D41" s="28"/>
-      <c r="E41" s="54">
-        <v>44271</v>
-      </c>
-      <c r="F41" s="54">
-        <v>44275</v>
-      </c>
+      <c r="A41" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="B41" s="29">
+        <v>4</v>
+      </c>
+      <c r="C41" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="D41" s="30"/>
+      <c r="E41" s="31"/>
+      <c r="F41" s="32"/>
       <c r="G41" s="13"/>
-      <c r="H41" s="13"/>
+      <c r="H41" s="13" t="str">
+        <f t="shared" si="37"/>
+        <v/>
+      </c>
       <c r="I41" s="34"/>
       <c r="J41" s="34"/>
       <c r="K41" s="34"/>
@@ -7552,24 +7155,24 @@
       <c r="CA41" s="34"/>
       <c r="CB41" s="34"/>
       <c r="CC41" s="34"/>
-      <c r="CD41" s="34"/>
-      <c r="CE41" s="34"/>
-      <c r="CF41" s="34"/>
-      <c r="CG41" s="34"/>
-      <c r="CH41" s="34"/>
-      <c r="CI41" s="34"/>
-      <c r="CJ41" s="34"/>
-      <c r="CK41" s="34"/>
-      <c r="CL41" s="34"/>
-      <c r="CM41" s="34"/>
-      <c r="CN41" s="34"/>
-      <c r="CO41" s="34"/>
-      <c r="CP41" s="34"/>
-      <c r="CQ41" s="34"/>
-      <c r="CR41" s="34"/>
-      <c r="CS41" s="34"/>
-      <c r="CT41" s="34"/>
-      <c r="CU41" s="34"/>
+      <c r="CD41" s="79"/>
+      <c r="CE41" s="79"/>
+      <c r="CF41" s="79"/>
+      <c r="CG41" s="79"/>
+      <c r="CH41" s="79"/>
+      <c r="CI41" s="79"/>
+      <c r="CJ41" s="79"/>
+      <c r="CK41" s="79"/>
+      <c r="CL41" s="79"/>
+      <c r="CM41" s="79"/>
+      <c r="CN41" s="79"/>
+      <c r="CO41" s="79"/>
+      <c r="CP41" s="79"/>
+      <c r="CQ41" s="79"/>
+      <c r="CR41" s="79"/>
+      <c r="CS41" s="79"/>
+      <c r="CT41" s="79"/>
+      <c r="CU41" s="79"/>
       <c r="CV41" s="34"/>
       <c r="CW41" s="34"/>
       <c r="CX41" s="34"/>
@@ -7580,19 +7183,22 @@
     </row>
     <row r="42" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="47"/>
-      <c r="B42" s="79">
-        <v>3.4</v>
-      </c>
-      <c r="C42" s="58" t="s">
-        <v>75</v>
-      </c>
-      <c r="D42" s="28"/>
-      <c r="E42" s="54">
-        <v>44276</v>
-      </c>
-      <c r="F42" s="54">
-        <f>E42+10</f>
-        <v>44286</v>
+      <c r="B42" s="74">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="C42" s="59" t="s">
+        <v>73</v>
+      </c>
+      <c r="D42" s="33">
+        <v>0</v>
+      </c>
+      <c r="E42" s="55">
+        <f>F38+1</f>
+        <v>44287</v>
+      </c>
+      <c r="F42" s="55">
+        <f>E43-1</f>
+        <v>44292</v>
       </c>
       <c r="G42" s="13"/>
       <c r="H42" s="13"/>
@@ -7697,19 +7303,22 @@
     </row>
     <row r="43" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="47"/>
-      <c r="B43" s="79">
-        <v>3.5</v>
-      </c>
-      <c r="C43" s="58" t="s">
-        <v>79</v>
-      </c>
-      <c r="D43" s="28"/>
-      <c r="E43" s="54">
-        <v>44276</v>
-      </c>
-      <c r="F43" s="54">
-        <f>E43+2</f>
-        <v>44278</v>
+      <c r="B43" s="74">
+        <v>4.2</v>
+      </c>
+      <c r="C43" s="59" t="s">
+        <v>65</v>
+      </c>
+      <c r="D43" s="33">
+        <v>0</v>
+      </c>
+      <c r="E43" s="55">
+        <f>F40+14</f>
+        <v>44293</v>
+      </c>
+      <c r="F43" s="55">
+        <f>E43+7</f>
+        <v>44300</v>
       </c>
       <c r="G43" s="13"/>
       <c r="H43" s="13"/>
@@ -7814,25 +7423,25 @@
     </row>
     <row r="44" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="47"/>
-      <c r="B44" s="79">
-        <v>3.6</v>
-      </c>
-      <c r="C44" s="58" t="s">
-        <v>90</v>
-      </c>
-      <c r="D44" s="28"/>
-      <c r="E44" s="54">
-        <f>F43+1</f>
-        <v>44279</v>
-      </c>
-      <c r="F44" s="54">
-        <f>E44+3</f>
-        <v>44282</v>
+      <c r="B44" s="74">
+        <v>4.3</v>
+      </c>
+      <c r="C44" s="59" t="s">
+        <v>58</v>
+      </c>
+      <c r="D44" s="33">
+        <v>0</v>
+      </c>
+      <c r="E44" s="55">
+        <v>44301</v>
+      </c>
+      <c r="F44" s="55">
+        <v>44302</v>
       </c>
       <c r="G44" s="13"/>
       <c r="H44" s="13">
         <f t="shared" si="37"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I44" s="34"/>
       <c r="J44" s="34"/>
@@ -7934,22 +7543,26 @@
       <c r="DB44" s="34"/>
     </row>
     <row r="45" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="47" t="s">
-        <v>21</v>
-      </c>
-      <c r="B45" s="29">
-        <v>4</v>
-      </c>
-      <c r="C45" s="29" t="s">
-        <v>65</v>
-      </c>
-      <c r="D45" s="30"/>
-      <c r="E45" s="31"/>
-      <c r="F45" s="32"/>
+      <c r="A45" s="47"/>
+      <c r="B45" s="74">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="C45" s="59" t="s">
+        <v>57</v>
+      </c>
+      <c r="D45" s="33">
+        <v>0</v>
+      </c>
+      <c r="E45" s="55">
+        <v>44303</v>
+      </c>
+      <c r="F45" s="55">
+        <v>44304</v>
+      </c>
       <c r="G45" s="13"/>
-      <c r="H45" s="13" t="str">
+      <c r="H45" s="13">
         <f t="shared" si="37"/>
-        <v/>
+        <v>2</v>
       </c>
       <c r="I45" s="34"/>
       <c r="J45" s="34"/>
@@ -8024,24 +7637,24 @@
       <c r="CA45" s="34"/>
       <c r="CB45" s="34"/>
       <c r="CC45" s="34"/>
-      <c r="CD45" s="86"/>
-      <c r="CE45" s="86"/>
-      <c r="CF45" s="86"/>
-      <c r="CG45" s="86"/>
-      <c r="CH45" s="86"/>
-      <c r="CI45" s="86"/>
-      <c r="CJ45" s="86"/>
-      <c r="CK45" s="86"/>
-      <c r="CL45" s="86"/>
-      <c r="CM45" s="86"/>
-      <c r="CN45" s="86"/>
-      <c r="CO45" s="86"/>
-      <c r="CP45" s="86"/>
-      <c r="CQ45" s="86"/>
-      <c r="CR45" s="86"/>
-      <c r="CS45" s="86"/>
-      <c r="CT45" s="86"/>
-      <c r="CU45" s="86"/>
+      <c r="CD45" s="34"/>
+      <c r="CE45" s="34"/>
+      <c r="CF45" s="34"/>
+      <c r="CG45" s="34"/>
+      <c r="CH45" s="34"/>
+      <c r="CI45" s="34"/>
+      <c r="CJ45" s="34"/>
+      <c r="CK45" s="34"/>
+      <c r="CL45" s="34"/>
+      <c r="CM45" s="34"/>
+      <c r="CN45" s="34"/>
+      <c r="CO45" s="34"/>
+      <c r="CP45" s="34"/>
+      <c r="CQ45" s="34"/>
+      <c r="CR45" s="34"/>
+      <c r="CS45" s="34"/>
+      <c r="CT45" s="34"/>
+      <c r="CU45" s="34"/>
       <c r="CV45" s="34"/>
       <c r="CW45" s="34"/>
       <c r="CX45" s="34"/>
@@ -8051,26 +7664,22 @@
       <c r="DB45" s="34"/>
     </row>
     <row r="46" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="47"/>
-      <c r="B46" s="81">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="C46" s="59" t="s">
-        <v>85</v>
-      </c>
-      <c r="D46" s="33"/>
-      <c r="E46" s="55">
-        <f>F42+1</f>
-        <v>44287</v>
-      </c>
-      <c r="F46" s="55">
-        <f>E47-1</f>
-        <v>44295</v>
-      </c>
+      <c r="A46" s="47" t="s">
+        <v>23</v>
+      </c>
+      <c r="B46" s="61">
+        <v>5</v>
+      </c>
+      <c r="C46" s="61" t="s">
+        <v>39</v>
+      </c>
+      <c r="D46" s="62"/>
+      <c r="E46" s="63"/>
+      <c r="F46" s="64"/>
       <c r="G46" s="13"/>
-      <c r="H46" s="13">
+      <c r="H46" s="13" t="str">
         <f t="shared" si="37"/>
-        <v>9</v>
+        <v/>
       </c>
       <c r="I46" s="34"/>
       <c r="J46" s="34"/>
@@ -8172,24 +7781,29 @@
       <c r="DB46" s="34"/>
     </row>
     <row r="47" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="47"/>
-      <c r="B47" s="81">
-        <v>4.2</v>
-      </c>
-      <c r="C47" s="59" t="s">
-        <v>89</v>
-      </c>
-      <c r="D47" s="33"/>
-      <c r="E47" s="55">
-        <f>F44+14</f>
-        <v>44296</v>
-      </c>
-      <c r="F47" s="55">
-        <f>E47+4</f>
-        <v>44300</v>
+      <c r="A47" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="B47" s="75">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="C47" s="65" t="s">
+        <v>75</v>
+      </c>
+      <c r="D47" s="66">
+        <v>0</v>
+      </c>
+      <c r="E47" s="67" t="s">
+        <v>56</v>
+      </c>
+      <c r="F47" s="67" t="s">
+        <v>56</v>
       </c>
       <c r="G47" s="13"/>
-      <c r="H47" s="13"/>
+      <c r="H47" s="13" t="e">
+        <f t="shared" si="37"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="I47" s="34"/>
       <c r="J47" s="34"/>
       <c r="K47" s="34"/>
@@ -8289,25 +7903,26 @@
       <c r="DA47" s="34"/>
       <c r="DB47" s="34"/>
     </row>
-    <row r="48" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="47"/>
-      <c r="B48" s="81">
-        <v>4.3</v>
-      </c>
-      <c r="C48" s="59" t="s">
-        <v>88</v>
-      </c>
-      <c r="D48" s="33"/>
-      <c r="E48" s="55">
-        <v>44301</v>
-      </c>
-      <c r="F48" s="55">
-        <v>44302</v>
+    <row r="48" spans="1:106" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B48" s="75">
+        <v>5.2</v>
+      </c>
+      <c r="C48" s="65" t="s">
+        <v>74</v>
+      </c>
+      <c r="D48" s="66">
+        <v>0</v>
+      </c>
+      <c r="E48" s="67" t="s">
+        <v>56</v>
+      </c>
+      <c r="F48" s="67" t="s">
+        <v>56</v>
       </c>
       <c r="G48" s="13"/>
-      <c r="H48" s="13">
+      <c r="H48" s="13" t="e">
         <f t="shared" si="37"/>
-        <v>2</v>
+        <v>#VALUE!</v>
       </c>
       <c r="I48" s="34"/>
       <c r="J48" s="34"/>
@@ -8408,717 +8023,6 @@
       <c r="DA48" s="34"/>
       <c r="DB48" s="34"/>
     </row>
-    <row r="49" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="47"/>
-      <c r="B49" s="81">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="C49" s="59" t="s">
-        <v>87</v>
-      </c>
-      <c r="D49" s="33"/>
-      <c r="E49" s="55">
-        <v>44303</v>
-      </c>
-      <c r="F49" s="55">
-        <v>44304</v>
-      </c>
-      <c r="G49" s="13"/>
-      <c r="H49" s="13">
-        <f t="shared" si="37"/>
-        <v>2</v>
-      </c>
-      <c r="I49" s="34"/>
-      <c r="J49" s="34"/>
-      <c r="K49" s="34"/>
-      <c r="L49" s="34"/>
-      <c r="M49" s="34"/>
-      <c r="N49" s="34"/>
-      <c r="O49" s="34"/>
-      <c r="P49" s="34"/>
-      <c r="Q49" s="34"/>
-      <c r="R49" s="34"/>
-      <c r="S49" s="34"/>
-      <c r="T49" s="34"/>
-      <c r="U49" s="34"/>
-      <c r="V49" s="34"/>
-      <c r="W49" s="34"/>
-      <c r="X49" s="34"/>
-      <c r="Y49" s="34"/>
-      <c r="Z49" s="34"/>
-      <c r="AA49" s="34"/>
-      <c r="AB49" s="34"/>
-      <c r="AC49" s="34"/>
-      <c r="AD49" s="34"/>
-      <c r="AE49" s="34"/>
-      <c r="AF49" s="34"/>
-      <c r="AG49" s="34"/>
-      <c r="AH49" s="34"/>
-      <c r="AI49" s="34"/>
-      <c r="AJ49" s="34"/>
-      <c r="AK49" s="34"/>
-      <c r="AL49" s="34"/>
-      <c r="AM49" s="34"/>
-      <c r="AN49" s="34"/>
-      <c r="AO49" s="34"/>
-      <c r="AP49" s="34"/>
-      <c r="AQ49" s="34"/>
-      <c r="AR49" s="34"/>
-      <c r="AS49" s="34"/>
-      <c r="AT49" s="34"/>
-      <c r="AU49" s="34"/>
-      <c r="AV49" s="34"/>
-      <c r="AW49" s="34"/>
-      <c r="AX49" s="34"/>
-      <c r="AY49" s="34"/>
-      <c r="AZ49" s="34"/>
-      <c r="BA49" s="34"/>
-      <c r="BB49" s="34"/>
-      <c r="BC49" s="34"/>
-      <c r="BD49" s="34"/>
-      <c r="BE49" s="34"/>
-      <c r="BF49" s="34"/>
-      <c r="BG49" s="34"/>
-      <c r="BH49" s="34"/>
-      <c r="BI49" s="34"/>
-      <c r="BJ49" s="34"/>
-      <c r="BK49" s="34"/>
-      <c r="BL49" s="34"/>
-      <c r="BM49" s="34"/>
-      <c r="BN49" s="34"/>
-      <c r="BO49" s="34"/>
-      <c r="BP49" s="34"/>
-      <c r="BQ49" s="34"/>
-      <c r="BR49" s="34"/>
-      <c r="BS49" s="34"/>
-      <c r="BT49" s="34"/>
-      <c r="BU49" s="34"/>
-      <c r="BV49" s="34"/>
-      <c r="BW49" s="34"/>
-      <c r="BX49" s="34"/>
-      <c r="BY49" s="34"/>
-      <c r="BZ49" s="34"/>
-      <c r="CA49" s="34"/>
-      <c r="CB49" s="34"/>
-      <c r="CC49" s="34"/>
-      <c r="CD49" s="34"/>
-      <c r="CE49" s="34"/>
-      <c r="CF49" s="34"/>
-      <c r="CG49" s="34"/>
-      <c r="CH49" s="34"/>
-      <c r="CI49" s="34"/>
-      <c r="CJ49" s="34"/>
-      <c r="CK49" s="34"/>
-      <c r="CL49" s="34"/>
-      <c r="CM49" s="34"/>
-      <c r="CN49" s="34"/>
-      <c r="CO49" s="34"/>
-      <c r="CP49" s="34"/>
-      <c r="CQ49" s="34"/>
-      <c r="CR49" s="34"/>
-      <c r="CS49" s="34"/>
-      <c r="CT49" s="34"/>
-      <c r="CU49" s="34"/>
-      <c r="CV49" s="34"/>
-      <c r="CW49" s="34"/>
-      <c r="CX49" s="34"/>
-      <c r="CY49" s="34"/>
-      <c r="CZ49" s="34"/>
-      <c r="DA49" s="34"/>
-      <c r="DB49" s="34"/>
-    </row>
-    <row r="50" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="47" t="s">
-        <v>23</v>
-      </c>
-      <c r="B50" s="66">
-        <v>5</v>
-      </c>
-      <c r="C50" s="66" t="s">
-        <v>40</v>
-      </c>
-      <c r="D50" s="67"/>
-      <c r="E50" s="68"/>
-      <c r="F50" s="69"/>
-      <c r="G50" s="13"/>
-      <c r="H50" s="13" t="str">
-        <f t="shared" si="37"/>
-        <v/>
-      </c>
-      <c r="I50" s="34"/>
-      <c r="J50" s="34"/>
-      <c r="K50" s="34"/>
-      <c r="L50" s="34"/>
-      <c r="M50" s="34"/>
-      <c r="N50" s="34"/>
-      <c r="O50" s="34"/>
-      <c r="P50" s="34"/>
-      <c r="Q50" s="34"/>
-      <c r="R50" s="34"/>
-      <c r="S50" s="34"/>
-      <c r="T50" s="34"/>
-      <c r="U50" s="34"/>
-      <c r="V50" s="34"/>
-      <c r="W50" s="34"/>
-      <c r="X50" s="34"/>
-      <c r="Y50" s="34"/>
-      <c r="Z50" s="34"/>
-      <c r="AA50" s="34"/>
-      <c r="AB50" s="34"/>
-      <c r="AC50" s="34"/>
-      <c r="AD50" s="34"/>
-      <c r="AE50" s="34"/>
-      <c r="AF50" s="34"/>
-      <c r="AG50" s="34"/>
-      <c r="AH50" s="34"/>
-      <c r="AI50" s="34"/>
-      <c r="AJ50" s="34"/>
-      <c r="AK50" s="34"/>
-      <c r="AL50" s="34"/>
-      <c r="AM50" s="34"/>
-      <c r="AN50" s="34"/>
-      <c r="AO50" s="34"/>
-      <c r="AP50" s="34"/>
-      <c r="AQ50" s="34"/>
-      <c r="AR50" s="34"/>
-      <c r="AS50" s="34"/>
-      <c r="AT50" s="34"/>
-      <c r="AU50" s="34"/>
-      <c r="AV50" s="34"/>
-      <c r="AW50" s="34"/>
-      <c r="AX50" s="34"/>
-      <c r="AY50" s="34"/>
-      <c r="AZ50" s="34"/>
-      <c r="BA50" s="34"/>
-      <c r="BB50" s="34"/>
-      <c r="BC50" s="34"/>
-      <c r="BD50" s="34"/>
-      <c r="BE50" s="34"/>
-      <c r="BF50" s="34"/>
-      <c r="BG50" s="34"/>
-      <c r="BH50" s="34"/>
-      <c r="BI50" s="34"/>
-      <c r="BJ50" s="34"/>
-      <c r="BK50" s="34"/>
-      <c r="BL50" s="34"/>
-      <c r="BM50" s="34"/>
-      <c r="BN50" s="34"/>
-      <c r="BO50" s="34"/>
-      <c r="BP50" s="34"/>
-      <c r="BQ50" s="34"/>
-      <c r="BR50" s="34"/>
-      <c r="BS50" s="34"/>
-      <c r="BT50" s="34"/>
-      <c r="BU50" s="34"/>
-      <c r="BV50" s="34"/>
-      <c r="BW50" s="34"/>
-      <c r="BX50" s="34"/>
-      <c r="BY50" s="34"/>
-      <c r="BZ50" s="34"/>
-      <c r="CA50" s="34"/>
-      <c r="CB50" s="34"/>
-      <c r="CC50" s="34"/>
-      <c r="CD50" s="34"/>
-      <c r="CE50" s="34"/>
-      <c r="CF50" s="34"/>
-      <c r="CG50" s="34"/>
-      <c r="CH50" s="34"/>
-      <c r="CI50" s="34"/>
-      <c r="CJ50" s="34"/>
-      <c r="CK50" s="34"/>
-      <c r="CL50" s="34"/>
-      <c r="CM50" s="34"/>
-      <c r="CN50" s="34"/>
-      <c r="CO50" s="34"/>
-      <c r="CP50" s="34"/>
-      <c r="CQ50" s="34"/>
-      <c r="CR50" s="34"/>
-      <c r="CS50" s="34"/>
-      <c r="CT50" s="34"/>
-      <c r="CU50" s="34"/>
-      <c r="CV50" s="34"/>
-      <c r="CW50" s="34"/>
-      <c r="CX50" s="34"/>
-      <c r="CY50" s="34"/>
-      <c r="CZ50" s="34"/>
-      <c r="DA50" s="34"/>
-      <c r="DB50" s="34"/>
-    </row>
-    <row r="51" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="B51" s="82">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="C51" s="70" t="s">
-        <v>80</v>
-      </c>
-      <c r="D51" s="71"/>
-      <c r="E51" s="72" t="s">
-        <v>86</v>
-      </c>
-      <c r="F51" s="72" t="s">
-        <v>86</v>
-      </c>
-      <c r="G51" s="13"/>
-      <c r="H51" s="13" t="e">
-        <f t="shared" si="37"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I51" s="34"/>
-      <c r="J51" s="34"/>
-      <c r="K51" s="34"/>
-      <c r="L51" s="34"/>
-      <c r="M51" s="34"/>
-      <c r="N51" s="34"/>
-      <c r="O51" s="34"/>
-      <c r="P51" s="34"/>
-      <c r="Q51" s="34"/>
-      <c r="R51" s="34"/>
-      <c r="S51" s="34"/>
-      <c r="T51" s="34"/>
-      <c r="U51" s="34"/>
-      <c r="V51" s="34"/>
-      <c r="W51" s="34"/>
-      <c r="X51" s="34"/>
-      <c r="Y51" s="34"/>
-      <c r="Z51" s="34"/>
-      <c r="AA51" s="34"/>
-      <c r="AB51" s="34"/>
-      <c r="AC51" s="34"/>
-      <c r="AD51" s="34"/>
-      <c r="AE51" s="34"/>
-      <c r="AF51" s="34"/>
-      <c r="AG51" s="34"/>
-      <c r="AH51" s="34"/>
-      <c r="AI51" s="34"/>
-      <c r="AJ51" s="34"/>
-      <c r="AK51" s="34"/>
-      <c r="AL51" s="34"/>
-      <c r="AM51" s="34"/>
-      <c r="AN51" s="34"/>
-      <c r="AO51" s="34"/>
-      <c r="AP51" s="34"/>
-      <c r="AQ51" s="34"/>
-      <c r="AR51" s="34"/>
-      <c r="AS51" s="34"/>
-      <c r="AT51" s="34"/>
-      <c r="AU51" s="34"/>
-      <c r="AV51" s="34"/>
-      <c r="AW51" s="34"/>
-      <c r="AX51" s="34"/>
-      <c r="AY51" s="34"/>
-      <c r="AZ51" s="34"/>
-      <c r="BA51" s="34"/>
-      <c r="BB51" s="34"/>
-      <c r="BC51" s="34"/>
-      <c r="BD51" s="34"/>
-      <c r="BE51" s="34"/>
-      <c r="BF51" s="34"/>
-      <c r="BG51" s="34"/>
-      <c r="BH51" s="34"/>
-      <c r="BI51" s="34"/>
-      <c r="BJ51" s="34"/>
-      <c r="BK51" s="34"/>
-      <c r="BL51" s="34"/>
-      <c r="BM51" s="34"/>
-      <c r="BN51" s="34"/>
-      <c r="BO51" s="34"/>
-      <c r="BP51" s="34"/>
-      <c r="BQ51" s="34"/>
-      <c r="BR51" s="34"/>
-      <c r="BS51" s="34"/>
-      <c r="BT51" s="34"/>
-      <c r="BU51" s="34"/>
-      <c r="BV51" s="34"/>
-      <c r="BW51" s="34"/>
-      <c r="BX51" s="34"/>
-      <c r="BY51" s="34"/>
-      <c r="BZ51" s="34"/>
-      <c r="CA51" s="34"/>
-      <c r="CB51" s="34"/>
-      <c r="CC51" s="34"/>
-      <c r="CD51" s="34"/>
-      <c r="CE51" s="34"/>
-      <c r="CF51" s="34"/>
-      <c r="CG51" s="34"/>
-      <c r="CH51" s="34"/>
-      <c r="CI51" s="34"/>
-      <c r="CJ51" s="34"/>
-      <c r="CK51" s="34"/>
-      <c r="CL51" s="34"/>
-      <c r="CM51" s="34"/>
-      <c r="CN51" s="34"/>
-      <c r="CO51" s="34"/>
-      <c r="CP51" s="34"/>
-      <c r="CQ51" s="34"/>
-      <c r="CR51" s="34"/>
-      <c r="CS51" s="34"/>
-      <c r="CT51" s="34"/>
-      <c r="CU51" s="34"/>
-      <c r="CV51" s="34"/>
-      <c r="CW51" s="34"/>
-      <c r="CX51" s="34"/>
-      <c r="CY51" s="34"/>
-      <c r="CZ51" s="34"/>
-      <c r="DA51" s="34"/>
-      <c r="DB51" s="34"/>
-    </row>
-    <row r="52" spans="1:106" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="82">
-        <v>5.2</v>
-      </c>
-      <c r="C52" s="70" t="s">
-        <v>81</v>
-      </c>
-      <c r="D52" s="71"/>
-      <c r="E52" s="72" t="s">
-        <v>86</v>
-      </c>
-      <c r="F52" s="72" t="s">
-        <v>86</v>
-      </c>
-      <c r="G52" s="13"/>
-      <c r="H52" s="13" t="e">
-        <f t="shared" si="37"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I52" s="34"/>
-      <c r="J52" s="34"/>
-      <c r="K52" s="34"/>
-      <c r="L52" s="34"/>
-      <c r="M52" s="34"/>
-      <c r="N52" s="34"/>
-      <c r="O52" s="34"/>
-      <c r="P52" s="34"/>
-      <c r="Q52" s="34"/>
-      <c r="R52" s="34"/>
-      <c r="S52" s="34"/>
-      <c r="T52" s="34"/>
-      <c r="U52" s="34"/>
-      <c r="V52" s="34"/>
-      <c r="W52" s="34"/>
-      <c r="X52" s="34"/>
-      <c r="Y52" s="34"/>
-      <c r="Z52" s="34"/>
-      <c r="AA52" s="34"/>
-      <c r="AB52" s="34"/>
-      <c r="AC52" s="34"/>
-      <c r="AD52" s="34"/>
-      <c r="AE52" s="34"/>
-      <c r="AF52" s="34"/>
-      <c r="AG52" s="34"/>
-      <c r="AH52" s="34"/>
-      <c r="AI52" s="34"/>
-      <c r="AJ52" s="34"/>
-      <c r="AK52" s="34"/>
-      <c r="AL52" s="34"/>
-      <c r="AM52" s="34"/>
-      <c r="AN52" s="34"/>
-      <c r="AO52" s="34"/>
-      <c r="AP52" s="34"/>
-      <c r="AQ52" s="34"/>
-      <c r="AR52" s="34"/>
-      <c r="AS52" s="34"/>
-      <c r="AT52" s="34"/>
-      <c r="AU52" s="34"/>
-      <c r="AV52" s="34"/>
-      <c r="AW52" s="34"/>
-      <c r="AX52" s="34"/>
-      <c r="AY52" s="34"/>
-      <c r="AZ52" s="34"/>
-      <c r="BA52" s="34"/>
-      <c r="BB52" s="34"/>
-      <c r="BC52" s="34"/>
-      <c r="BD52" s="34"/>
-      <c r="BE52" s="34"/>
-      <c r="BF52" s="34"/>
-      <c r="BG52" s="34"/>
-      <c r="BH52" s="34"/>
-      <c r="BI52" s="34"/>
-      <c r="BJ52" s="34"/>
-      <c r="BK52" s="34"/>
-      <c r="BL52" s="34"/>
-      <c r="BM52" s="34"/>
-      <c r="BN52" s="34"/>
-      <c r="BO52" s="34"/>
-      <c r="BP52" s="34"/>
-      <c r="BQ52" s="34"/>
-      <c r="BR52" s="34"/>
-      <c r="BS52" s="34"/>
-      <c r="BT52" s="34"/>
-      <c r="BU52" s="34"/>
-      <c r="BV52" s="34"/>
-      <c r="BW52" s="34"/>
-      <c r="BX52" s="34"/>
-      <c r="BY52" s="34"/>
-      <c r="BZ52" s="34"/>
-      <c r="CA52" s="34"/>
-      <c r="CB52" s="34"/>
-      <c r="CC52" s="34"/>
-      <c r="CD52" s="34"/>
-      <c r="CE52" s="34"/>
-      <c r="CF52" s="34"/>
-      <c r="CG52" s="34"/>
-      <c r="CH52" s="34"/>
-      <c r="CI52" s="34"/>
-      <c r="CJ52" s="34"/>
-      <c r="CK52" s="34"/>
-      <c r="CL52" s="34"/>
-      <c r="CM52" s="34"/>
-      <c r="CN52" s="34"/>
-      <c r="CO52" s="34"/>
-      <c r="CP52" s="34"/>
-      <c r="CQ52" s="34"/>
-      <c r="CR52" s="34"/>
-      <c r="CS52" s="34"/>
-      <c r="CT52" s="34"/>
-      <c r="CU52" s="34"/>
-      <c r="CV52" s="34"/>
-      <c r="CW52" s="34"/>
-      <c r="CX52" s="34"/>
-      <c r="CY52" s="34"/>
-      <c r="CZ52" s="34"/>
-      <c r="DA52" s="34"/>
-      <c r="DB52" s="34"/>
-    </row>
-    <row r="53" spans="1:106" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B53" s="82">
-        <v>5.3</v>
-      </c>
-      <c r="C53" s="70" t="s">
-        <v>82</v>
-      </c>
-      <c r="D53" s="71"/>
-      <c r="E53" s="72" t="s">
-        <v>86</v>
-      </c>
-      <c r="F53" s="72" t="s">
-        <v>86</v>
-      </c>
-      <c r="G53" s="13"/>
-      <c r="H53" s="13" t="e">
-        <f t="shared" si="37"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I53" s="34"/>
-      <c r="J53" s="34"/>
-      <c r="K53" s="34"/>
-      <c r="L53" s="34"/>
-      <c r="M53" s="34"/>
-      <c r="N53" s="34"/>
-      <c r="O53" s="34"/>
-      <c r="P53" s="34"/>
-      <c r="Q53" s="34"/>
-      <c r="R53" s="34"/>
-      <c r="S53" s="34"/>
-      <c r="T53" s="34"/>
-      <c r="U53" s="34"/>
-      <c r="V53" s="34"/>
-      <c r="W53" s="34"/>
-      <c r="X53" s="34"/>
-      <c r="Y53" s="34"/>
-      <c r="Z53" s="34"/>
-      <c r="AA53" s="34"/>
-      <c r="AB53" s="34"/>
-      <c r="AC53" s="34"/>
-      <c r="AD53" s="34"/>
-      <c r="AE53" s="34"/>
-      <c r="AF53" s="34"/>
-      <c r="AG53" s="34"/>
-      <c r="AH53" s="34"/>
-      <c r="AI53" s="34"/>
-      <c r="AJ53" s="34"/>
-      <c r="AK53" s="34"/>
-      <c r="AL53" s="34"/>
-      <c r="AM53" s="34"/>
-      <c r="AN53" s="34"/>
-      <c r="AO53" s="34"/>
-      <c r="AP53" s="34"/>
-      <c r="AQ53" s="34"/>
-      <c r="AR53" s="34"/>
-      <c r="AS53" s="34"/>
-      <c r="AT53" s="34"/>
-      <c r="AU53" s="34"/>
-      <c r="AV53" s="34"/>
-      <c r="AW53" s="34"/>
-      <c r="AX53" s="34"/>
-      <c r="AY53" s="34"/>
-      <c r="AZ53" s="34"/>
-      <c r="BA53" s="34"/>
-      <c r="BB53" s="34"/>
-      <c r="BC53" s="34"/>
-      <c r="BD53" s="34"/>
-      <c r="BE53" s="34"/>
-      <c r="BF53" s="34"/>
-      <c r="BG53" s="34"/>
-      <c r="BH53" s="34"/>
-      <c r="BI53" s="34"/>
-      <c r="BJ53" s="34"/>
-      <c r="BK53" s="34"/>
-      <c r="BL53" s="34"/>
-      <c r="BM53" s="34"/>
-      <c r="BN53" s="34"/>
-      <c r="BO53" s="34"/>
-      <c r="BP53" s="34"/>
-      <c r="BQ53" s="34"/>
-      <c r="BR53" s="34"/>
-      <c r="BS53" s="34"/>
-      <c r="BT53" s="34"/>
-      <c r="BU53" s="34"/>
-      <c r="BV53" s="34"/>
-      <c r="BW53" s="34"/>
-      <c r="BX53" s="34"/>
-      <c r="BY53" s="34"/>
-      <c r="BZ53" s="34"/>
-      <c r="CA53" s="34"/>
-      <c r="CB53" s="34"/>
-      <c r="CC53" s="34"/>
-      <c r="CD53" s="34"/>
-      <c r="CE53" s="34"/>
-      <c r="CF53" s="34"/>
-      <c r="CG53" s="34"/>
-      <c r="CH53" s="34"/>
-      <c r="CI53" s="34"/>
-      <c r="CJ53" s="34"/>
-      <c r="CK53" s="34"/>
-      <c r="CL53" s="34"/>
-      <c r="CM53" s="34"/>
-      <c r="CN53" s="34"/>
-      <c r="CO53" s="34"/>
-      <c r="CP53" s="34"/>
-      <c r="CQ53" s="34"/>
-      <c r="CR53" s="34"/>
-      <c r="CS53" s="34"/>
-      <c r="CT53" s="34"/>
-      <c r="CU53" s="34"/>
-      <c r="CV53" s="34"/>
-      <c r="CW53" s="34"/>
-      <c r="CX53" s="34"/>
-      <c r="CY53" s="34"/>
-      <c r="CZ53" s="34"/>
-      <c r="DA53" s="34"/>
-      <c r="DB53" s="34"/>
-    </row>
-    <row r="54" spans="1:106" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="82">
-        <v>5.4</v>
-      </c>
-      <c r="C54" s="70" t="s">
-        <v>83</v>
-      </c>
-      <c r="D54" s="71"/>
-      <c r="E54" s="72" t="s">
-        <v>86</v>
-      </c>
-      <c r="F54" s="72" t="s">
-        <v>86</v>
-      </c>
-      <c r="G54" s="13"/>
-      <c r="H54" s="13" t="e">
-        <f t="shared" si="37"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I54" s="34"/>
-      <c r="J54" s="34"/>
-      <c r="K54" s="34"/>
-      <c r="L54" s="34"/>
-      <c r="M54" s="34"/>
-      <c r="N54" s="34"/>
-      <c r="O54" s="34"/>
-      <c r="P54" s="34"/>
-      <c r="Q54" s="34"/>
-      <c r="R54" s="34"/>
-      <c r="S54" s="34"/>
-      <c r="T54" s="34"/>
-      <c r="U54" s="34"/>
-      <c r="V54" s="34"/>
-      <c r="W54" s="34"/>
-      <c r="X54" s="34"/>
-      <c r="Y54" s="34"/>
-      <c r="Z54" s="34"/>
-      <c r="AA54" s="34"/>
-      <c r="AB54" s="34"/>
-      <c r="AC54" s="34"/>
-      <c r="AD54" s="34"/>
-      <c r="AE54" s="34"/>
-      <c r="AF54" s="34"/>
-      <c r="AG54" s="34"/>
-      <c r="AH54" s="34"/>
-      <c r="AI54" s="34"/>
-      <c r="AJ54" s="34"/>
-      <c r="AK54" s="34"/>
-      <c r="AL54" s="34"/>
-      <c r="AM54" s="34"/>
-      <c r="AN54" s="34"/>
-      <c r="AO54" s="34"/>
-      <c r="AP54" s="34"/>
-      <c r="AQ54" s="34"/>
-      <c r="AR54" s="34"/>
-      <c r="AS54" s="34"/>
-      <c r="AT54" s="34"/>
-      <c r="AU54" s="34"/>
-      <c r="AV54" s="34"/>
-      <c r="AW54" s="34"/>
-      <c r="AX54" s="34"/>
-      <c r="AY54" s="34"/>
-      <c r="AZ54" s="34"/>
-      <c r="BA54" s="34"/>
-      <c r="BB54" s="34"/>
-      <c r="BC54" s="34"/>
-      <c r="BD54" s="34"/>
-      <c r="BE54" s="34"/>
-      <c r="BF54" s="34"/>
-      <c r="BG54" s="34"/>
-      <c r="BH54" s="34"/>
-      <c r="BI54" s="34"/>
-      <c r="BJ54" s="34"/>
-      <c r="BK54" s="34"/>
-      <c r="BL54" s="34"/>
-      <c r="BM54" s="34"/>
-      <c r="BN54" s="34"/>
-      <c r="BO54" s="34"/>
-      <c r="BP54" s="34"/>
-      <c r="BQ54" s="34"/>
-      <c r="BR54" s="34"/>
-      <c r="BS54" s="34"/>
-      <c r="BT54" s="34"/>
-      <c r="BU54" s="34"/>
-      <c r="BV54" s="34"/>
-      <c r="BW54" s="34"/>
-      <c r="BX54" s="34"/>
-      <c r="BY54" s="34"/>
-      <c r="BZ54" s="34"/>
-      <c r="CA54" s="34"/>
-      <c r="CB54" s="34"/>
-      <c r="CC54" s="34"/>
-      <c r="CD54" s="34"/>
-      <c r="CE54" s="34"/>
-      <c r="CF54" s="34"/>
-      <c r="CG54" s="34"/>
-      <c r="CH54" s="34"/>
-      <c r="CI54" s="34"/>
-      <c r="CJ54" s="34"/>
-      <c r="CK54" s="34"/>
-      <c r="CL54" s="34"/>
-      <c r="CM54" s="34"/>
-      <c r="CN54" s="34"/>
-      <c r="CO54" s="34"/>
-      <c r="CP54" s="34"/>
-      <c r="CQ54" s="34"/>
-      <c r="CR54" s="34"/>
-      <c r="CS54" s="34"/>
-      <c r="CT54" s="34"/>
-      <c r="CU54" s="34"/>
-      <c r="CV54" s="34"/>
-      <c r="CW54" s="34"/>
-      <c r="CX54" s="34"/>
-      <c r="CY54" s="34"/>
-      <c r="CZ54" s="34"/>
-      <c r="DA54" s="34"/>
-      <c r="DB54" s="34"/>
-    </row>
   </sheetData>
   <mergeCells count="16">
     <mergeCell ref="CV4:DB4"/>
@@ -9138,7 +8042,7 @@
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="AD4:AJ4"/>
   </mergeCells>
-  <conditionalFormatting sqref="D7:D49">
+  <conditionalFormatting sqref="D7:D48">
     <cfRule type="dataBar" priority="120">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -9152,394 +8056,198 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I5:DB50">
-    <cfRule type="expression" dxfId="86" priority="139">
+  <conditionalFormatting sqref="I5:DB46">
+    <cfRule type="expression" dxfId="44" priority="139">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I7:DB50">
-    <cfRule type="expression" dxfId="85" priority="133">
+  <conditionalFormatting sqref="I7:DB46">
+    <cfRule type="expression" dxfId="43" priority="133">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="84" priority="134" stopIfTrue="1">
+    <cfRule type="expression" dxfId="42" priority="134" stopIfTrue="1">
       <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D50:D54">
-    <cfRule type="dataBar" priority="106">
-      <dataBar>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="1"/>
-        <color theme="0" tint="-0.249977111117893"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{FFEC5DDB-C5BB-49AF-B8EA-B3E6AB9311C2}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I51:BL51">
-    <cfRule type="expression" dxfId="83" priority="105">
+  <conditionalFormatting sqref="I47:BL47">
+    <cfRule type="expression" dxfId="41" priority="105">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I51:BL51">
-    <cfRule type="expression" dxfId="82" priority="103">
+  <conditionalFormatting sqref="I47:BL47">
+    <cfRule type="expression" dxfId="40" priority="103">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="81" priority="104" stopIfTrue="1">
+    <cfRule type="expression" dxfId="39" priority="104" stopIfTrue="1">
       <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I52:BL52">
-    <cfRule type="expression" dxfId="80" priority="102">
+  <conditionalFormatting sqref="I48:BL48">
+    <cfRule type="expression" dxfId="38" priority="102">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I52:BL52">
-    <cfRule type="expression" dxfId="79" priority="100">
+  <conditionalFormatting sqref="I48:BL48">
+    <cfRule type="expression" dxfId="37" priority="100">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="78" priority="101" stopIfTrue="1">
+    <cfRule type="expression" dxfId="36" priority="101" stopIfTrue="1">
       <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I53:BL53">
-    <cfRule type="expression" dxfId="77" priority="99">
-      <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I53:BL53">
-    <cfRule type="expression" dxfId="76" priority="97">
-      <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="75" priority="98" stopIfTrue="1">
-      <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I54:BL54">
-    <cfRule type="expression" dxfId="74" priority="96">
-      <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I54:BL54">
-    <cfRule type="expression" dxfId="73" priority="94">
-      <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="72" priority="95" stopIfTrue="1">
-      <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="BM51:BS51">
-    <cfRule type="expression" dxfId="71" priority="87">
+  <conditionalFormatting sqref="BM47:BS47">
+    <cfRule type="expression" dxfId="35" priority="87">
       <formula>AND(TODAY()&gt;=BM$5,TODAY()&lt;BN$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BM51:BS51">
-    <cfRule type="expression" dxfId="70" priority="85">
+  <conditionalFormatting sqref="BM47:BS47">
+    <cfRule type="expression" dxfId="34" priority="85">
       <formula>AND(task_start&lt;=BM$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=BM$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="69" priority="86" stopIfTrue="1">
+    <cfRule type="expression" dxfId="33" priority="86" stopIfTrue="1">
       <formula>AND(task_end&gt;=BM$5,task_start&lt;BN$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BM52:BS52">
-    <cfRule type="expression" dxfId="68" priority="84">
+  <conditionalFormatting sqref="BM48:BS48">
+    <cfRule type="expression" dxfId="32" priority="84">
       <formula>AND(TODAY()&gt;=BM$5,TODAY()&lt;BN$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BM52:BS52">
-    <cfRule type="expression" dxfId="67" priority="82">
+  <conditionalFormatting sqref="BM48:BS48">
+    <cfRule type="expression" dxfId="31" priority="82">
       <formula>AND(task_start&lt;=BM$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=BM$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="66" priority="83" stopIfTrue="1">
+    <cfRule type="expression" dxfId="30" priority="83" stopIfTrue="1">
       <formula>AND(task_end&gt;=BM$5,task_start&lt;BN$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BM53:BS53">
-    <cfRule type="expression" dxfId="65" priority="81">
-      <formula>AND(TODAY()&gt;=BM$5,TODAY()&lt;BN$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="BM53:BS53">
-    <cfRule type="expression" dxfId="64" priority="79">
-      <formula>AND(task_start&lt;=BM$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=BM$5)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="63" priority="80" stopIfTrue="1">
-      <formula>AND(task_end&gt;=BM$5,task_start&lt;BN$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="BM54:BS54">
-    <cfRule type="expression" dxfId="62" priority="78">
-      <formula>AND(TODAY()&gt;=BM$5,TODAY()&lt;BN$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="BM54:BS54">
-    <cfRule type="expression" dxfId="61" priority="76">
-      <formula>AND(task_start&lt;=BM$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=BM$5)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="60" priority="77" stopIfTrue="1">
-      <formula>AND(task_end&gt;=BM$5,task_start&lt;BN$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="BT51:BZ51">
-    <cfRule type="expression" dxfId="59" priority="72">
+  <conditionalFormatting sqref="BT47:BZ47">
+    <cfRule type="expression" dxfId="29" priority="72">
       <formula>AND(TODAY()&gt;=BT$5,TODAY()&lt;BU$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BT51:BZ51">
-    <cfRule type="expression" dxfId="58" priority="70">
+  <conditionalFormatting sqref="BT47:BZ47">
+    <cfRule type="expression" dxfId="28" priority="70">
       <formula>AND(task_start&lt;=BT$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=BT$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="57" priority="71" stopIfTrue="1">
+    <cfRule type="expression" dxfId="27" priority="71" stopIfTrue="1">
       <formula>AND(task_end&gt;=BT$5,task_start&lt;BU$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BT52:BZ52">
-    <cfRule type="expression" dxfId="56" priority="69">
+  <conditionalFormatting sqref="BT48:BZ48">
+    <cfRule type="expression" dxfId="26" priority="69">
       <formula>AND(TODAY()&gt;=BT$5,TODAY()&lt;BU$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BT52:BZ52">
-    <cfRule type="expression" dxfId="55" priority="67">
+  <conditionalFormatting sqref="BT48:BZ48">
+    <cfRule type="expression" dxfId="25" priority="67">
       <formula>AND(task_start&lt;=BT$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=BT$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="54" priority="68" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="68" stopIfTrue="1">
       <formula>AND(task_end&gt;=BT$5,task_start&lt;BU$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BT53:BZ53">
-    <cfRule type="expression" dxfId="53" priority="66">
-      <formula>AND(TODAY()&gt;=BT$5,TODAY()&lt;BU$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="BT53:BZ53">
-    <cfRule type="expression" dxfId="52" priority="64">
-      <formula>AND(task_start&lt;=BT$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=BT$5)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="51" priority="65" stopIfTrue="1">
-      <formula>AND(task_end&gt;=BT$5,task_start&lt;BU$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="BT54:BZ54">
-    <cfRule type="expression" dxfId="50" priority="63">
-      <formula>AND(TODAY()&gt;=BT$5,TODAY()&lt;BU$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="BT54:BZ54">
-    <cfRule type="expression" dxfId="49" priority="61">
-      <formula>AND(task_start&lt;=BT$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=BT$5)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="48" priority="62" stopIfTrue="1">
-      <formula>AND(task_end&gt;=BT$5,task_start&lt;BU$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="CA51:CG51">
-    <cfRule type="expression" dxfId="47" priority="57">
+  <conditionalFormatting sqref="CA47:CG47">
+    <cfRule type="expression" dxfId="23" priority="57">
       <formula>AND(TODAY()&gt;=CA$5,TODAY()&lt;CB$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="CA51:CG51">
-    <cfRule type="expression" dxfId="46" priority="55">
+  <conditionalFormatting sqref="CA47:CG47">
+    <cfRule type="expression" dxfId="22" priority="55">
       <formula>AND(task_start&lt;=CA$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=CA$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="45" priority="56" stopIfTrue="1">
+    <cfRule type="expression" dxfId="21" priority="56" stopIfTrue="1">
       <formula>AND(task_end&gt;=CA$5,task_start&lt;CB$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="CA52:CG52">
-    <cfRule type="expression" dxfId="44" priority="54">
+  <conditionalFormatting sqref="CA48:CG48">
+    <cfRule type="expression" dxfId="20" priority="54">
       <formula>AND(TODAY()&gt;=CA$5,TODAY()&lt;CB$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="CA52:CG52">
-    <cfRule type="expression" dxfId="43" priority="52">
+  <conditionalFormatting sqref="CA48:CG48">
+    <cfRule type="expression" dxfId="19" priority="52">
       <formula>AND(task_start&lt;=CA$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=CA$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="53" stopIfTrue="1">
+    <cfRule type="expression" dxfId="18" priority="53" stopIfTrue="1">
       <formula>AND(task_end&gt;=CA$5,task_start&lt;CB$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="CA53:CG53">
-    <cfRule type="expression" dxfId="41" priority="51">
-      <formula>AND(TODAY()&gt;=CA$5,TODAY()&lt;CB$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="CA53:CG53">
-    <cfRule type="expression" dxfId="40" priority="49">
-      <formula>AND(task_start&lt;=CA$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=CA$5)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="39" priority="50" stopIfTrue="1">
-      <formula>AND(task_end&gt;=CA$5,task_start&lt;CB$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="CA54:CG54">
-    <cfRule type="expression" dxfId="38" priority="48">
-      <formula>AND(TODAY()&gt;=CA$5,TODAY()&lt;CB$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="CA54:CG54">
-    <cfRule type="expression" dxfId="37" priority="46">
-      <formula>AND(task_start&lt;=CA$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=CA$5)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="36" priority="47" stopIfTrue="1">
-      <formula>AND(task_end&gt;=CA$5,task_start&lt;CB$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="CH51:CN51">
-    <cfRule type="expression" dxfId="35" priority="42">
+  <conditionalFormatting sqref="CH47:CN47">
+    <cfRule type="expression" dxfId="17" priority="42">
       <formula>AND(TODAY()&gt;=CH$5,TODAY()&lt;CI$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="CH51:CN51">
-    <cfRule type="expression" dxfId="34" priority="40">
+  <conditionalFormatting sqref="CH47:CN47">
+    <cfRule type="expression" dxfId="16" priority="40">
       <formula>AND(task_start&lt;=CH$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=CH$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="41" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="41" stopIfTrue="1">
       <formula>AND(task_end&gt;=CH$5,task_start&lt;CI$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="CH52:CN52">
-    <cfRule type="expression" dxfId="32" priority="39">
+  <conditionalFormatting sqref="CH48:CN48">
+    <cfRule type="expression" dxfId="14" priority="39">
       <formula>AND(TODAY()&gt;=CH$5,TODAY()&lt;CI$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="CH52:CN52">
-    <cfRule type="expression" dxfId="31" priority="37">
+  <conditionalFormatting sqref="CH48:CN48">
+    <cfRule type="expression" dxfId="13" priority="37">
       <formula>AND(task_start&lt;=CH$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=CH$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="38" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="38" stopIfTrue="1">
       <formula>AND(task_end&gt;=CH$5,task_start&lt;CI$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="CH53:CN53">
-    <cfRule type="expression" dxfId="29" priority="36">
-      <formula>AND(TODAY()&gt;=CH$5,TODAY()&lt;CI$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="CH53:CN53">
-    <cfRule type="expression" dxfId="28" priority="34">
-      <formula>AND(task_start&lt;=CH$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=CH$5)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="27" priority="35" stopIfTrue="1">
-      <formula>AND(task_end&gt;=CH$5,task_start&lt;CI$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="CH54:CN54">
-    <cfRule type="expression" dxfId="26" priority="33">
-      <formula>AND(TODAY()&gt;=CH$5,TODAY()&lt;CI$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="CH54:CN54">
-    <cfRule type="expression" dxfId="25" priority="31">
-      <formula>AND(task_start&lt;=CH$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=CH$5)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="24" priority="32" stopIfTrue="1">
-      <formula>AND(task_end&gt;=CH$5,task_start&lt;CI$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="CO51:CU51">
-    <cfRule type="expression" dxfId="23" priority="27">
+  <conditionalFormatting sqref="CO47:CU47">
+    <cfRule type="expression" dxfId="11" priority="27">
       <formula>AND(TODAY()&gt;=CO$5,TODAY()&lt;CP$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="CO51:CU51">
-    <cfRule type="expression" dxfId="22" priority="25">
+  <conditionalFormatting sqref="CO47:CU47">
+    <cfRule type="expression" dxfId="10" priority="25">
       <formula>AND(task_start&lt;=CO$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=CO$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="26" stopIfTrue="1">
       <formula>AND(task_end&gt;=CO$5,task_start&lt;CP$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="CO52:CU52">
-    <cfRule type="expression" dxfId="20" priority="24">
+  <conditionalFormatting sqref="CO48:CU48">
+    <cfRule type="expression" dxfId="8" priority="24">
       <formula>AND(TODAY()&gt;=CO$5,TODAY()&lt;CP$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="CO52:CU52">
-    <cfRule type="expression" dxfId="19" priority="22">
+  <conditionalFormatting sqref="CO48:CU48">
+    <cfRule type="expression" dxfId="7" priority="22">
       <formula>AND(task_start&lt;=CO$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=CO$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="23" stopIfTrue="1">
       <formula>AND(task_end&gt;=CO$5,task_start&lt;CP$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="CO53:CU53">
-    <cfRule type="expression" dxfId="17" priority="21">
-      <formula>AND(TODAY()&gt;=CO$5,TODAY()&lt;CP$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="CO53:CU53">
-    <cfRule type="expression" dxfId="16" priority="19">
-      <formula>AND(task_start&lt;=CO$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=CO$5)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="15" priority="20" stopIfTrue="1">
-      <formula>AND(task_end&gt;=CO$5,task_start&lt;CP$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="CO54:CU54">
-    <cfRule type="expression" dxfId="14" priority="18">
-      <formula>AND(TODAY()&gt;=CO$5,TODAY()&lt;CP$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="CO54:CU54">
-    <cfRule type="expression" dxfId="13" priority="16">
-      <formula>AND(task_start&lt;=CO$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=CO$5)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="12" priority="17" stopIfTrue="1">
-      <formula>AND(task_end&gt;=CO$5,task_start&lt;CP$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="CV51:DB51">
-    <cfRule type="expression" dxfId="11" priority="12">
+  <conditionalFormatting sqref="CV47:DB47">
+    <cfRule type="expression" dxfId="5" priority="12">
       <formula>AND(TODAY()&gt;=CV$5,TODAY()&lt;CW$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="CV51:DB51">
-    <cfRule type="expression" dxfId="10" priority="10">
+  <conditionalFormatting sqref="CV47:DB47">
+    <cfRule type="expression" dxfId="4" priority="10">
       <formula>AND(task_start&lt;=CV$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=CV$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="11" stopIfTrue="1">
       <formula>AND(task_end&gt;=CV$5,task_start&lt;CW$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="CV52:DB52">
-    <cfRule type="expression" dxfId="8" priority="9">
+  <conditionalFormatting sqref="CV48:DB48">
+    <cfRule type="expression" dxfId="2" priority="9">
       <formula>AND(TODAY()&gt;=CV$5,TODAY()&lt;CW$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="CV52:DB52">
-    <cfRule type="expression" dxfId="7" priority="7">
+  <conditionalFormatting sqref="CV48:DB48">
+    <cfRule type="expression" dxfId="1" priority="7">
       <formula>AND(task_start&lt;=CV$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=CV$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="8" stopIfTrue="1">
-      <formula>AND(task_end&gt;=CV$5,task_start&lt;CW$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="CV53:DB53">
-    <cfRule type="expression" dxfId="5" priority="6">
-      <formula>AND(TODAY()&gt;=CV$5,TODAY()&lt;CW$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="CV53:DB53">
-    <cfRule type="expression" dxfId="4" priority="4">
-      <formula>AND(task_start&lt;=CV$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=CV$5)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="3" priority="5" stopIfTrue="1">
-      <formula>AND(task_end&gt;=CV$5,task_start&lt;CW$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="CV54:DB54">
-    <cfRule type="expression" dxfId="2" priority="3">
-      <formula>AND(TODAY()&gt;=CV$5,TODAY()&lt;CW$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="CV54:DB54">
-    <cfRule type="expression" dxfId="1" priority="1">
-      <formula>AND(task_start&lt;=CV$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=CV$5)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="0" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="0" priority="8" stopIfTrue="1">
       <formula>AND(task_end&gt;=CV$5,task_start&lt;CW$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9574,22 +8282,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D7:D49</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{FFEC5DDB-C5BB-49AF-B8EA-B3E6AB9311C2}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="num">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>D50:D54</xm:sqref>
+          <xm:sqref>D7:D48</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
Backing up documentation for viewing on laptop
</commit_message>
<xml_diff>
--- a/docs/Gantt Chart.xlsx
+++ b/docs/Gantt Chart.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE1547AC-1989-4AFF-9B79-822DAF8B08E6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9553CF76-626D-4783-BDC0-E80751E87443}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="78">
   <si>
     <t>PROGRESS</t>
   </si>
@@ -221,9 +221,6 @@
     <t>Wireless Communication</t>
   </si>
   <si>
-    <t xml:space="preserve">        Build "stretch" sensors and measure min/max resistances</t>
-  </si>
-  <si>
     <t xml:space="preserve">        SW to read data from each joint's sensor</t>
   </si>
   <si>
@@ -266,9 +263,6 @@
     <t xml:space="preserve">        Part placement &amp; order from JLCPCB</t>
   </si>
   <si>
-    <t>Presentation</t>
-  </si>
-  <si>
     <t>First PCB assembly &amp; Debugging</t>
   </si>
   <si>
@@ -276,9 +270,6 @@
   </si>
   <si>
     <t>Second PCB assembly &amp; Debugging</t>
-  </si>
-  <si>
-    <t>Li-ion Battery Charger - Circuit design</t>
   </si>
   <si>
     <t xml:space="preserve">        Build voltage divider / mux circuits for each joint sensor (proto with potentiometers)</t>
@@ -302,9 +293,6 @@
     <t>Extra time if tasks took longer than expected. Otherwise, stretch goal SW development goes here.</t>
   </si>
   <si>
-    <t>Hand Movement Software - Modify Bluetooth message protocol, add accelerometer data, make simple demo</t>
-  </si>
-  <si>
     <t>Finger spread detection sensors</t>
   </si>
   <si>
@@ -315,6 +303,15 @@
   </si>
   <si>
     <t xml:space="preserve">        Voltage amplifier + AB Amplifier</t>
+  </si>
+  <si>
+    <t>Li-ion Battery Charger - CCCV research, circuit design</t>
+  </si>
+  <si>
+    <t>Hand Movement Software - Modify Bluetooth message protocol, process accelerometer data, make new demo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Build "flex" sensors and measure min/max resistances</t>
   </si>
 </sst>
 </file>
@@ -465,7 +462,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="17">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -547,18 +544,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -714,7 +699,7 @@
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -907,9 +892,6 @@
     <xf numFmtId="164" fontId="6" fillId="14" borderId="2" xfId="10" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -934,16 +916,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyProtection="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="3" xfId="9">
@@ -1945,11 +1918,11 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:DB48"/>
+  <dimension ref="A1:DB47"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="BV13" sqref="BV13"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O24" sqref="O24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1986,7 +1959,7 @@
         <v>20</v>
       </c>
       <c r="C2" s="50"/>
-      <c r="I2" s="76" t="s">
+      <c r="I2" s="75" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1998,11 +1971,11 @@
         <v>36</v>
       </c>
       <c r="D3" s="60"/>
-      <c r="E3" s="81">
+      <c r="E3" s="77">
         <f ca="1">TODAY()</f>
-        <v>44225</v>
-      </c>
-      <c r="F3" s="81"/>
+        <v>44230</v>
+      </c>
+      <c r="F3" s="77"/>
     </row>
     <row r="4" spans="1:106" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="48" t="s">
@@ -2013,555 +1986,555 @@
       <c r="E4" s="5">
         <v>0</v>
       </c>
-      <c r="I4" s="82">
+      <c r="I4" s="78">
         <f ca="1">I5</f>
-        <v>44214</v>
-      </c>
-      <c r="J4" s="83"/>
-      <c r="K4" s="83"/>
-      <c r="L4" s="83"/>
-      <c r="M4" s="83"/>
-      <c r="N4" s="83"/>
-      <c r="O4" s="84"/>
-      <c r="P4" s="82">
+        <v>44221</v>
+      </c>
+      <c r="J4" s="79"/>
+      <c r="K4" s="79"/>
+      <c r="L4" s="79"/>
+      <c r="M4" s="79"/>
+      <c r="N4" s="79"/>
+      <c r="O4" s="80"/>
+      <c r="P4" s="78">
         <f ca="1">P5</f>
-        <v>44221</v>
-      </c>
-      <c r="Q4" s="83"/>
-      <c r="R4" s="83"/>
-      <c r="S4" s="83"/>
-      <c r="T4" s="83"/>
-      <c r="U4" s="83"/>
-      <c r="V4" s="84"/>
-      <c r="W4" s="82">
+        <v>44228</v>
+      </c>
+      <c r="Q4" s="79"/>
+      <c r="R4" s="79"/>
+      <c r="S4" s="79"/>
+      <c r="T4" s="79"/>
+      <c r="U4" s="79"/>
+      <c r="V4" s="80"/>
+      <c r="W4" s="78">
         <f ca="1">W5</f>
-        <v>44228</v>
-      </c>
-      <c r="X4" s="83"/>
-      <c r="Y4" s="83"/>
-      <c r="Z4" s="83"/>
-      <c r="AA4" s="83"/>
-      <c r="AB4" s="83"/>
-      <c r="AC4" s="84"/>
-      <c r="AD4" s="82">
+        <v>44235</v>
+      </c>
+      <c r="X4" s="79"/>
+      <c r="Y4" s="79"/>
+      <c r="Z4" s="79"/>
+      <c r="AA4" s="79"/>
+      <c r="AB4" s="79"/>
+      <c r="AC4" s="80"/>
+      <c r="AD4" s="78">
         <f ca="1">AD5</f>
-        <v>44235</v>
-      </c>
-      <c r="AE4" s="83"/>
-      <c r="AF4" s="83"/>
-      <c r="AG4" s="83"/>
-      <c r="AH4" s="83"/>
-      <c r="AI4" s="83"/>
-      <c r="AJ4" s="84"/>
-      <c r="AK4" s="82">
+        <v>44242</v>
+      </c>
+      <c r="AE4" s="79"/>
+      <c r="AF4" s="79"/>
+      <c r="AG4" s="79"/>
+      <c r="AH4" s="79"/>
+      <c r="AI4" s="79"/>
+      <c r="AJ4" s="80"/>
+      <c r="AK4" s="78">
         <f ca="1">AK5</f>
-        <v>44242</v>
-      </c>
-      <c r="AL4" s="83"/>
-      <c r="AM4" s="83"/>
-      <c r="AN4" s="83"/>
-      <c r="AO4" s="83"/>
-      <c r="AP4" s="83"/>
-      <c r="AQ4" s="84"/>
-      <c r="AR4" s="82">
+        <v>44249</v>
+      </c>
+      <c r="AL4" s="79"/>
+      <c r="AM4" s="79"/>
+      <c r="AN4" s="79"/>
+      <c r="AO4" s="79"/>
+      <c r="AP4" s="79"/>
+      <c r="AQ4" s="80"/>
+      <c r="AR4" s="78">
         <f ca="1">AR5</f>
-        <v>44249</v>
-      </c>
-      <c r="AS4" s="83"/>
-      <c r="AT4" s="83"/>
-      <c r="AU4" s="83"/>
-      <c r="AV4" s="83"/>
-      <c r="AW4" s="83"/>
-      <c r="AX4" s="84"/>
-      <c r="AY4" s="82">
+        <v>44256</v>
+      </c>
+      <c r="AS4" s="79"/>
+      <c r="AT4" s="79"/>
+      <c r="AU4" s="79"/>
+      <c r="AV4" s="79"/>
+      <c r="AW4" s="79"/>
+      <c r="AX4" s="80"/>
+      <c r="AY4" s="78">
         <f ca="1">AY5</f>
-        <v>44256</v>
-      </c>
-      <c r="AZ4" s="83"/>
-      <c r="BA4" s="83"/>
-      <c r="BB4" s="83"/>
-      <c r="BC4" s="83"/>
-      <c r="BD4" s="83"/>
-      <c r="BE4" s="84"/>
-      <c r="BF4" s="82">
+        <v>44263</v>
+      </c>
+      <c r="AZ4" s="79"/>
+      <c r="BA4" s="79"/>
+      <c r="BB4" s="79"/>
+      <c r="BC4" s="79"/>
+      <c r="BD4" s="79"/>
+      <c r="BE4" s="80"/>
+      <c r="BF4" s="78">
         <f ca="1">BF5</f>
-        <v>44263</v>
-      </c>
-      <c r="BG4" s="83"/>
-      <c r="BH4" s="83"/>
-      <c r="BI4" s="83"/>
-      <c r="BJ4" s="83"/>
-      <c r="BK4" s="83"/>
-      <c r="BL4" s="84"/>
-      <c r="BM4" s="82">
+        <v>44270</v>
+      </c>
+      <c r="BG4" s="79"/>
+      <c r="BH4" s="79"/>
+      <c r="BI4" s="79"/>
+      <c r="BJ4" s="79"/>
+      <c r="BK4" s="79"/>
+      <c r="BL4" s="80"/>
+      <c r="BM4" s="78">
         <f ca="1">BM5</f>
-        <v>44270</v>
-      </c>
-      <c r="BN4" s="83"/>
-      <c r="BO4" s="83"/>
-      <c r="BP4" s="83"/>
-      <c r="BQ4" s="83"/>
-      <c r="BR4" s="83"/>
-      <c r="BS4" s="84"/>
-      <c r="BT4" s="82">
+        <v>44277</v>
+      </c>
+      <c r="BN4" s="79"/>
+      <c r="BO4" s="79"/>
+      <c r="BP4" s="79"/>
+      <c r="BQ4" s="79"/>
+      <c r="BR4" s="79"/>
+      <c r="BS4" s="80"/>
+      <c r="BT4" s="78">
         <f ca="1">BT5</f>
-        <v>44277</v>
-      </c>
-      <c r="BU4" s="83"/>
-      <c r="BV4" s="83"/>
-      <c r="BW4" s="83"/>
-      <c r="BX4" s="83"/>
-      <c r="BY4" s="83"/>
-      <c r="BZ4" s="84"/>
-      <c r="CA4" s="82">
+        <v>44284</v>
+      </c>
+      <c r="BU4" s="79"/>
+      <c r="BV4" s="79"/>
+      <c r="BW4" s="79"/>
+      <c r="BX4" s="79"/>
+      <c r="BY4" s="79"/>
+      <c r="BZ4" s="80"/>
+      <c r="CA4" s="78">
         <f ca="1">CA5</f>
-        <v>44284</v>
-      </c>
-      <c r="CB4" s="83"/>
-      <c r="CC4" s="83"/>
-      <c r="CD4" s="83"/>
-      <c r="CE4" s="83"/>
-      <c r="CF4" s="83"/>
-      <c r="CG4" s="84"/>
-      <c r="CH4" s="82">
+        <v>44291</v>
+      </c>
+      <c r="CB4" s="79"/>
+      <c r="CC4" s="79"/>
+      <c r="CD4" s="79"/>
+      <c r="CE4" s="79"/>
+      <c r="CF4" s="79"/>
+      <c r="CG4" s="80"/>
+      <c r="CH4" s="78">
         <f ca="1">CH5</f>
-        <v>44291</v>
-      </c>
-      <c r="CI4" s="83"/>
-      <c r="CJ4" s="83"/>
-      <c r="CK4" s="83"/>
-      <c r="CL4" s="83"/>
-      <c r="CM4" s="83"/>
-      <c r="CN4" s="84"/>
-      <c r="CO4" s="82">
+        <v>44298</v>
+      </c>
+      <c r="CI4" s="79"/>
+      <c r="CJ4" s="79"/>
+      <c r="CK4" s="79"/>
+      <c r="CL4" s="79"/>
+      <c r="CM4" s="79"/>
+      <c r="CN4" s="80"/>
+      <c r="CO4" s="78">
         <f ca="1">CO5</f>
-        <v>44298</v>
-      </c>
-      <c r="CP4" s="83"/>
-      <c r="CQ4" s="83"/>
-      <c r="CR4" s="83"/>
-      <c r="CS4" s="83"/>
-      <c r="CT4" s="83"/>
-      <c r="CU4" s="84"/>
-      <c r="CV4" s="82">
+        <v>44305</v>
+      </c>
+      <c r="CP4" s="79"/>
+      <c r="CQ4" s="79"/>
+      <c r="CR4" s="79"/>
+      <c r="CS4" s="79"/>
+      <c r="CT4" s="79"/>
+      <c r="CU4" s="80"/>
+      <c r="CV4" s="78">
         <f ca="1">CV5</f>
-        <v>44305</v>
-      </c>
-      <c r="CW4" s="83"/>
-      <c r="CX4" s="83"/>
-      <c r="CY4" s="83"/>
-      <c r="CZ4" s="83"/>
-      <c r="DA4" s="83"/>
-      <c r="DB4" s="84"/>
+        <v>44312</v>
+      </c>
+      <c r="CW4" s="79"/>
+      <c r="CX4" s="79"/>
+      <c r="CY4" s="79"/>
+      <c r="CZ4" s="79"/>
+      <c r="DA4" s="79"/>
+      <c r="DB4" s="80"/>
     </row>
     <row r="5" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="48" t="s">
         <v>28</v>
       </c>
       <c r="B5" s="48"/>
-      <c r="C5" s="85"/>
-      <c r="D5" s="85"/>
-      <c r="E5" s="85"/>
-      <c r="F5" s="85"/>
-      <c r="G5" s="85"/>
+      <c r="C5" s="81"/>
+      <c r="D5" s="81"/>
+      <c r="E5" s="81"/>
+      <c r="F5" s="81"/>
+      <c r="G5" s="81"/>
       <c r="I5" s="9">
         <f ca="1">Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
-        <v>44214</v>
+        <v>44221</v>
       </c>
       <c r="J5" s="8">
         <f ca="1">I5+1</f>
-        <v>44215</v>
+        <v>44222</v>
       </c>
       <c r="K5" s="8">
         <f t="shared" ref="K5:AX5" ca="1" si="0">J5+1</f>
-        <v>44216</v>
+        <v>44223</v>
       </c>
       <c r="L5" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>44217</v>
+        <v>44224</v>
       </c>
       <c r="M5" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>44218</v>
+        <v>44225</v>
       </c>
       <c r="N5" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>44219</v>
+        <v>44226</v>
       </c>
       <c r="O5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44220</v>
+        <v>44227</v>
       </c>
       <c r="P5" s="9">
         <f ca="1">O5+1</f>
-        <v>44221</v>
+        <v>44228</v>
       </c>
       <c r="Q5" s="8">
         <f ca="1">P5+1</f>
-        <v>44222</v>
+        <v>44229</v>
       </c>
       <c r="R5" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>44223</v>
+        <v>44230</v>
       </c>
       <c r="S5" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>44224</v>
+        <v>44231</v>
       </c>
       <c r="T5" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>44225</v>
+        <v>44232</v>
       </c>
       <c r="U5" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>44226</v>
+        <v>44233</v>
       </c>
       <c r="V5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44227</v>
+        <v>44234</v>
       </c>
       <c r="W5" s="9">
         <f ca="1">V5+1</f>
-        <v>44228</v>
+        <v>44235</v>
       </c>
       <c r="X5" s="8">
         <f ca="1">W5+1</f>
-        <v>44229</v>
+        <v>44236</v>
       </c>
       <c r="Y5" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>44230</v>
+        <v>44237</v>
       </c>
       <c r="Z5" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>44231</v>
+        <v>44238</v>
       </c>
       <c r="AA5" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>44232</v>
+        <v>44239</v>
       </c>
       <c r="AB5" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>44233</v>
+        <v>44240</v>
       </c>
       <c r="AC5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44234</v>
+        <v>44241</v>
       </c>
       <c r="AD5" s="9">
         <f ca="1">AC5+1</f>
-        <v>44235</v>
+        <v>44242</v>
       </c>
       <c r="AE5" s="8">
         <f ca="1">AD5+1</f>
-        <v>44236</v>
+        <v>44243</v>
       </c>
       <c r="AF5" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>44237</v>
+        <v>44244</v>
       </c>
       <c r="AG5" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>44238</v>
+        <v>44245</v>
       </c>
       <c r="AH5" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>44239</v>
+        <v>44246</v>
       </c>
       <c r="AI5" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>44240</v>
+        <v>44247</v>
       </c>
       <c r="AJ5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44241</v>
+        <v>44248</v>
       </c>
       <c r="AK5" s="9">
         <f ca="1">AJ5+1</f>
-        <v>44242</v>
+        <v>44249</v>
       </c>
       <c r="AL5" s="8">
         <f ca="1">AK5+1</f>
-        <v>44243</v>
+        <v>44250</v>
       </c>
       <c r="AM5" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>44244</v>
+        <v>44251</v>
       </c>
       <c r="AN5" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>44245</v>
+        <v>44252</v>
       </c>
       <c r="AO5" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>44246</v>
+        <v>44253</v>
       </c>
       <c r="AP5" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>44247</v>
+        <v>44254</v>
       </c>
       <c r="AQ5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44248</v>
+        <v>44255</v>
       </c>
       <c r="AR5" s="9">
         <f ca="1">AQ5+1</f>
-        <v>44249</v>
+        <v>44256</v>
       </c>
       <c r="AS5" s="8">
         <f ca="1">AR5+1</f>
-        <v>44250</v>
+        <v>44257</v>
       </c>
       <c r="AT5" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>44251</v>
+        <v>44258</v>
       </c>
       <c r="AU5" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>44252</v>
+        <v>44259</v>
       </c>
       <c r="AV5" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>44253</v>
+        <v>44260</v>
       </c>
       <c r="AW5" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>44254</v>
+        <v>44261</v>
       </c>
       <c r="AX5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44255</v>
+        <v>44262</v>
       </c>
       <c r="AY5" s="9">
         <f ca="1">AX5+1</f>
-        <v>44256</v>
+        <v>44263</v>
       </c>
       <c r="AZ5" s="8">
         <f ca="1">AY5+1</f>
-        <v>44257</v>
+        <v>44264</v>
       </c>
       <c r="BA5" s="8">
         <f t="shared" ref="BA5:BE5" ca="1" si="1">AZ5+1</f>
-        <v>44258</v>
+        <v>44265</v>
       </c>
       <c r="BB5" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>44259</v>
+        <v>44266</v>
       </c>
       <c r="BC5" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>44260</v>
+        <v>44267</v>
       </c>
       <c r="BD5" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>44261</v>
+        <v>44268</v>
       </c>
       <c r="BE5" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>44262</v>
+        <v>44269</v>
       </c>
       <c r="BF5" s="9">
         <f ca="1">BE5+1</f>
-        <v>44263</v>
+        <v>44270</v>
       </c>
       <c r="BG5" s="8">
         <f ca="1">BF5+1</f>
-        <v>44264</v>
+        <v>44271</v>
       </c>
       <c r="BH5" s="8">
         <f t="shared" ref="BH5:BL5" ca="1" si="2">BG5+1</f>
-        <v>44265</v>
+        <v>44272</v>
       </c>
       <c r="BI5" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>44266</v>
+        <v>44273</v>
       </c>
       <c r="BJ5" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>44267</v>
+        <v>44274</v>
       </c>
       <c r="BK5" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>44268</v>
+        <v>44275</v>
       </c>
       <c r="BL5" s="10">
         <f t="shared" ca="1" si="2"/>
-        <v>44269</v>
+        <v>44276</v>
       </c>
       <c r="BM5" s="9">
         <f ca="1">BL5+1</f>
-        <v>44270</v>
+        <v>44277</v>
       </c>
       <c r="BN5" s="8">
         <f ca="1">BM5+1</f>
-        <v>44271</v>
+        <v>44278</v>
       </c>
       <c r="BO5" s="8">
         <f t="shared" ref="BO5" ca="1" si="3">BN5+1</f>
-        <v>44272</v>
+        <v>44279</v>
       </c>
       <c r="BP5" s="8">
         <f t="shared" ref="BP5" ca="1" si="4">BO5+1</f>
-        <v>44273</v>
+        <v>44280</v>
       </c>
       <c r="BQ5" s="8">
         <f t="shared" ref="BQ5" ca="1" si="5">BP5+1</f>
-        <v>44274</v>
+        <v>44281</v>
       </c>
       <c r="BR5" s="8">
         <f t="shared" ref="BR5" ca="1" si="6">BQ5+1</f>
-        <v>44275</v>
+        <v>44282</v>
       </c>
       <c r="BS5" s="10">
         <f t="shared" ref="BS5" ca="1" si="7">BR5+1</f>
-        <v>44276</v>
+        <v>44283</v>
       </c>
       <c r="BT5" s="9">
         <f ca="1">BS5+1</f>
-        <v>44277</v>
+        <v>44284</v>
       </c>
       <c r="BU5" s="8">
         <f ca="1">BT5+1</f>
-        <v>44278</v>
+        <v>44285</v>
       </c>
       <c r="BV5" s="8">
         <f t="shared" ref="BV5" ca="1" si="8">BU5+1</f>
-        <v>44279</v>
+        <v>44286</v>
       </c>
       <c r="BW5" s="8">
         <f t="shared" ref="BW5" ca="1" si="9">BV5+1</f>
-        <v>44280</v>
+        <v>44287</v>
       </c>
       <c r="BX5" s="8">
         <f t="shared" ref="BX5" ca="1" si="10">BW5+1</f>
-        <v>44281</v>
+        <v>44288</v>
       </c>
       <c r="BY5" s="8">
         <f t="shared" ref="BY5" ca="1" si="11">BX5+1</f>
-        <v>44282</v>
+        <v>44289</v>
       </c>
       <c r="BZ5" s="10">
         <f t="shared" ref="BZ5" ca="1" si="12">BY5+1</f>
-        <v>44283</v>
+        <v>44290</v>
       </c>
       <c r="CA5" s="9">
         <f ca="1">BZ5+1</f>
-        <v>44284</v>
+        <v>44291</v>
       </c>
       <c r="CB5" s="8">
         <f ca="1">CA5+1</f>
-        <v>44285</v>
+        <v>44292</v>
       </c>
       <c r="CC5" s="8">
         <f t="shared" ref="CC5" ca="1" si="13">CB5+1</f>
-        <v>44286</v>
+        <v>44293</v>
       </c>
       <c r="CD5" s="8">
         <f t="shared" ref="CD5" ca="1" si="14">CC5+1</f>
-        <v>44287</v>
+        <v>44294</v>
       </c>
       <c r="CE5" s="8">
         <f t="shared" ref="CE5" ca="1" si="15">CD5+1</f>
-        <v>44288</v>
+        <v>44295</v>
       </c>
       <c r="CF5" s="8">
         <f t="shared" ref="CF5" ca="1" si="16">CE5+1</f>
-        <v>44289</v>
+        <v>44296</v>
       </c>
       <c r="CG5" s="10">
         <f t="shared" ref="CG5" ca="1" si="17">CF5+1</f>
-        <v>44290</v>
+        <v>44297</v>
       </c>
       <c r="CH5" s="9">
         <f ca="1">CG5+1</f>
-        <v>44291</v>
+        <v>44298</v>
       </c>
       <c r="CI5" s="8">
         <f ca="1">CH5+1</f>
-        <v>44292</v>
+        <v>44299</v>
       </c>
       <c r="CJ5" s="8">
         <f t="shared" ref="CJ5" ca="1" si="18">CI5+1</f>
-        <v>44293</v>
+        <v>44300</v>
       </c>
       <c r="CK5" s="8">
         <f t="shared" ref="CK5" ca="1" si="19">CJ5+1</f>
-        <v>44294</v>
+        <v>44301</v>
       </c>
       <c r="CL5" s="8">
         <f t="shared" ref="CL5" ca="1" si="20">CK5+1</f>
-        <v>44295</v>
+        <v>44302</v>
       </c>
       <c r="CM5" s="8">
         <f t="shared" ref="CM5" ca="1" si="21">CL5+1</f>
-        <v>44296</v>
+        <v>44303</v>
       </c>
       <c r="CN5" s="10">
         <f t="shared" ref="CN5" ca="1" si="22">CM5+1</f>
-        <v>44297</v>
+        <v>44304</v>
       </c>
       <c r="CO5" s="9">
         <f ca="1">CN5+1</f>
-        <v>44298</v>
+        <v>44305</v>
       </c>
       <c r="CP5" s="8">
         <f ca="1">CO5+1</f>
-        <v>44299</v>
+        <v>44306</v>
       </c>
       <c r="CQ5" s="8">
         <f t="shared" ref="CQ5" ca="1" si="23">CP5+1</f>
-        <v>44300</v>
+        <v>44307</v>
       </c>
       <c r="CR5" s="8">
         <f t="shared" ref="CR5" ca="1" si="24">CQ5+1</f>
-        <v>44301</v>
+        <v>44308</v>
       </c>
       <c r="CS5" s="8">
         <f t="shared" ref="CS5" ca="1" si="25">CR5+1</f>
-        <v>44302</v>
+        <v>44309</v>
       </c>
       <c r="CT5" s="8">
         <f t="shared" ref="CT5" ca="1" si="26">CS5+1</f>
-        <v>44303</v>
+        <v>44310</v>
       </c>
       <c r="CU5" s="10">
         <f t="shared" ref="CU5" ca="1" si="27">CT5+1</f>
-        <v>44304</v>
+        <v>44311</v>
       </c>
       <c r="CV5" s="9">
         <f ca="1">CU5+1</f>
-        <v>44305</v>
+        <v>44312</v>
       </c>
       <c r="CW5" s="8">
         <f ca="1">CV5+1</f>
-        <v>44306</v>
+        <v>44313</v>
       </c>
       <c r="CX5" s="8">
         <f t="shared" ref="CX5" ca="1" si="28">CW5+1</f>
-        <v>44307</v>
+        <v>44314</v>
       </c>
       <c r="CY5" s="8">
         <f t="shared" ref="CY5" ca="1" si="29">CX5+1</f>
-        <v>44308</v>
+        <v>44315</v>
       </c>
       <c r="CZ5" s="8">
         <f t="shared" ref="CZ5" ca="1" si="30">CY5+1</f>
-        <v>44309</v>
+        <v>44316</v>
       </c>
       <c r="DA5" s="8">
         <f t="shared" ref="DA5" ca="1" si="31">CZ5+1</f>
-        <v>44310</v>
+        <v>44317</v>
       </c>
       <c r="DB5" s="10">
         <f t="shared" ref="DB5" ca="1" si="32">DA5+1</f>
-        <v>44311</v>
+        <v>44318</v>
       </c>
     </row>
     <row r="6" spans="1:106" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="48" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="69" t="s">
+      <c r="B6" s="68" t="s">
         <v>43</v>
       </c>
       <c r="C6" s="6" t="s">
@@ -3096,7 +3069,7 @@
       <c r="F8" s="17"/>
       <c r="G8" s="13"/>
       <c r="H8" s="13" t="str">
-        <f t="shared" ref="H8:H48" si="37">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <f t="shared" ref="H8:H47" si="37">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v/>
       </c>
       <c r="I8" s="34"/>
@@ -3104,17 +3077,17 @@
       <c r="K8" s="34"/>
       <c r="L8" s="34"/>
       <c r="M8" s="34"/>
-      <c r="N8" s="68"/>
-      <c r="O8" s="68"/>
-      <c r="P8" s="68"/>
-      <c r="Q8" s="68"/>
-      <c r="R8" s="68"/>
-      <c r="S8" s="68"/>
-      <c r="T8" s="68"/>
-      <c r="U8" s="68"/>
-      <c r="V8" s="34"/>
-      <c r="W8" s="34"/>
-      <c r="X8" s="34"/>
+      <c r="N8" s="76"/>
+      <c r="O8" s="76"/>
+      <c r="P8" s="76"/>
+      <c r="Q8" s="76"/>
+      <c r="R8" s="76"/>
+      <c r="S8" s="76"/>
+      <c r="T8" s="76"/>
+      <c r="U8" s="76"/>
+      <c r="V8" s="76"/>
+      <c r="W8" s="76"/>
+      <c r="X8" s="76"/>
       <c r="Y8" s="34"/>
       <c r="Z8" s="34"/>
       <c r="AA8" s="34"/>
@@ -3202,11 +3175,11 @@
       <c r="A9" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="71">
+      <c r="B9" s="70">
         <v>1.1000000000000001</v>
       </c>
       <c r="C9" s="56" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="D9" s="18">
         <v>0.75</v>
@@ -3325,14 +3298,14 @@
       <c r="A10" s="48" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="71">
+      <c r="B10" s="70">
         <v>1.2</v>
       </c>
       <c r="C10" s="56" t="s">
         <v>40</v>
       </c>
       <c r="D10" s="18">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="E10" s="52">
         <f>F9</f>
@@ -3448,7 +3421,7 @@
     </row>
     <row r="11" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="47"/>
-      <c r="B11" s="71">
+      <c r="B11" s="70">
         <v>1.3</v>
       </c>
       <c r="C11" s="56" t="s">
@@ -3567,28 +3540,25 @@
       <c r="DA11" s="34"/>
       <c r="DB11" s="34"/>
     </row>
-    <row r="12" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="47"/>
-      <c r="B12" s="71">
+    <row r="12" spans="1:106" s="2" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="48"/>
+      <c r="B12" s="70">
         <v>1.4</v>
       </c>
       <c r="C12" s="56" t="s">
-        <v>62</v>
+        <v>42</v>
       </c>
       <c r="D12" s="18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12" s="52">
-        <v>44223</v>
+        <v>44224</v>
       </c>
       <c r="F12" s="52">
-        <v>44223</v>
+        <v>44224</v>
       </c>
       <c r="G12" s="13"/>
-      <c r="H12" s="13">
-        <f t="shared" si="37"/>
-        <v>1</v>
-      </c>
+      <c r="H12" s="13"/>
       <c r="I12" s="34"/>
       <c r="J12" s="34"/>
       <c r="K12" s="34"/>
@@ -3601,8 +3571,8 @@
       <c r="R12" s="34"/>
       <c r="S12" s="34"/>
       <c r="T12" s="34"/>
-      <c r="U12" s="34"/>
-      <c r="V12" s="34"/>
+      <c r="U12" s="35"/>
+      <c r="V12" s="35"/>
       <c r="W12" s="34"/>
       <c r="X12" s="34"/>
       <c r="Y12" s="34"/>
@@ -3690,20 +3660,20 @@
     </row>
     <row r="13" spans="1:106" s="2" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="48"/>
-      <c r="B13" s="71">
+      <c r="B13" s="70">
         <v>1.5</v>
       </c>
       <c r="C13" s="56" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D13" s="18">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E13" s="52">
-        <v>44224</v>
+        <v>44226</v>
       </c>
       <c r="F13" s="52">
-        <v>44224</v>
+        <v>44226</v>
       </c>
       <c r="G13" s="13"/>
       <c r="H13" s="13"/>
@@ -3806,19 +3776,19 @@
       <c r="DA13" s="34"/>
       <c r="DB13" s="34"/>
     </row>
-    <row r="14" spans="1:106" s="2" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="48"/>
-      <c r="B14" s="71">
+    <row r="14" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="47"/>
+      <c r="B14" s="70">
         <v>1.6</v>
       </c>
       <c r="C14" s="56" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="D14" s="18">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="E14" s="52">
-        <v>44226</v>
+        <v>44220</v>
       </c>
       <c r="F14" s="52">
         <v>44226</v>
@@ -3837,11 +3807,11 @@
       <c r="R14" s="34"/>
       <c r="S14" s="34"/>
       <c r="T14" s="34"/>
-      <c r="U14" s="35"/>
-      <c r="V14" s="35"/>
+      <c r="U14" s="34"/>
+      <c r="V14" s="34"/>
       <c r="W14" s="34"/>
       <c r="X14" s="34"/>
-      <c r="Y14" s="34"/>
+      <c r="Y14" s="35"/>
       <c r="Z14" s="34"/>
       <c r="AA14" s="34"/>
       <c r="AB14" s="34"/>
@@ -3925,24 +3895,23 @@
       <c r="DB14" s="34"/>
     </row>
     <row r="15" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="47"/>
-      <c r="B15" s="71">
-        <v>1.7</v>
-      </c>
-      <c r="C15" s="56" t="s">
-        <v>45</v>
-      </c>
-      <c r="D15" s="18">
-        <v>0.5</v>
-      </c>
-      <c r="E15" s="52">
-        <v>44220</v>
-      </c>
-      <c r="F15" s="52">
-        <v>44226</v>
-      </c>
+      <c r="A15" s="48" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="19">
+        <v>2</v>
+      </c>
+      <c r="C15" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" s="20"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="22"/>
       <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
+      <c r="H15" s="13" t="str">
+        <f t="shared" si="37"/>
+        <v/>
+      </c>
       <c r="I15" s="34"/>
       <c r="J15" s="34"/>
       <c r="K15" s="34"/>
@@ -3953,43 +3922,43 @@
       <c r="P15" s="34"/>
       <c r="Q15" s="34"/>
       <c r="R15" s="34"/>
-      <c r="S15" s="34"/>
-      <c r="T15" s="34"/>
-      <c r="U15" s="34"/>
-      <c r="V15" s="34"/>
-      <c r="W15" s="34"/>
-      <c r="X15" s="34"/>
-      <c r="Y15" s="35"/>
-      <c r="Z15" s="34"/>
-      <c r="AA15" s="34"/>
-      <c r="AB15" s="34"/>
-      <c r="AC15" s="34"/>
-      <c r="AD15" s="34"/>
-      <c r="AE15" s="34"/>
-      <c r="AF15" s="34"/>
-      <c r="AG15" s="34"/>
-      <c r="AH15" s="34"/>
-      <c r="AI15" s="34"/>
-      <c r="AJ15" s="34"/>
-      <c r="AK15" s="34"/>
-      <c r="AL15" s="34"/>
-      <c r="AM15" s="34"/>
-      <c r="AN15" s="34"/>
-      <c r="AO15" s="34"/>
-      <c r="AP15" s="34"/>
-      <c r="AQ15" s="34"/>
-      <c r="AR15" s="34"/>
-      <c r="AS15" s="34"/>
-      <c r="AT15" s="34"/>
-      <c r="AU15" s="34"/>
-      <c r="AV15" s="34"/>
-      <c r="AW15" s="34"/>
-      <c r="AX15" s="34"/>
-      <c r="AY15" s="34"/>
-      <c r="AZ15" s="34"/>
-      <c r="BA15" s="34"/>
-      <c r="BB15" s="34"/>
-      <c r="BC15" s="34"/>
+      <c r="S15" s="76"/>
+      <c r="T15" s="76"/>
+      <c r="U15" s="76"/>
+      <c r="V15" s="76"/>
+      <c r="W15" s="76"/>
+      <c r="X15" s="76"/>
+      <c r="Y15" s="76"/>
+      <c r="Z15" s="76"/>
+      <c r="AA15" s="76"/>
+      <c r="AB15" s="76"/>
+      <c r="AC15" s="76"/>
+      <c r="AD15" s="76"/>
+      <c r="AE15" s="76"/>
+      <c r="AF15" s="76"/>
+      <c r="AG15" s="76"/>
+      <c r="AH15" s="76"/>
+      <c r="AI15" s="76"/>
+      <c r="AJ15" s="76"/>
+      <c r="AK15" s="76"/>
+      <c r="AL15" s="76"/>
+      <c r="AM15" s="76"/>
+      <c r="AN15" s="76"/>
+      <c r="AO15" s="76"/>
+      <c r="AP15" s="76"/>
+      <c r="AQ15" s="76"/>
+      <c r="AR15" s="76"/>
+      <c r="AS15" s="76"/>
+      <c r="AT15" s="76"/>
+      <c r="AU15" s="76"/>
+      <c r="AV15" s="76"/>
+      <c r="AW15" s="76"/>
+      <c r="AX15" s="76"/>
+      <c r="AY15" s="76"/>
+      <c r="AZ15" s="76"/>
+      <c r="BA15" s="76"/>
+      <c r="BB15" s="76"/>
+      <c r="BC15" s="76"/>
       <c r="BD15" s="34"/>
       <c r="BE15" s="34"/>
       <c r="BF15" s="34"/>
@@ -4043,23 +4012,26 @@
       <c r="DB15" s="34"/>
     </row>
     <row r="16" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="48" t="s">
-        <v>33</v>
-      </c>
-      <c r="B16" s="19">
-        <v>2</v>
-      </c>
-      <c r="C16" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="D16" s="20"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="22"/>
+      <c r="A16" s="47"/>
+      <c r="B16" s="69">
+        <v>2.1</v>
+      </c>
+      <c r="C16" s="71" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" s="23">
+        <v>0</v>
+      </c>
+      <c r="E16" s="53">
+        <f>F14+1</f>
+        <v>44227</v>
+      </c>
+      <c r="F16" s="53">
+        <f>E16+4</f>
+        <v>44231</v>
+      </c>
       <c r="G16" s="13"/>
-      <c r="H16" s="13" t="str">
-        <f t="shared" si="37"/>
-        <v/>
-      </c>
+      <c r="H16" s="13"/>
       <c r="I16" s="34"/>
       <c r="J16" s="34"/>
       <c r="K16" s="34"/>
@@ -4070,40 +4042,40 @@
       <c r="P16" s="34"/>
       <c r="Q16" s="34"/>
       <c r="R16" s="34"/>
-      <c r="S16" s="80"/>
-      <c r="T16" s="80"/>
-      <c r="U16" s="80"/>
-      <c r="V16" s="77"/>
-      <c r="W16" s="77"/>
-      <c r="X16" s="77"/>
-      <c r="Y16" s="77"/>
-      <c r="Z16" s="77"/>
-      <c r="AA16" s="77"/>
-      <c r="AB16" s="77"/>
-      <c r="AC16" s="77"/>
-      <c r="AD16" s="77"/>
-      <c r="AE16" s="77"/>
-      <c r="AF16" s="77"/>
-      <c r="AG16" s="77"/>
-      <c r="AH16" s="77"/>
-      <c r="AI16" s="77"/>
-      <c r="AJ16" s="77"/>
-      <c r="AK16" s="77"/>
-      <c r="AL16" s="77"/>
-      <c r="AM16" s="77"/>
-      <c r="AN16" s="77"/>
-      <c r="AO16" s="77"/>
-      <c r="AP16" s="77"/>
-      <c r="AQ16" s="77"/>
-      <c r="AR16" s="77"/>
-      <c r="AS16" s="77"/>
-      <c r="AT16" s="77"/>
-      <c r="AU16" s="77"/>
-      <c r="AV16" s="77"/>
-      <c r="AW16" s="77"/>
-      <c r="AX16" s="77"/>
-      <c r="AY16" s="77"/>
-      <c r="AZ16" s="77"/>
+      <c r="S16" s="34"/>
+      <c r="T16" s="34"/>
+      <c r="U16" s="35"/>
+      <c r="V16" s="35"/>
+      <c r="W16" s="34"/>
+      <c r="X16" s="34"/>
+      <c r="Y16" s="34"/>
+      <c r="Z16" s="34"/>
+      <c r="AA16" s="34"/>
+      <c r="AB16" s="34"/>
+      <c r="AC16" s="34"/>
+      <c r="AD16" s="34"/>
+      <c r="AE16" s="34"/>
+      <c r="AF16" s="34"/>
+      <c r="AG16" s="34"/>
+      <c r="AH16" s="34"/>
+      <c r="AI16" s="34"/>
+      <c r="AJ16" s="34"/>
+      <c r="AK16" s="34"/>
+      <c r="AL16" s="34"/>
+      <c r="AM16" s="34"/>
+      <c r="AN16" s="34"/>
+      <c r="AO16" s="34"/>
+      <c r="AP16" s="34"/>
+      <c r="AQ16" s="34"/>
+      <c r="AR16" s="34"/>
+      <c r="AS16" s="34"/>
+      <c r="AT16" s="34"/>
+      <c r="AU16" s="34"/>
+      <c r="AV16" s="34"/>
+      <c r="AW16" s="34"/>
+      <c r="AX16" s="34"/>
+      <c r="AY16" s="34"/>
+      <c r="AZ16" s="34"/>
       <c r="BA16" s="34"/>
       <c r="BB16" s="34"/>
       <c r="BC16" s="34"/>
@@ -4161,25 +4133,29 @@
     </row>
     <row r="17" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="47"/>
-      <c r="B17" s="70">
-        <v>2.1</v>
-      </c>
-      <c r="C17" s="72" t="s">
-        <v>44</v>
+      <c r="B17" s="57" t="str">
+        <f>_xlfn.CONCAT(B16,".1")</f>
+        <v>2.1.1</v>
+      </c>
+      <c r="C17" s="57" t="s">
+        <v>64</v>
       </c>
       <c r="D17" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E17" s="53">
-        <f>F15+1</f>
+        <f>E16</f>
         <v>44227</v>
       </c>
       <c r="F17" s="53">
-        <f>E17+4</f>
-        <v>44231</v>
+        <f>E17+0</f>
+        <v>44227</v>
       </c>
       <c r="G17" s="13"/>
-      <c r="H17" s="13"/>
+      <c r="H17" s="13">
+        <f t="shared" si="37"/>
+        <v>1</v>
+      </c>
       <c r="I17" s="34"/>
       <c r="J17" s="34"/>
       <c r="K17" s="34"/>
@@ -4192,11 +4168,11 @@
       <c r="R17" s="34"/>
       <c r="S17" s="34"/>
       <c r="T17" s="34"/>
-      <c r="U17" s="35"/>
-      <c r="V17" s="35"/>
+      <c r="U17" s="34"/>
+      <c r="V17" s="34"/>
       <c r="W17" s="34"/>
       <c r="X17" s="34"/>
-      <c r="Y17" s="34"/>
+      <c r="Y17" s="35"/>
       <c r="Z17" s="34"/>
       <c r="AA17" s="34"/>
       <c r="AB17" s="34"/>
@@ -4282,11 +4258,11 @@
     <row r="18" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="47"/>
       <c r="B18" s="57" t="str">
-        <f>_xlfn.CONCAT(B17,".1")</f>
-        <v>2.1.1</v>
+        <f>_xlfn.CONCAT(B16,".2")</f>
+        <v>2.1.2</v>
       </c>
       <c r="C18" s="57" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
       <c r="D18" s="23">
         <v>0</v>
@@ -4296,14 +4272,11 @@
         <v>44227</v>
       </c>
       <c r="F18" s="53">
-        <f>E18+0</f>
+        <f>E18</f>
         <v>44227</v>
       </c>
       <c r="G18" s="13"/>
-      <c r="H18" s="13">
-        <f t="shared" si="37"/>
-        <v>1</v>
-      </c>
+      <c r="H18" s="13"/>
       <c r="I18" s="34"/>
       <c r="J18" s="34"/>
       <c r="K18" s="34"/>
@@ -4320,7 +4293,7 @@
       <c r="V18" s="34"/>
       <c r="W18" s="34"/>
       <c r="X18" s="34"/>
-      <c r="Y18" s="35"/>
+      <c r="Y18" s="34"/>
       <c r="Z18" s="34"/>
       <c r="AA18" s="34"/>
       <c r="AB18" s="34"/>
@@ -4406,25 +4379,28 @@
     <row r="19" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="47"/>
       <c r="B19" s="57" t="str">
-        <f>_xlfn.CONCAT(B17,".2")</f>
-        <v>2.1.2</v>
+        <f>_xlfn.CONCAT(B16,".3")</f>
+        <v>2.1.3</v>
       </c>
       <c r="C19" s="57" t="s">
-        <v>48</v>
+        <v>77</v>
       </c>
       <c r="D19" s="23">
         <v>0</v>
       </c>
       <c r="E19" s="53">
-        <f>E18</f>
-        <v>44227</v>
+        <f>F18+1</f>
+        <v>44228</v>
       </c>
       <c r="F19" s="53">
-        <f>E19</f>
-        <v>44227</v>
+        <f>F16</f>
+        <v>44231</v>
       </c>
       <c r="G19" s="13"/>
-      <c r="H19" s="13"/>
+      <c r="H19" s="13">
+        <f t="shared" si="37"/>
+        <v>4</v>
+      </c>
       <c r="I19" s="34"/>
       <c r="J19" s="34"/>
       <c r="K19" s="34"/>
@@ -4526,29 +4502,25 @@
     </row>
     <row r="20" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="47"/>
-      <c r="B20" s="57" t="str">
-        <f>_xlfn.CONCAT(B17,".3")</f>
-        <v>2.1.3</v>
-      </c>
-      <c r="C20" s="57" t="s">
-        <v>47</v>
+      <c r="B20" s="69">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="C20" s="71" t="s">
+        <v>46</v>
       </c>
       <c r="D20" s="23">
         <v>0</v>
       </c>
       <c r="E20" s="53">
-        <f>F19+1</f>
-        <v>44228</v>
+        <f>F16+1</f>
+        <v>44232</v>
       </c>
       <c r="F20" s="53">
-        <f>F17</f>
-        <v>44231</v>
+        <f>E20+4</f>
+        <v>44236</v>
       </c>
       <c r="G20" s="13"/>
-      <c r="H20" s="13">
-        <f t="shared" si="37"/>
-        <v>4</v>
-      </c>
+      <c r="H20" s="13"/>
       <c r="I20" s="34"/>
       <c r="J20" s="34"/>
       <c r="K20" s="34"/>
@@ -4650,22 +4622,23 @@
     </row>
     <row r="21" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="47"/>
-      <c r="B21" s="70">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="C21" s="72" t="s">
-        <v>46</v>
+      <c r="B21" s="57" t="str">
+        <f>_xlfn.CONCAT(B20,".1")</f>
+        <v>2.2.1</v>
+      </c>
+      <c r="C21" s="57" t="s">
+        <v>48</v>
       </c>
       <c r="D21" s="23">
         <v>0</v>
       </c>
       <c r="E21" s="53">
-        <f>F17+1</f>
+        <f>E20</f>
         <v>44232</v>
       </c>
       <c r="F21" s="53">
-        <f>E21+4</f>
-        <v>44236</v>
+        <f>E21</f>
+        <v>44232</v>
       </c>
       <c r="G21" s="13"/>
       <c r="H21" s="13"/>
@@ -4685,7 +4658,7 @@
       <c r="V21" s="34"/>
       <c r="W21" s="34"/>
       <c r="X21" s="34"/>
-      <c r="Y21" s="34"/>
+      <c r="Y21" s="35"/>
       <c r="Z21" s="34"/>
       <c r="AA21" s="34"/>
       <c r="AB21" s="34"/>
@@ -4771,22 +4744,22 @@
     <row r="22" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="47"/>
       <c r="B22" s="57" t="str">
-        <f>_xlfn.CONCAT(B21,".1")</f>
-        <v>2.2.1</v>
+        <f>_xlfn.CONCAT(B20,".2")</f>
+        <v>2.2.2</v>
       </c>
       <c r="C22" s="57" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="D22" s="23">
         <v>0</v>
       </c>
       <c r="E22" s="53">
-        <f>E21</f>
-        <v>44232</v>
+        <f>F21+1</f>
+        <v>44233</v>
       </c>
       <c r="F22" s="53">
-        <f>E22</f>
-        <v>44232</v>
+        <f>E22+3</f>
+        <v>44236</v>
       </c>
       <c r="G22" s="13"/>
       <c r="H22" s="13"/>
@@ -4891,23 +4864,22 @@
     </row>
     <row r="23" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="47"/>
-      <c r="B23" s="57" t="str">
-        <f>_xlfn.CONCAT(B21,".2")</f>
-        <v>2.2.2</v>
+      <c r="B23" s="69">
+        <v>2.2999999999999998</v>
       </c>
       <c r="C23" s="57" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="D23" s="23">
         <v>0</v>
       </c>
       <c r="E23" s="53">
-        <f>F22+1</f>
-        <v>44233</v>
+        <f>E20+3</f>
+        <v>44235</v>
       </c>
       <c r="F23" s="53">
-        <f>E23+3</f>
-        <v>44236</v>
+        <f>E23+7</f>
+        <v>44242</v>
       </c>
       <c r="G23" s="13"/>
       <c r="H23" s="13"/>
@@ -5012,22 +4984,23 @@
     </row>
     <row r="24" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="47"/>
-      <c r="B24" s="70">
-        <v>2.2999999999999998</v>
+      <c r="B24" s="57" t="str">
+        <f>_xlfn.CONCAT(B23,".1")</f>
+        <v>2.3.1</v>
       </c>
       <c r="C24" s="57" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D24" s="23">
         <v>0</v>
       </c>
       <c r="E24" s="53">
-        <f>E21+3</f>
+        <f>E23</f>
         <v>44235</v>
       </c>
       <c r="F24" s="53">
-        <f>E24+7</f>
-        <v>44242</v>
+        <f>E24+1</f>
+        <v>44236</v>
       </c>
       <c r="G24" s="13"/>
       <c r="H24" s="13"/>
@@ -5132,23 +5105,23 @@
     </row>
     <row r="25" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="47"/>
-      <c r="B25" s="57" t="str">
-        <f>_xlfn.CONCAT(B24,".1")</f>
-        <v>2.3.1</v>
+      <c r="B25" s="71" t="str">
+        <f>_xlfn.CONCAT(B23,".2")</f>
+        <v>2.3.2</v>
       </c>
       <c r="C25" s="57" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D25" s="23">
         <v>0</v>
       </c>
       <c r="E25" s="53">
-        <f>E24</f>
-        <v>44235</v>
+        <f>F24+1</f>
+        <v>44237</v>
       </c>
       <c r="F25" s="53">
-        <f>E25+1</f>
-        <v>44236</v>
+        <f>F23</f>
+        <v>44242</v>
       </c>
       <c r="G25" s="13"/>
       <c r="H25" s="13"/>
@@ -5253,22 +5226,21 @@
     </row>
     <row r="26" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="47"/>
-      <c r="B26" s="72" t="str">
-        <f>_xlfn.CONCAT(B24,".2")</f>
-        <v>2.3.2</v>
-      </c>
-      <c r="C26" s="57" t="s">
-        <v>78</v>
+      <c r="B26" s="69">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="C26" s="71" t="s">
+        <v>65</v>
       </c>
       <c r="D26" s="23">
         <v>0</v>
       </c>
       <c r="E26" s="53">
-        <f>F25+1</f>
+        <f>F20+1</f>
         <v>44237</v>
       </c>
       <c r="F26" s="53">
-        <f>F24</f>
+        <f>E26+5</f>
         <v>44242</v>
       </c>
       <c r="G26" s="13"/>
@@ -5374,22 +5346,22 @@
     </row>
     <row r="27" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="47"/>
-      <c r="B27" s="70">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="C27" s="72" t="s">
-        <v>68</v>
+      <c r="B27" s="69">
+        <v>2.4</v>
+      </c>
+      <c r="C27" s="57" t="s">
+        <v>51</v>
       </c>
       <c r="D27" s="23">
         <v>0</v>
       </c>
       <c r="E27" s="53">
-        <f>F21+1</f>
-        <v>44237</v>
+        <f>F26+1</f>
+        <v>44243</v>
       </c>
       <c r="F27" s="53">
-        <f>E27+5</f>
-        <v>44242</v>
+        <f>E27</f>
+        <v>44243</v>
       </c>
       <c r="G27" s="13"/>
       <c r="H27" s="13"/>
@@ -5494,25 +5466,28 @@
     </row>
     <row r="28" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="47"/>
-      <c r="B28" s="70">
-        <v>2.4</v>
+      <c r="B28" s="69">
+        <v>2.5</v>
       </c>
       <c r="C28" s="57" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D28" s="23">
         <v>0</v>
       </c>
       <c r="E28" s="53">
         <f>F27+1</f>
-        <v>44243</v>
+        <v>44244</v>
       </c>
       <c r="F28" s="53">
-        <f>E28</f>
-        <v>44243</v>
+        <f>E28+3</f>
+        <v>44247</v>
       </c>
       <c r="G28" s="13"/>
-      <c r="H28" s="13"/>
+      <c r="H28" s="13">
+        <f t="shared" si="37"/>
+        <v>4</v>
+      </c>
       <c r="I28" s="34"/>
       <c r="J28" s="34"/>
       <c r="K28" s="34"/>
@@ -5525,11 +5500,11 @@
       <c r="R28" s="34"/>
       <c r="S28" s="34"/>
       <c r="T28" s="34"/>
-      <c r="U28" s="34"/>
-      <c r="V28" s="34"/>
+      <c r="U28" s="35"/>
+      <c r="V28" s="35"/>
       <c r="W28" s="34"/>
       <c r="X28" s="34"/>
-      <c r="Y28" s="35"/>
+      <c r="Y28" s="34"/>
       <c r="Z28" s="34"/>
       <c r="AA28" s="34"/>
       <c r="AB28" s="34"/>
@@ -5613,28 +5588,28 @@
       <c r="DB28" s="34"/>
     </row>
     <row r="29" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="47"/>
-      <c r="B29" s="70">
-        <v>2.5</v>
-      </c>
-      <c r="C29" s="57" t="s">
-        <v>55</v>
+      <c r="A29" s="48"/>
+      <c r="B29" s="69">
+        <v>2.6</v>
+      </c>
+      <c r="C29" s="71" t="s">
+        <v>53</v>
       </c>
       <c r="D29" s="23">
         <v>0</v>
       </c>
       <c r="E29" s="53">
         <f>F28+1</f>
-        <v>44244</v>
+        <v>44248</v>
       </c>
       <c r="F29" s="53">
-        <f>E29+3</f>
-        <v>44247</v>
+        <f>E29+2</f>
+        <v>44250</v>
       </c>
       <c r="G29" s="13"/>
       <c r="H29" s="13">
         <f t="shared" si="37"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I29" s="34"/>
       <c r="J29" s="34"/>
@@ -5648,8 +5623,8 @@
       <c r="R29" s="34"/>
       <c r="S29" s="34"/>
       <c r="T29" s="34"/>
-      <c r="U29" s="35"/>
-      <c r="V29" s="35"/>
+      <c r="U29" s="34"/>
+      <c r="V29" s="34"/>
       <c r="W29" s="34"/>
       <c r="X29" s="34"/>
       <c r="Y29" s="34"/>
@@ -5736,28 +5711,26 @@
       <c r="DB29" s="34"/>
     </row>
     <row r="30" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="48"/>
-      <c r="B30" s="70">
-        <v>2.6</v>
-      </c>
-      <c r="C30" s="72" t="s">
-        <v>54</v>
+      <c r="A30" s="47"/>
+      <c r="B30" s="69">
+        <v>2.7</v>
+      </c>
+      <c r="C30" s="71" t="s">
+        <v>59</v>
       </c>
       <c r="D30" s="23">
         <v>0</v>
       </c>
       <c r="E30" s="53">
-        <f>F29+1</f>
-        <v>44248</v>
+        <v>44227</v>
       </c>
       <c r="F30" s="53">
-        <f>E30+2</f>
-        <v>44250</v>
+        <v>44255</v>
       </c>
       <c r="G30" s="13"/>
       <c r="H30" s="13">
         <f t="shared" si="37"/>
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="I30" s="34"/>
       <c r="J30" s="34"/>
@@ -5860,11 +5833,12 @@
     </row>
     <row r="31" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="47"/>
-      <c r="B31" s="70">
-        <v>2.7</v>
-      </c>
-      <c r="C31" s="72" t="s">
-        <v>60</v>
+      <c r="B31" s="71" t="str">
+        <f>_xlfn.CONCAT(B30,".1")</f>
+        <v>2.7.1</v>
+      </c>
+      <c r="C31" s="57" t="s">
+        <v>66</v>
       </c>
       <c r="D31" s="23">
         <v>0</v>
@@ -5873,13 +5847,11 @@
         <v>44227</v>
       </c>
       <c r="F31" s="53">
-        <v>44255</v>
+        <f>F29+2</f>
+        <v>44252</v>
       </c>
       <c r="G31" s="13"/>
-      <c r="H31" s="13">
-        <f t="shared" si="37"/>
-        <v>29</v>
-      </c>
+      <c r="H31" s="13"/>
       <c r="I31" s="34"/>
       <c r="J31" s="34"/>
       <c r="K31" s="34"/>
@@ -5896,7 +5868,7 @@
       <c r="V31" s="34"/>
       <c r="W31" s="34"/>
       <c r="X31" s="34"/>
-      <c r="Y31" s="34"/>
+      <c r="Y31" s="35"/>
       <c r="Z31" s="34"/>
       <c r="AA31" s="34"/>
       <c r="AB31" s="34"/>
@@ -5981,22 +5953,22 @@
     </row>
     <row r="32" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="47"/>
-      <c r="B32" s="72" t="str">
-        <f>_xlfn.CONCAT(B31,".1")</f>
-        <v>2.7.1</v>
-      </c>
-      <c r="C32" s="57" t="s">
-        <v>69</v>
+      <c r="B32" s="71" t="str">
+        <f>_xlfn.CONCAT(B30,".2")</f>
+        <v>2.7.2</v>
+      </c>
+      <c r="C32" s="71" t="s">
+        <v>60</v>
       </c>
       <c r="D32" s="23">
         <v>0</v>
       </c>
       <c r="E32" s="53">
-        <v>44227</v>
+        <f>F31+1</f>
+        <v>44253</v>
       </c>
       <c r="F32" s="53">
-        <f>F30+2</f>
-        <v>44252</v>
+        <v>44255</v>
       </c>
       <c r="G32" s="13"/>
       <c r="H32" s="13"/>
@@ -6016,7 +5988,7 @@
       <c r="V32" s="34"/>
       <c r="W32" s="34"/>
       <c r="X32" s="34"/>
-      <c r="Y32" s="35"/>
+      <c r="Y32" s="34"/>
       <c r="Z32" s="34"/>
       <c r="AA32" s="34"/>
       <c r="AB32" s="34"/>
@@ -6100,26 +6072,23 @@
       <c r="DB32" s="34"/>
     </row>
     <row r="33" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="47"/>
-      <c r="B33" s="72" t="str">
-        <f>_xlfn.CONCAT(B31,".2")</f>
-        <v>2.7.2</v>
-      </c>
-      <c r="C33" s="72" t="s">
-        <v>61</v>
-      </c>
-      <c r="D33" s="23">
-        <v>0</v>
-      </c>
-      <c r="E33" s="53">
-        <f>F32+1</f>
-        <v>44253</v>
-      </c>
-      <c r="F33" s="53">
-        <v>44255</v>
-      </c>
+      <c r="A33" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="B33" s="24">
+        <v>3</v>
+      </c>
+      <c r="C33" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="D33" s="25"/>
+      <c r="E33" s="26"/>
+      <c r="F33" s="27"/>
       <c r="G33" s="13"/>
-      <c r="H33" s="13"/>
+      <c r="H33" s="13" t="str">
+        <f t="shared" si="37"/>
+        <v/>
+      </c>
       <c r="I33" s="34"/>
       <c r="J33" s="34"/>
       <c r="K33" s="34"/>
@@ -6161,39 +6130,39 @@
       <c r="AU33" s="34"/>
       <c r="AV33" s="34"/>
       <c r="AW33" s="34"/>
-      <c r="AX33" s="34"/>
-      <c r="AY33" s="34"/>
-      <c r="AZ33" s="34"/>
-      <c r="BA33" s="34"/>
-      <c r="BB33" s="34"/>
-      <c r="BC33" s="34"/>
-      <c r="BD33" s="34"/>
-      <c r="BE33" s="34"/>
-      <c r="BF33" s="34"/>
-      <c r="BG33" s="34"/>
-      <c r="BH33" s="34"/>
-      <c r="BI33" s="34"/>
-      <c r="BJ33" s="34"/>
-      <c r="BK33" s="34"/>
-      <c r="BL33" s="34"/>
-      <c r="BM33" s="34"/>
-      <c r="BN33" s="34"/>
-      <c r="BO33" s="34"/>
-      <c r="BP33" s="34"/>
-      <c r="BQ33" s="34"/>
-      <c r="BR33" s="34"/>
-      <c r="BS33" s="34"/>
-      <c r="BT33" s="34"/>
-      <c r="BU33" s="34"/>
-      <c r="BV33" s="34"/>
-      <c r="BW33" s="34"/>
-      <c r="BX33" s="34"/>
-      <c r="BY33" s="34"/>
-      <c r="BZ33" s="34"/>
-      <c r="CA33" s="34"/>
-      <c r="CB33" s="34"/>
-      <c r="CC33" s="34"/>
-      <c r="CD33" s="34"/>
+      <c r="AX33" s="76"/>
+      <c r="AY33" s="76"/>
+      <c r="AZ33" s="76"/>
+      <c r="BA33" s="76"/>
+      <c r="BB33" s="76"/>
+      <c r="BC33" s="76"/>
+      <c r="BD33" s="76"/>
+      <c r="BE33" s="76"/>
+      <c r="BF33" s="76"/>
+      <c r="BG33" s="76"/>
+      <c r="BH33" s="76"/>
+      <c r="BI33" s="76"/>
+      <c r="BJ33" s="76"/>
+      <c r="BK33" s="76"/>
+      <c r="BL33" s="76"/>
+      <c r="BM33" s="76"/>
+      <c r="BN33" s="76"/>
+      <c r="BO33" s="76"/>
+      <c r="BP33" s="76"/>
+      <c r="BQ33" s="76"/>
+      <c r="BR33" s="76"/>
+      <c r="BS33" s="76"/>
+      <c r="BT33" s="76"/>
+      <c r="BU33" s="76"/>
+      <c r="BV33" s="76"/>
+      <c r="BW33" s="76"/>
+      <c r="BX33" s="76"/>
+      <c r="BY33" s="76"/>
+      <c r="BZ33" s="76"/>
+      <c r="CA33" s="76"/>
+      <c r="CB33" s="76"/>
+      <c r="CC33" s="76"/>
+      <c r="CD33" s="76"/>
       <c r="CE33" s="34"/>
       <c r="CF33" s="34"/>
       <c r="CG33" s="34"/>
@@ -6219,24 +6188,26 @@
       <c r="DA33" s="34"/>
       <c r="DB33" s="34"/>
     </row>
-    <row r="34" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="47" t="s">
-        <v>21</v>
-      </c>
-      <c r="B34" s="24">
-        <v>3</v>
-      </c>
-      <c r="C34" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="D34" s="25"/>
-      <c r="E34" s="26"/>
-      <c r="F34" s="27"/>
+    <row r="34" spans="1:106" s="2" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="48"/>
+      <c r="B34" s="72">
+        <v>3.1</v>
+      </c>
+      <c r="C34" s="58" t="s">
+        <v>67</v>
+      </c>
+      <c r="D34" s="28">
+        <v>0</v>
+      </c>
+      <c r="E34" s="54">
+        <v>44256</v>
+      </c>
+      <c r="F34" s="54">
+        <f>E34+3</f>
+        <v>44259</v>
+      </c>
       <c r="G34" s="13"/>
-      <c r="H34" s="13" t="str">
-        <f t="shared" si="37"/>
-        <v/>
-      </c>
+      <c r="H34" s="13"/>
       <c r="I34" s="34"/>
       <c r="J34" s="34"/>
       <c r="K34" s="34"/>
@@ -6249,8 +6220,8 @@
       <c r="R34" s="34"/>
       <c r="S34" s="34"/>
       <c r="T34" s="34"/>
-      <c r="U34" s="34"/>
-      <c r="V34" s="34"/>
+      <c r="U34" s="35"/>
+      <c r="V34" s="35"/>
       <c r="W34" s="34"/>
       <c r="X34" s="34"/>
       <c r="Y34" s="34"/>
@@ -6279,37 +6250,37 @@
       <c r="AV34" s="34"/>
       <c r="AW34" s="34"/>
       <c r="AX34" s="34"/>
-      <c r="AY34" s="78"/>
-      <c r="AZ34" s="78"/>
-      <c r="BA34" s="78"/>
-      <c r="BB34" s="78"/>
-      <c r="BC34" s="78"/>
-      <c r="BD34" s="78"/>
-      <c r="BE34" s="78"/>
-      <c r="BF34" s="78"/>
-      <c r="BG34" s="78"/>
-      <c r="BH34" s="78"/>
-      <c r="BI34" s="78"/>
-      <c r="BJ34" s="78"/>
-      <c r="BK34" s="78"/>
-      <c r="BL34" s="78"/>
-      <c r="BM34" s="78"/>
-      <c r="BN34" s="78"/>
-      <c r="BO34" s="78"/>
-      <c r="BP34" s="78"/>
-      <c r="BQ34" s="78"/>
-      <c r="BR34" s="78"/>
-      <c r="BS34" s="78"/>
-      <c r="BT34" s="78"/>
-      <c r="BU34" s="78"/>
-      <c r="BV34" s="78"/>
-      <c r="BW34" s="78"/>
-      <c r="BX34" s="78"/>
-      <c r="BY34" s="78"/>
-      <c r="BZ34" s="78"/>
-      <c r="CA34" s="78"/>
-      <c r="CB34" s="78"/>
-      <c r="CC34" s="78"/>
+      <c r="AY34" s="34"/>
+      <c r="AZ34" s="34"/>
+      <c r="BA34" s="34"/>
+      <c r="BB34" s="34"/>
+      <c r="BC34" s="34"/>
+      <c r="BD34" s="34"/>
+      <c r="BE34" s="34"/>
+      <c r="BF34" s="34"/>
+      <c r="BG34" s="34"/>
+      <c r="BH34" s="34"/>
+      <c r="BI34" s="34"/>
+      <c r="BJ34" s="34"/>
+      <c r="BK34" s="34"/>
+      <c r="BL34" s="34"/>
+      <c r="BM34" s="34"/>
+      <c r="BN34" s="34"/>
+      <c r="BO34" s="34"/>
+      <c r="BP34" s="34"/>
+      <c r="BQ34" s="34"/>
+      <c r="BR34" s="34"/>
+      <c r="BS34" s="34"/>
+      <c r="BT34" s="34"/>
+      <c r="BU34" s="34"/>
+      <c r="BV34" s="34"/>
+      <c r="BW34" s="34"/>
+      <c r="BX34" s="34"/>
+      <c r="BY34" s="34"/>
+      <c r="BZ34" s="34"/>
+      <c r="CA34" s="34"/>
+      <c r="CB34" s="34"/>
+      <c r="CC34" s="34"/>
       <c r="CD34" s="34"/>
       <c r="CE34" s="34"/>
       <c r="CF34" s="34"/>
@@ -6336,23 +6307,24 @@
       <c r="DA34" s="34"/>
       <c r="DB34" s="34"/>
     </row>
-    <row r="35" spans="1:106" s="2" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="48"/>
-      <c r="B35" s="73">
-        <v>3.1</v>
+    <row r="35" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="47"/>
+      <c r="B35" s="72">
+        <v>3.2</v>
       </c>
       <c r="C35" s="58" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="D35" s="28">
         <v>0</v>
       </c>
       <c r="E35" s="54">
-        <v>44256</v>
+        <f>F34+1</f>
+        <v>44260</v>
       </c>
       <c r="F35" s="54">
-        <f>E35+3</f>
-        <v>44259</v>
+        <f>E35+4</f>
+        <v>44264</v>
       </c>
       <c r="G35" s="13"/>
       <c r="H35" s="13"/>
@@ -6368,8 +6340,8 @@
       <c r="R35" s="34"/>
       <c r="S35" s="34"/>
       <c r="T35" s="34"/>
-      <c r="U35" s="35"/>
-      <c r="V35" s="35"/>
+      <c r="U35" s="34"/>
+      <c r="V35" s="34"/>
       <c r="W35" s="34"/>
       <c r="X35" s="34"/>
       <c r="Y35" s="34"/>
@@ -6457,25 +6429,28 @@
     </row>
     <row r="36" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="47"/>
-      <c r="B36" s="73">
-        <v>3.2</v>
+      <c r="B36" s="72">
+        <v>3.3</v>
       </c>
       <c r="C36" s="58" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="D36" s="28">
         <v>0</v>
       </c>
       <c r="E36" s="54">
         <f>F35+1</f>
-        <v>44260</v>
+        <v>44265</v>
       </c>
       <c r="F36" s="54">
-        <f>E36+4</f>
-        <v>44264</v>
+        <f>E36+10</f>
+        <v>44275</v>
       </c>
       <c r="G36" s="13"/>
-      <c r="H36" s="13"/>
+      <c r="H36" s="13">
+        <f t="shared" si="37"/>
+        <v>11</v>
+      </c>
       <c r="I36" s="34"/>
       <c r="J36" s="34"/>
       <c r="K36" s="34"/>
@@ -6577,22 +6552,22 @@
     </row>
     <row r="37" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="47"/>
-      <c r="B37" s="73">
-        <v>3.3</v>
+      <c r="B37" s="72">
+        <v>3.4</v>
       </c>
       <c r="C37" s="58" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="D37" s="28">
         <v>0</v>
       </c>
       <c r="E37" s="54">
         <f>F36+1</f>
-        <v>44265</v>
+        <v>44276</v>
       </c>
       <c r="F37" s="54">
         <f>E37+10</f>
-        <v>44275</v>
+        <v>44286</v>
       </c>
       <c r="G37" s="13"/>
       <c r="H37" s="13">
@@ -6700,28 +6675,25 @@
     </row>
     <row r="38" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="47"/>
-      <c r="B38" s="73">
-        <v>3.4</v>
+      <c r="B38" s="72">
+        <v>3.5</v>
       </c>
       <c r="C38" s="58" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="D38" s="28">
         <v>0</v>
       </c>
       <c r="E38" s="54">
-        <f>F37+1</f>
-        <v>44276</v>
+        <f>F32+14</f>
+        <v>44269</v>
       </c>
       <c r="F38" s="54">
-        <f>E38+10</f>
-        <v>44286</v>
+        <f>E38+5</f>
+        <v>44274</v>
       </c>
       <c r="G38" s="13"/>
-      <c r="H38" s="13">
-        <f t="shared" si="37"/>
-        <v>11</v>
-      </c>
+      <c r="H38" s="13"/>
       <c r="I38" s="34"/>
       <c r="J38" s="34"/>
       <c r="K38" s="34"/>
@@ -6823,25 +6795,28 @@
     </row>
     <row r="39" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="47"/>
-      <c r="B39" s="73">
-        <v>3.5</v>
+      <c r="B39" s="72">
+        <v>3.6</v>
       </c>
       <c r="C39" s="58" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="D39" s="28">
         <v>0</v>
       </c>
       <c r="E39" s="54">
-        <f>F33+14</f>
-        <v>44269</v>
+        <f>F38+1</f>
+        <v>44275</v>
       </c>
       <c r="F39" s="54">
-        <f>E39+5</f>
-        <v>44274</v>
+        <f>E39+4</f>
+        <v>44279</v>
       </c>
       <c r="G39" s="13"/>
-      <c r="H39" s="13"/>
+      <c r="H39" s="13">
+        <f t="shared" si="37"/>
+        <v>5</v>
+      </c>
       <c r="I39" s="34"/>
       <c r="J39" s="34"/>
       <c r="K39" s="34"/>
@@ -6942,28 +6917,22 @@
       <c r="DB39" s="34"/>
     </row>
     <row r="40" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="47"/>
-      <c r="B40" s="73">
-        <v>3.6</v>
-      </c>
-      <c r="C40" s="58" t="s">
-        <v>72</v>
-      </c>
-      <c r="D40" s="28">
-        <v>0</v>
-      </c>
-      <c r="E40" s="54">
-        <f>F39+1</f>
-        <v>44275</v>
-      </c>
-      <c r="F40" s="54">
-        <f>E40+4</f>
-        <v>44279</v>
-      </c>
+      <c r="A40" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="B40" s="29">
+        <v>4</v>
+      </c>
+      <c r="C40" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="D40" s="30"/>
+      <c r="E40" s="31"/>
+      <c r="F40" s="32"/>
       <c r="G40" s="13"/>
-      <c r="H40" s="13">
+      <c r="H40" s="13" t="str">
         <f t="shared" si="37"/>
-        <v>5</v>
+        <v/>
       </c>
       <c r="I40" s="34"/>
       <c r="J40" s="34"/>
@@ -7034,54 +7003,57 @@
       <c r="BW40" s="34"/>
       <c r="BX40" s="34"/>
       <c r="BY40" s="34"/>
-      <c r="BZ40" s="34"/>
-      <c r="CA40" s="34"/>
-      <c r="CB40" s="34"/>
-      <c r="CC40" s="34"/>
-      <c r="CD40" s="34"/>
-      <c r="CE40" s="34"/>
-      <c r="CF40" s="34"/>
-      <c r="CG40" s="34"/>
-      <c r="CH40" s="34"/>
-      <c r="CI40" s="34"/>
-      <c r="CJ40" s="34"/>
-      <c r="CK40" s="34"/>
-      <c r="CL40" s="34"/>
-      <c r="CM40" s="34"/>
-      <c r="CN40" s="34"/>
-      <c r="CO40" s="34"/>
-      <c r="CP40" s="34"/>
-      <c r="CQ40" s="34"/>
-      <c r="CR40" s="34"/>
-      <c r="CS40" s="34"/>
-      <c r="CT40" s="34"/>
-      <c r="CU40" s="34"/>
-      <c r="CV40" s="34"/>
-      <c r="CW40" s="34"/>
-      <c r="CX40" s="34"/>
-      <c r="CY40" s="34"/>
+      <c r="BZ40" s="76"/>
+      <c r="CA40" s="76"/>
+      <c r="CB40" s="76"/>
+      <c r="CC40" s="76"/>
+      <c r="CD40" s="76"/>
+      <c r="CE40" s="76"/>
+      <c r="CF40" s="76"/>
+      <c r="CG40" s="76"/>
+      <c r="CH40" s="76"/>
+      <c r="CI40" s="76"/>
+      <c r="CJ40" s="76"/>
+      <c r="CK40" s="76"/>
+      <c r="CL40" s="76"/>
+      <c r="CM40" s="76"/>
+      <c r="CN40" s="76"/>
+      <c r="CO40" s="76"/>
+      <c r="CP40" s="76"/>
+      <c r="CQ40" s="76"/>
+      <c r="CR40" s="76"/>
+      <c r="CS40" s="76"/>
+      <c r="CT40" s="76"/>
+      <c r="CU40" s="76"/>
+      <c r="CV40" s="76"/>
+      <c r="CW40" s="76"/>
+      <c r="CX40" s="76"/>
+      <c r="CY40" s="76"/>
       <c r="CZ40" s="34"/>
       <c r="DA40" s="34"/>
       <c r="DB40" s="34"/>
     </row>
     <row r="41" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="47" t="s">
-        <v>21</v>
-      </c>
-      <c r="B41" s="29">
-        <v>4</v>
-      </c>
-      <c r="C41" s="29" t="s">
-        <v>50</v>
-      </c>
-      <c r="D41" s="30"/>
-      <c r="E41" s="31"/>
-      <c r="F41" s="32"/>
+      <c r="A41" s="47"/>
+      <c r="B41" s="73">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="C41" s="59" t="s">
+        <v>70</v>
+      </c>
+      <c r="D41" s="33">
+        <v>0</v>
+      </c>
+      <c r="E41" s="55">
+        <f>F37+1</f>
+        <v>44287</v>
+      </c>
+      <c r="F41" s="55">
+        <f>E42-1</f>
+        <v>44292</v>
+      </c>
       <c r="G41" s="13"/>
-      <c r="H41" s="13" t="str">
-        <f t="shared" si="37"/>
-        <v/>
-      </c>
+      <c r="H41" s="13"/>
       <c r="I41" s="34"/>
       <c r="J41" s="34"/>
       <c r="K41" s="34"/>
@@ -7155,24 +7127,24 @@
       <c r="CA41" s="34"/>
       <c r="CB41" s="34"/>
       <c r="CC41" s="34"/>
-      <c r="CD41" s="79"/>
-      <c r="CE41" s="79"/>
-      <c r="CF41" s="79"/>
-      <c r="CG41" s="79"/>
-      <c r="CH41" s="79"/>
-      <c r="CI41" s="79"/>
-      <c r="CJ41" s="79"/>
-      <c r="CK41" s="79"/>
-      <c r="CL41" s="79"/>
-      <c r="CM41" s="79"/>
-      <c r="CN41" s="79"/>
-      <c r="CO41" s="79"/>
-      <c r="CP41" s="79"/>
-      <c r="CQ41" s="79"/>
-      <c r="CR41" s="79"/>
-      <c r="CS41" s="79"/>
-      <c r="CT41" s="79"/>
-      <c r="CU41" s="79"/>
+      <c r="CD41" s="34"/>
+      <c r="CE41" s="34"/>
+      <c r="CF41" s="34"/>
+      <c r="CG41" s="34"/>
+      <c r="CH41" s="34"/>
+      <c r="CI41" s="34"/>
+      <c r="CJ41" s="34"/>
+      <c r="CK41" s="34"/>
+      <c r="CL41" s="34"/>
+      <c r="CM41" s="34"/>
+      <c r="CN41" s="34"/>
+      <c r="CO41" s="34"/>
+      <c r="CP41" s="34"/>
+      <c r="CQ41" s="34"/>
+      <c r="CR41" s="34"/>
+      <c r="CS41" s="34"/>
+      <c r="CT41" s="34"/>
+      <c r="CU41" s="34"/>
       <c r="CV41" s="34"/>
       <c r="CW41" s="34"/>
       <c r="CX41" s="34"/>
@@ -7183,22 +7155,22 @@
     </row>
     <row r="42" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="47"/>
-      <c r="B42" s="74">
-        <v>4.0999999999999996</v>
+      <c r="B42" s="73">
+        <v>4.2</v>
       </c>
       <c r="C42" s="59" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="D42" s="33">
         <v>0</v>
       </c>
       <c r="E42" s="55">
-        <f>F38+1</f>
-        <v>44287</v>
+        <f>F39+14</f>
+        <v>44293</v>
       </c>
       <c r="F42" s="55">
-        <f>E43-1</f>
-        <v>44292</v>
+        <f>E42+7</f>
+        <v>44300</v>
       </c>
       <c r="G42" s="13"/>
       <c r="H42" s="13"/>
@@ -7303,25 +7275,26 @@
     </row>
     <row r="43" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="47"/>
-      <c r="B43" s="74">
-        <v>4.2</v>
+      <c r="B43" s="73">
+        <v>4.3</v>
       </c>
       <c r="C43" s="59" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="D43" s="33">
         <v>0</v>
       </c>
       <c r="E43" s="55">
-        <f>F40+14</f>
-        <v>44293</v>
+        <v>44301</v>
       </c>
       <c r="F43" s="55">
-        <f>E43+7</f>
-        <v>44300</v>
+        <v>44302</v>
       </c>
       <c r="G43" s="13"/>
-      <c r="H43" s="13"/>
+      <c r="H43" s="13">
+        <f t="shared" si="37"/>
+        <v>2</v>
+      </c>
       <c r="I43" s="34"/>
       <c r="J43" s="34"/>
       <c r="K43" s="34"/>
@@ -7423,20 +7396,20 @@
     </row>
     <row r="44" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="47"/>
-      <c r="B44" s="74">
-        <v>4.3</v>
+      <c r="B44" s="73">
+        <v>4.4000000000000004</v>
       </c>
       <c r="C44" s="59" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D44" s="33">
         <v>0</v>
       </c>
       <c r="E44" s="55">
-        <v>44301</v>
+        <v>44303</v>
       </c>
       <c r="F44" s="55">
-        <v>44302</v>
+        <v>44304</v>
       </c>
       <c r="G44" s="13"/>
       <c r="H44" s="13">
@@ -7543,26 +7516,22 @@
       <c r="DB44" s="34"/>
     </row>
     <row r="45" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="47"/>
-      <c r="B45" s="74">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="C45" s="59" t="s">
-        <v>57</v>
-      </c>
-      <c r="D45" s="33">
-        <v>0</v>
-      </c>
-      <c r="E45" s="55">
-        <v>44303</v>
-      </c>
-      <c r="F45" s="55">
-        <v>44304</v>
-      </c>
+      <c r="A45" s="47" t="s">
+        <v>23</v>
+      </c>
+      <c r="B45" s="61">
+        <v>5</v>
+      </c>
+      <c r="C45" s="61" t="s">
+        <v>39</v>
+      </c>
+      <c r="D45" s="62"/>
+      <c r="E45" s="63"/>
+      <c r="F45" s="64"/>
       <c r="G45" s="13"/>
-      <c r="H45" s="13">
+      <c r="H45" s="13" t="str">
         <f t="shared" si="37"/>
-        <v>2</v>
+        <v/>
       </c>
       <c r="I45" s="34"/>
       <c r="J45" s="34"/>
@@ -7664,22 +7633,28 @@
       <c r="DB45" s="34"/>
     </row>
     <row r="46" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="47" t="s">
-        <v>23</v>
-      </c>
-      <c r="B46" s="61">
-        <v>5</v>
-      </c>
-      <c r="C46" s="61" t="s">
-        <v>39</v>
-      </c>
-      <c r="D46" s="62"/>
-      <c r="E46" s="63"/>
-      <c r="F46" s="64"/>
+      <c r="A46" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="B46" s="74">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="C46" s="65" t="s">
+        <v>71</v>
+      </c>
+      <c r="D46" s="66">
+        <v>0</v>
+      </c>
+      <c r="E46" s="67" t="s">
+        <v>55</v>
+      </c>
+      <c r="F46" s="67" t="s">
+        <v>55</v>
+      </c>
       <c r="G46" s="13"/>
-      <c r="H46" s="13" t="str">
+      <c r="H46" s="13" t="e">
         <f t="shared" si="37"/>
-        <v/>
+        <v>#VALUE!</v>
       </c>
       <c r="I46" s="34"/>
       <c r="J46" s="34"/>
@@ -7780,24 +7755,21 @@
       <c r="DA46" s="34"/>
       <c r="DB46" s="34"/>
     </row>
-    <row r="47" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="B47" s="75">
-        <v>5.0999999999999996</v>
+    <row r="47" spans="1:106" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B47" s="74">
+        <v>5.2</v>
       </c>
       <c r="C47" s="65" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D47" s="66">
         <v>0</v>
       </c>
       <c r="E47" s="67" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F47" s="67" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G47" s="13"/>
       <c r="H47" s="13" t="e">
@@ -7903,126 +7875,6 @@
       <c r="DA47" s="34"/>
       <c r="DB47" s="34"/>
     </row>
-    <row r="48" spans="1:106" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="75">
-        <v>5.2</v>
-      </c>
-      <c r="C48" s="65" t="s">
-        <v>74</v>
-      </c>
-      <c r="D48" s="66">
-        <v>0</v>
-      </c>
-      <c r="E48" s="67" t="s">
-        <v>56</v>
-      </c>
-      <c r="F48" s="67" t="s">
-        <v>56</v>
-      </c>
-      <c r="G48" s="13"/>
-      <c r="H48" s="13" t="e">
-        <f t="shared" si="37"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I48" s="34"/>
-      <c r="J48" s="34"/>
-      <c r="K48" s="34"/>
-      <c r="L48" s="34"/>
-      <c r="M48" s="34"/>
-      <c r="N48" s="34"/>
-      <c r="O48" s="34"/>
-      <c r="P48" s="34"/>
-      <c r="Q48" s="34"/>
-      <c r="R48" s="34"/>
-      <c r="S48" s="34"/>
-      <c r="T48" s="34"/>
-      <c r="U48" s="34"/>
-      <c r="V48" s="34"/>
-      <c r="W48" s="34"/>
-      <c r="X48" s="34"/>
-      <c r="Y48" s="34"/>
-      <c r="Z48" s="34"/>
-      <c r="AA48" s="34"/>
-      <c r="AB48" s="34"/>
-      <c r="AC48" s="34"/>
-      <c r="AD48" s="34"/>
-      <c r="AE48" s="34"/>
-      <c r="AF48" s="34"/>
-      <c r="AG48" s="34"/>
-      <c r="AH48" s="34"/>
-      <c r="AI48" s="34"/>
-      <c r="AJ48" s="34"/>
-      <c r="AK48" s="34"/>
-      <c r="AL48" s="34"/>
-      <c r="AM48" s="34"/>
-      <c r="AN48" s="34"/>
-      <c r="AO48" s="34"/>
-      <c r="AP48" s="34"/>
-      <c r="AQ48" s="34"/>
-      <c r="AR48" s="34"/>
-      <c r="AS48" s="34"/>
-      <c r="AT48" s="34"/>
-      <c r="AU48" s="34"/>
-      <c r="AV48" s="34"/>
-      <c r="AW48" s="34"/>
-      <c r="AX48" s="34"/>
-      <c r="AY48" s="34"/>
-      <c r="AZ48" s="34"/>
-      <c r="BA48" s="34"/>
-      <c r="BB48" s="34"/>
-      <c r="BC48" s="34"/>
-      <c r="BD48" s="34"/>
-      <c r="BE48" s="34"/>
-      <c r="BF48" s="34"/>
-      <c r="BG48" s="34"/>
-      <c r="BH48" s="34"/>
-      <c r="BI48" s="34"/>
-      <c r="BJ48" s="34"/>
-      <c r="BK48" s="34"/>
-      <c r="BL48" s="34"/>
-      <c r="BM48" s="34"/>
-      <c r="BN48" s="34"/>
-      <c r="BO48" s="34"/>
-      <c r="BP48" s="34"/>
-      <c r="BQ48" s="34"/>
-      <c r="BR48" s="34"/>
-      <c r="BS48" s="34"/>
-      <c r="BT48" s="34"/>
-      <c r="BU48" s="34"/>
-      <c r="BV48" s="34"/>
-      <c r="BW48" s="34"/>
-      <c r="BX48" s="34"/>
-      <c r="BY48" s="34"/>
-      <c r="BZ48" s="34"/>
-      <c r="CA48" s="34"/>
-      <c r="CB48" s="34"/>
-      <c r="CC48" s="34"/>
-      <c r="CD48" s="34"/>
-      <c r="CE48" s="34"/>
-      <c r="CF48" s="34"/>
-      <c r="CG48" s="34"/>
-      <c r="CH48" s="34"/>
-      <c r="CI48" s="34"/>
-      <c r="CJ48" s="34"/>
-      <c r="CK48" s="34"/>
-      <c r="CL48" s="34"/>
-      <c r="CM48" s="34"/>
-      <c r="CN48" s="34"/>
-      <c r="CO48" s="34"/>
-      <c r="CP48" s="34"/>
-      <c r="CQ48" s="34"/>
-      <c r="CR48" s="34"/>
-      <c r="CS48" s="34"/>
-      <c r="CT48" s="34"/>
-      <c r="CU48" s="34"/>
-      <c r="CV48" s="34"/>
-      <c r="CW48" s="34"/>
-      <c r="CX48" s="34"/>
-      <c r="CY48" s="34"/>
-      <c r="CZ48" s="34"/>
-      <c r="DA48" s="34"/>
-      <c r="DB48" s="34"/>
-    </row>
   </sheetData>
   <mergeCells count="16">
     <mergeCell ref="CV4:DB4"/>
@@ -8042,7 +7894,7 @@
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="AD4:AJ4"/>
   </mergeCells>
-  <conditionalFormatting sqref="D7:D48">
+  <conditionalFormatting sqref="D7:D47">
     <cfRule type="dataBar" priority="120">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -8056,12 +7908,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I5:DB46">
+  <conditionalFormatting sqref="I5:DB45">
     <cfRule type="expression" dxfId="44" priority="139">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I7:DB46">
+  <conditionalFormatting sqref="I7:DB45">
     <cfRule type="expression" dxfId="43" priority="133">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
@@ -8069,12 +7921,12 @@
       <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I47:BL47">
+  <conditionalFormatting sqref="I46:BL46">
     <cfRule type="expression" dxfId="41" priority="105">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I47:BL47">
+  <conditionalFormatting sqref="I46:BL46">
     <cfRule type="expression" dxfId="40" priority="103">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
@@ -8082,12 +7934,12 @@
       <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I48:BL48">
+  <conditionalFormatting sqref="I47:BL47">
     <cfRule type="expression" dxfId="38" priority="102">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I48:BL48">
+  <conditionalFormatting sqref="I47:BL47">
     <cfRule type="expression" dxfId="37" priority="100">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
@@ -8095,12 +7947,12 @@
       <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BM47:BS47">
+  <conditionalFormatting sqref="BM46:BS46">
     <cfRule type="expression" dxfId="35" priority="87">
       <formula>AND(TODAY()&gt;=BM$5,TODAY()&lt;BN$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BM47:BS47">
+  <conditionalFormatting sqref="BM46:BS46">
     <cfRule type="expression" dxfId="34" priority="85">
       <formula>AND(task_start&lt;=BM$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=BM$5)</formula>
     </cfRule>
@@ -8108,12 +7960,12 @@
       <formula>AND(task_end&gt;=BM$5,task_start&lt;BN$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BM48:BS48">
+  <conditionalFormatting sqref="BM47:BS47">
     <cfRule type="expression" dxfId="32" priority="84">
       <formula>AND(TODAY()&gt;=BM$5,TODAY()&lt;BN$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BM48:BS48">
+  <conditionalFormatting sqref="BM47:BS47">
     <cfRule type="expression" dxfId="31" priority="82">
       <formula>AND(task_start&lt;=BM$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=BM$5)</formula>
     </cfRule>
@@ -8121,12 +7973,12 @@
       <formula>AND(task_end&gt;=BM$5,task_start&lt;BN$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BT47:BZ47">
+  <conditionalFormatting sqref="BT46:BZ46">
     <cfRule type="expression" dxfId="29" priority="72">
       <formula>AND(TODAY()&gt;=BT$5,TODAY()&lt;BU$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BT47:BZ47">
+  <conditionalFormatting sqref="BT46:BZ46">
     <cfRule type="expression" dxfId="28" priority="70">
       <formula>AND(task_start&lt;=BT$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=BT$5)</formula>
     </cfRule>
@@ -8134,12 +7986,12 @@
       <formula>AND(task_end&gt;=BT$5,task_start&lt;BU$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BT48:BZ48">
+  <conditionalFormatting sqref="BT47:BZ47">
     <cfRule type="expression" dxfId="26" priority="69">
       <formula>AND(TODAY()&gt;=BT$5,TODAY()&lt;BU$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BT48:BZ48">
+  <conditionalFormatting sqref="BT47:BZ47">
     <cfRule type="expression" dxfId="25" priority="67">
       <formula>AND(task_start&lt;=BT$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=BT$5)</formula>
     </cfRule>
@@ -8147,12 +7999,12 @@
       <formula>AND(task_end&gt;=BT$5,task_start&lt;BU$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="CA47:CG47">
+  <conditionalFormatting sqref="CA46:CG46">
     <cfRule type="expression" dxfId="23" priority="57">
       <formula>AND(TODAY()&gt;=CA$5,TODAY()&lt;CB$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="CA47:CG47">
+  <conditionalFormatting sqref="CA46:CG46">
     <cfRule type="expression" dxfId="22" priority="55">
       <formula>AND(task_start&lt;=CA$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=CA$5)</formula>
     </cfRule>
@@ -8160,12 +8012,12 @@
       <formula>AND(task_end&gt;=CA$5,task_start&lt;CB$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="CA48:CG48">
+  <conditionalFormatting sqref="CA47:CG47">
     <cfRule type="expression" dxfId="20" priority="54">
       <formula>AND(TODAY()&gt;=CA$5,TODAY()&lt;CB$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="CA48:CG48">
+  <conditionalFormatting sqref="CA47:CG47">
     <cfRule type="expression" dxfId="19" priority="52">
       <formula>AND(task_start&lt;=CA$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=CA$5)</formula>
     </cfRule>
@@ -8173,12 +8025,12 @@
       <formula>AND(task_end&gt;=CA$5,task_start&lt;CB$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="CH47:CN47">
+  <conditionalFormatting sqref="CH46:CN46">
     <cfRule type="expression" dxfId="17" priority="42">
       <formula>AND(TODAY()&gt;=CH$5,TODAY()&lt;CI$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="CH47:CN47">
+  <conditionalFormatting sqref="CH46:CN46">
     <cfRule type="expression" dxfId="16" priority="40">
       <formula>AND(task_start&lt;=CH$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=CH$5)</formula>
     </cfRule>
@@ -8186,12 +8038,12 @@
       <formula>AND(task_end&gt;=CH$5,task_start&lt;CI$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="CH48:CN48">
+  <conditionalFormatting sqref="CH47:CN47">
     <cfRule type="expression" dxfId="14" priority="39">
       <formula>AND(TODAY()&gt;=CH$5,TODAY()&lt;CI$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="CH48:CN48">
+  <conditionalFormatting sqref="CH47:CN47">
     <cfRule type="expression" dxfId="13" priority="37">
       <formula>AND(task_start&lt;=CH$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=CH$5)</formula>
     </cfRule>
@@ -8199,12 +8051,12 @@
       <formula>AND(task_end&gt;=CH$5,task_start&lt;CI$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="CO47:CU47">
+  <conditionalFormatting sqref="CO46:CU46">
     <cfRule type="expression" dxfId="11" priority="27">
       <formula>AND(TODAY()&gt;=CO$5,TODAY()&lt;CP$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="CO47:CU47">
+  <conditionalFormatting sqref="CO46:CU46">
     <cfRule type="expression" dxfId="10" priority="25">
       <formula>AND(task_start&lt;=CO$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=CO$5)</formula>
     </cfRule>
@@ -8212,12 +8064,12 @@
       <formula>AND(task_end&gt;=CO$5,task_start&lt;CP$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="CO48:CU48">
+  <conditionalFormatting sqref="CO47:CU47">
     <cfRule type="expression" dxfId="8" priority="24">
       <formula>AND(TODAY()&gt;=CO$5,TODAY()&lt;CP$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="CO48:CU48">
+  <conditionalFormatting sqref="CO47:CU47">
     <cfRule type="expression" dxfId="7" priority="22">
       <formula>AND(task_start&lt;=CO$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=CO$5)</formula>
     </cfRule>
@@ -8225,12 +8077,12 @@
       <formula>AND(task_end&gt;=CO$5,task_start&lt;CP$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="CV47:DB47">
+  <conditionalFormatting sqref="CV46:DB46">
     <cfRule type="expression" dxfId="5" priority="12">
       <formula>AND(TODAY()&gt;=CV$5,TODAY()&lt;CW$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="CV47:DB47">
+  <conditionalFormatting sqref="CV46:DB46">
     <cfRule type="expression" dxfId="4" priority="10">
       <formula>AND(task_start&lt;=CV$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=CV$5)</formula>
     </cfRule>
@@ -8238,12 +8090,12 @@
       <formula>AND(task_end&gt;=CV$5,task_start&lt;CW$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="CV48:DB48">
+  <conditionalFormatting sqref="CV47:DB47">
     <cfRule type="expression" dxfId="2" priority="9">
       <formula>AND(TODAY()&gt;=CV$5,TODAY()&lt;CW$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="CV48:DB48">
+  <conditionalFormatting sqref="CV47:DB47">
     <cfRule type="expression" dxfId="1" priority="7">
       <formula>AND(task_start&lt;=CV$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=CV$5)</formula>
     </cfRule>
@@ -8282,7 +8134,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D7:D48</xm:sqref>
+          <xm:sqref>D7:D47</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>